<commit_message>
Initial work on ODS code mapping. More work to be done.
</commit_message>
<xml_diff>
--- a/Data/Test Suite Prerequisites.xlsx
+++ b/Data/Test Suite Prerequisites.xlsx
@@ -1513,13 +1513,15 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Encounters changes. The summary screen now shows a maximum of 3 Encounters.
</commit_message>
<xml_diff>
--- a/Data/Test Suite Prerequisites.xlsx
+++ b/Data/Test Suite Prerequisites.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Patients" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="53">
   <si>
     <t xml:space="preserve">Cells containing a '0' should not have any data for that section
 Cells containing an 'x' should have data for that section 
@@ -80,7 +80,13 @@
     <t xml:space="preserve">Patient 2</t>
   </si>
   <si>
-    <t xml:space="preserve">( 01/05/2015 - 01/07/2016 )</t>
+    <t xml:space="preserve">(01/05/2015 - 01/07/2016)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">** &gt;3 ** (01/05/2015 - 01/07/2016)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Min 4 encounters</t>
   </si>
   <si>
     <t xml:space="preserve">Patient 3</t>
@@ -316,7 +322,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -391,6 +397,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFF9900"/>
+        <bgColor rgb="FFFFCC00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFBE5D6"/>
         <bgColor rgb="FFFFF2CC"/>
       </patternFill>
@@ -507,7 +519,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -556,6 +568,10 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="13" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="15" fillId="10" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -564,7 +580,7 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="13" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="14" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -679,8 +695,8 @@
   </sheetPr>
   <dimension ref="A1:O19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -800,7 +816,7 @@
       </c>
       <c r="O4" s="11"/>
     </row>
-    <row r="5" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
         <v>16</v>
       </c>
@@ -816,8 +832,8 @@
       <c r="E5" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="10" t="s">
-        <v>17</v>
+      <c r="F5" s="12" t="s">
+        <v>18</v>
       </c>
       <c r="G5" s="9" t="s">
         <v>17</v>
@@ -843,32 +859,34 @@
       <c r="N5" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="O5" s="11"/>
+      <c r="O5" s="11" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>21</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D6" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="E6" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>19</v>
+      <c r="E6" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>21</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I6" s="10" t="n">
         <v>0</v>
@@ -876,86 +894,86 @@
       <c r="J6" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="K6" s="12" t="s">
-        <v>19</v>
+      <c r="K6" s="13" t="s">
+        <v>21</v>
       </c>
       <c r="L6" s="10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="M6" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="N6" s="12" t="s">
-        <v>19</v>
+      <c r="N6" s="13" t="s">
+        <v>21</v>
       </c>
       <c r="O6" s="11"/>
     </row>
     <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>19</v>
+        <v>23</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>21</v>
       </c>
       <c r="C7" s="10" t="n">
         <v>0</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>19</v>
+        <v>22</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>21</v>
       </c>
       <c r="H7" s="10" t="n">
         <v>0</v>
       </c>
       <c r="I7" s="10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J7" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="K7" s="12" t="s">
-        <v>19</v>
+      <c r="K7" s="13" t="s">
+        <v>21</v>
       </c>
       <c r="L7" s="10" t="n">
         <v>0</v>
       </c>
       <c r="M7" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="N7" s="12" t="s">
-        <v>19</v>
+        <v>22</v>
+      </c>
+      <c r="N7" s="13" t="s">
+        <v>21</v>
       </c>
       <c r="O7" s="11"/>
     </row>
     <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="F8" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>19</v>
+        <v>24</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>21</v>
       </c>
       <c r="H8" s="10" t="n">
         <v>0</v>
@@ -964,213 +982,213 @@
         <v>0</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="K8" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="L8" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="M8" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="N8" s="12" t="s">
-        <v>19</v>
+        <v>22</v>
+      </c>
+      <c r="K8" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="L8" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="M8" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="N8" s="13" t="s">
+        <v>21</v>
       </c>
       <c r="O8" s="11"/>
     </row>
     <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="G9" s="12" t="s">
-        <v>19</v>
+        <v>25</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>21</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I9" s="10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J9" s="10" t="n">
         <v>0</v>
       </c>
-      <c r="K9" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="L9" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="M9" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="N9" s="12" t="s">
-        <v>19</v>
+      <c r="K9" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="L9" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="M9" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="N9" s="13" t="s">
+        <v>21</v>
       </c>
       <c r="O9" s="11"/>
     </row>
     <row r="10" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="F10" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="G10" s="12" t="s">
-        <v>19</v>
+        <v>26</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>21</v>
       </c>
       <c r="H10" s="10" t="n">
         <v>0</v>
       </c>
       <c r="I10" s="10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J10" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="K10" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="L10" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="M10" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="N10" s="12" t="s">
-        <v>19</v>
+        <v>22</v>
+      </c>
+      <c r="K10" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="L10" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="M10" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="N10" s="13" t="s">
+        <v>21</v>
       </c>
       <c r="O10" s="11"/>
     </row>
     <row r="11" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="F11" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="G11" s="12" t="s">
-        <v>19</v>
+        <v>27</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>21</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I11" s="10" t="n">
         <v>0</v>
       </c>
       <c r="J11" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="K11" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="L11" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="M11" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="N11" s="12" t="s">
-        <v>19</v>
+        <v>22</v>
+      </c>
+      <c r="K11" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="L11" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="M11" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="N11" s="13" t="s">
+        <v>21</v>
       </c>
       <c r="O11" s="11"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="14" t="s">
-        <v>26</v>
+      <c r="A12" s="15" t="s">
+        <v>28</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I12" s="10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J12" s="10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="K12" s="9" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="L12" s="10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="M12" s="10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="N12" s="9" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="O12" s="7" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="14" t="s">
-        <v>28</v>
+      <c r="A13" s="15" t="s">
+        <v>30</v>
       </c>
       <c r="B13" s="9" t="n">
         <v>0</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D13" s="10" t="n">
         <v>0</v>
@@ -1179,7 +1197,7 @@
         <v>0</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G13" s="9" t="n">
         <v>0</v>
@@ -1188,7 +1206,7 @@
         <v>0</v>
       </c>
       <c r="I13" s="10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J13" s="10" t="n">
         <v>0</v>
@@ -1197,298 +1215,298 @@
         <v>0</v>
       </c>
       <c r="L13" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="M13" s="13" t="s">
-        <v>19</v>
+        <v>22</v>
+      </c>
+      <c r="M13" s="14" t="s">
+        <v>21</v>
       </c>
       <c r="N13" s="9" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="O13" s="7" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="14" t="s">
-        <v>29</v>
+      <c r="A14" s="15" t="s">
+        <v>31</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H14" s="10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I14" s="10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="K14" s="9" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="L14" s="10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="M14" s="10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="N14" s="9" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="O14" s="7" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="14" t="s">
-        <v>31</v>
+      <c r="A15" s="15" t="s">
+        <v>33</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I15" s="10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J15" s="10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="K15" s="9" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="L15" s="10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="M15" s="10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="N15" s="9" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="O15" s="7" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="14" t="s">
-        <v>33</v>
+      <c r="A16" s="15" t="s">
+        <v>35</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H16" s="10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I16" s="10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J16" s="10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="K16" s="9" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="L16" s="10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="M16" s="10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="N16" s="9" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="O16" s="7" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="28.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="14" t="s">
-        <v>35</v>
+      <c r="A17" s="15" t="s">
+        <v>37</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H17" s="10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I17" s="10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J17" s="10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="K17" s="9" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="L17" s="10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="M17" s="10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="N17" s="9" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="O17" s="7" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="14" t="s">
-        <v>37</v>
+      <c r="A18" s="15" t="s">
+        <v>39</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H18" s="10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I18" s="10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="J18" s="10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="K18" s="9" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="L18" s="10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="M18" s="10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="N18" s="9" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="O18" s="7" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="22.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="B19" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="D19" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="E19" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="F19" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="G19" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="H19" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="I19" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="J19" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="K19" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="L19" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="M19" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="N19" s="15" t="s">
-        <v>19</v>
+      <c r="A19" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="F19" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G19" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="H19" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="I19" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="J19" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="K19" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="L19" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="M19" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="N19" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="O19" s="7" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1512,7 +1530,7 @@
   </sheetPr>
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
     </sheetView>
   </sheetViews>
@@ -1520,61 +1538,62 @@
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="17" t="s">
-        <v>43</v>
+      <c r="A2" s="18" t="s">
+        <v>45</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="18" t="s">
-        <v>49</v>
+      <c r="A7" s="19" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Practitioners have been parameterised.
</commit_message>
<xml_diff>
--- a/Data/Test Suite Prerequisites.xlsx
+++ b/Data/Test Suite Prerequisites.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Patients" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Organizations" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Practitioner" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" name="LOCAL_MYSQL_DATE_FORMAT" vbProcedure="false">REPT(local_year_format,4)&amp;local_date_separator&amp;REPT(local_month_format,2)&amp;local_date_separator&amp;REPT(local_day_format,2)&amp;" "&amp;REPT(local_hour_format,2)&amp;local_time_separator&amp;REPT(local_minute_format,2)&amp;local_time_separator&amp;REPT(local_second_format,2)</definedName>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="56">
   <si>
     <t xml:space="preserve">Cells containing a '0' should not have any data for that section
 Cells containing an 'x' should have data for that section 
@@ -186,6 +187,15 @@
   </si>
   <si>
     <t xml:space="preserve">Site Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Practitioner Code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G11111116</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G99999999</t>
   </si>
 </sst>
 </file>
@@ -695,11 +705,11 @@
   </sheetPr>
   <dimension ref="A1:O19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="2" style="2" width="19.91"/>
@@ -707,7 +717,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="16" style="1" width="11.54"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="54.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="43.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -771,7 +781,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
         <v>15</v>
       </c>
@@ -816,7 +826,7 @@
       </c>
       <c r="O4" s="11"/>
     </row>
-    <row r="5" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="22.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
         <v>16</v>
       </c>
@@ -863,7 +873,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
         <v>20</v>
       </c>
@@ -908,7 +918,7 @@
       </c>
       <c r="O6" s="11"/>
     </row>
-    <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
         <v>23</v>
       </c>
@@ -953,7 +963,7 @@
       </c>
       <c r="O7" s="11"/>
     </row>
-    <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
         <v>24</v>
       </c>
@@ -998,7 +1008,7 @@
       </c>
       <c r="O8" s="11"/>
     </row>
-    <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="s">
         <v>25</v>
       </c>
@@ -1043,7 +1053,7 @@
       </c>
       <c r="O9" s="11"/>
     </row>
-    <row r="10" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="8" t="s">
         <v>26</v>
       </c>
@@ -1088,7 +1098,7 @@
       </c>
       <c r="O10" s="11"/>
     </row>
-    <row r="11" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="8" t="s">
         <v>27</v>
       </c>
@@ -1274,7 +1284,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="15" t="s">
         <v>33</v>
       </c>
@@ -1321,7 +1331,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="15" t="s">
         <v>35</v>
       </c>
@@ -1368,7 +1378,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="28.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="22.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="15" t="s">
         <v>37</v>
       </c>
@@ -1415,7 +1425,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="29" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="22.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="15" t="s">
         <v>39</v>
       </c>
@@ -1462,7 +1472,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="22.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="22.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="15" t="s">
         <v>41</v>
       </c>
@@ -1530,8 +1540,8 @@
   </sheetPr>
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1612,4 +1622,56 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C26" activeCellId="0" sqref="C26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="18" width="16.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="18" width="23.82"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="18" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added more patient search test scenarios
</commit_message>
<xml_diff>
--- a/Data/Test Suite Prerequisites.xlsx
+++ b/Data/Test Suite Prerequisites.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Patients" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="61">
   <si>
     <t xml:space="preserve">Cells containing a '0' should not have any data for that section
 Cells containing an 'x' should have data for that section 
@@ -156,7 +156,16 @@
     <t xml:space="preserve">Patient 16</t>
   </si>
   <si>
-    <t xml:space="preserve">Patient with same NHS number as “Patient3”</t>
+    <t xml:space="preserve">Patient with same NHS number as “Patient18”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patient 17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deceased patient</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patient 18</t>
   </si>
   <si>
     <t xml:space="preserve">Organization Code</t>
@@ -709,13 +718,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O19"/>
+  <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O20" activeCellId="0" sqref="O20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="2" style="2" width="19.91"/>
@@ -1478,7 +1487,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="22.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="23.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="15" t="s">
         <v>41</v>
       </c>
@@ -1524,6 +1533,98 @@
       <c r="O19" s="7" t="s">
         <v>42</v>
       </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="F20" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G20" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="H20" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="I20" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="J20" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="K20" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="L20" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="M20" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="N20" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="O20" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="F21" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="G21" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="H21" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="I21" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="J21" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="K21" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="L21" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="M21" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="N21" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="O21" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1546,11 +1647,11 @@
   </sheetPr>
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="N15" activeCellId="0" sqref="N15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.14"/>
@@ -1559,57 +1660,57 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="18" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="19" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1637,11 +1738,11 @@
   </sheetPr>
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F21" activeCellId="0" sqref="F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="18" width="16.07"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="18" width="11.52"/>
@@ -1649,12 +1750,12 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="18" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1662,12 +1763,12 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="19" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added test scenario for Patient MultipleBirth field
</commit_message>
<xml_diff>
--- a/Data/Test Suite Prerequisites.xlsx
+++ b/Data/Test Suite Prerequisites.xlsx
@@ -162,7 +162,8 @@
     <t xml:space="preserve">Patient 17</t>
   </si>
   <si>
-    <t xml:space="preserve">Deceased patient</t>
+    <t xml:space="preserve">Deceased patient.
+Part of multiple birth.</t>
   </si>
   <si>
     <t xml:space="preserve">Patient 18</t>
@@ -721,7 +722,7 @@
   <dimension ref="A1:O21"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O20" activeCellId="0" sqref="O20"/>
+      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1534,7 +1535,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="22.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="15" t="s">
         <v>43</v>
       </c>

</xml_diff>

<commit_message>
Added getSchedule tests for validation of DateTime formats, also updated the test pre-requisits for what static and rolling available slots are required.
</commit_message>
<xml_diff>
--- a/Data/Test Suite Prerequisites.xlsx
+++ b/Data/Test Suite Prerequisites.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Patients" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Organizations" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Practitioner" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Sheet4" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" name="LOCAL_MYSQL_DATE_FORMAT" vbProcedure="false">REPT(local_year_format,4)&amp;local_date_separator&amp;REPT(local_month_format,2)&amp;local_date_separator&amp;REPT(local_day_format,2)&amp;" "&amp;REPT(local_hour_format,2)&amp;local_time_separator&amp;REPT(local_minute_format,2)&amp;local_time_separator&amp;REPT(local_second_format,2)</definedName>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="76">
   <si>
     <t xml:space="preserve">Cells containing a '0' should not have any data for that section
 Cells containing an 'x' should have data for that section 
@@ -239,16 +240,36 @@
   </si>
   <si>
     <t xml:space="preserve">practitioner4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Required Fixed Slots for testing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rolling Slots</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A set of rolling/available slots needs to be present from the current date for up to a 14 days into the future with the following number of slots for each of the following organizations.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Number of slots</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="YYYY\-MM\-DD"/>
+    <numFmt numFmtId="166" formatCode="HH:MM:SS"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -374,8 +395,16 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -460,6 +489,12 @@
         <bgColor rgb="FFFFF2CC"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCCCCC"/>
+        <bgColor rgb="FFBFBFBF"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="4">
     <border diagonalUp="false" diagonalDown="false">
@@ -572,7 +607,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="27">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -651,6 +686,34 @@
     </xf>
     <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -716,9 +779,9 @@
       <rgbColor rgb="FFE2F0D9"/>
       <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFF2CC"/>
+      <rgbColor rgb="FFCCCCCC"/>
+      <rgbColor rgb="FFFBE5D6"/>
       <rgbColor rgb="FFDDDDDD"/>
-      <rgbColor rgb="FFFBE5D6"/>
-      <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFCCCC"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
@@ -752,7 +815,7 @@
       <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="2" style="2" width="19.91"/>
@@ -1676,10 +1739,10 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N15" activeCellId="0" sqref="N15"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.14"/>
@@ -1766,14 +1829,14 @@
   </sheetPr>
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="18" width="16.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="18" width="15.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="18" width="15.27"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="18" width="11.52"/>
   </cols>
   <sheetData>
@@ -1845,4 +1908,227 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="B2:M17"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="20" width="4.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="20" width="19.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="20" width="14.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="20" width="9.31"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="20" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="2" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="25" t="n">
+        <v>42792</v>
+      </c>
+      <c r="D5" s="26" t="n">
+        <v>0.440972222222222</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="25" t="n">
+        <v>42737</v>
+      </c>
+      <c r="D6" s="26" t="n">
+        <v>0.527777777777778</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="25" t="n">
+        <v>43098</v>
+      </c>
+      <c r="D7" s="26" t="n">
+        <v>0.527777777777778</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" s="22"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+      <c r="G10" s="22"/>
+      <c r="H10" s="22"/>
+      <c r="I10" s="22"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="22"/>
+      <c r="L10" s="22"/>
+      <c r="M10" s="22"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="22"/>
+      <c r="L11" s="22"/>
+      <c r="M11" s="22"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="24"/>
+      <c r="L12" s="24"/>
+      <c r="M12" s="24"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="22"/>
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="22"/>
+      <c r="I13" s="22"/>
+      <c r="J13" s="22"/>
+      <c r="K13" s="22"/>
+      <c r="L13" s="22"/>
+      <c r="M13" s="22"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>75</v>
+      </c>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="22"/>
+      <c r="J14" s="22"/>
+      <c r="K14" s="22"/>
+      <c r="L14" s="22"/>
+      <c r="M14" s="22"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="22" t="n">
+        <v>30</v>
+      </c>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="22"/>
+      <c r="I15" s="22"/>
+      <c r="J15" s="22"/>
+      <c r="K15" s="22"/>
+      <c r="L15" s="22"/>
+      <c r="M15" s="22"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="22" t="n">
+        <v>20</v>
+      </c>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
+      <c r="K16" s="22"/>
+      <c r="L16" s="22"/>
+      <c r="M16" s="22"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
+      <c r="K17" s="22"/>
+      <c r="L17" s="22"/>
+      <c r="M17" s="22"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B12:M12"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added additional getSchedule test scenarios and improved some of the shared steps validation output.
</commit_message>
<xml_diff>
--- a/Data/Test Suite Prerequisites.xlsx
+++ b/Data/Test Suite Prerequisites.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="79">
   <si>
     <t xml:space="preserve">Cells containing a '0' should not have any data for that section
 Cells containing an 'x' should have data for that section 
@@ -249,6 +249,15 @@
   </si>
   <si>
     <t xml:space="preserve">Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Min Duration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 mins</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No other slots for ORG1 should appear for this date (29/12/2017)</t>
   </si>
   <si>
     <t xml:space="preserve">Rolling Slots</t>
@@ -607,7 +616,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -692,27 +701,35 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="18" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="18" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="15" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1915,10 +1932,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:M17"/>
+  <dimension ref="B2:I17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
+      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1926,8 +1943,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="20" width="4.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="20" width="19.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="20" width="14.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="20" width="9.31"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="20" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="20" width="9.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="20" width="14.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="20" width="54.88"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="20" width="11.52"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1936,11 +1955,15 @@
       </c>
       <c r="C2" s="21"/>
       <c r="D2" s="21"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="22"/>
       <c r="C3" s="22"/>
       <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="23" t="s">
@@ -1952,6 +1975,12 @@
       <c r="D4" s="23" t="s">
         <v>72</v>
       </c>
+      <c r="E4" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="F4" s="23" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="24" t="s">
@@ -1963,6 +1992,10 @@
       <c r="D5" s="26" t="n">
         <v>0.440972222222222</v>
       </c>
+      <c r="E5" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="F5" s="26"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="24" t="s">
@@ -1974,6 +2007,10 @@
       <c r="D6" s="26" t="n">
         <v>0.527777777777778</v>
       </c>
+      <c r="E6" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="F6" s="26"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="24" t="s">
@@ -1985,10 +2022,16 @@
       <c r="D7" s="26" t="n">
         <v>0.527777777777778</v>
       </c>
+      <c r="E7" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="F7" s="26" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="21" t="s">
-        <v>73</v>
+      <c r="B10" s="27" t="s">
+        <v>76</v>
       </c>
       <c r="C10" s="22"/>
       <c r="D10" s="22"/>
@@ -1997,10 +2040,6 @@
       <c r="G10" s="22"/>
       <c r="H10" s="22"/>
       <c r="I10" s="22"/>
-      <c r="J10" s="22"/>
-      <c r="K10" s="22"/>
-      <c r="L10" s="22"/>
-      <c r="M10" s="22"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="22"/>
@@ -2011,14 +2050,10 @@
       <c r="G11" s="22"/>
       <c r="H11" s="22"/>
       <c r="I11" s="22"/>
-      <c r="J11" s="22"/>
-      <c r="K11" s="22"/>
-      <c r="L11" s="22"/>
-      <c r="M11" s="22"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="24" t="s">
-        <v>74</v>
+      <c r="B12" s="28" t="s">
+        <v>77</v>
       </c>
       <c r="C12" s="24"/>
       <c r="D12" s="24"/>
@@ -2027,10 +2062,6 @@
       <c r="G12" s="24"/>
       <c r="H12" s="24"/>
       <c r="I12" s="24"/>
-      <c r="J12" s="24"/>
-      <c r="K12" s="24"/>
-      <c r="L12" s="24"/>
-      <c r="M12" s="24"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="22"/>
@@ -2041,17 +2072,13 @@
       <c r="G13" s="22"/>
       <c r="H13" s="22"/>
       <c r="I13" s="22"/>
-      <c r="J13" s="22"/>
-      <c r="K13" s="22"/>
-      <c r="L13" s="22"/>
-      <c r="M13" s="22"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="23" t="s">
         <v>46</v>
       </c>
       <c r="C14" s="23" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="D14" s="22"/>
       <c r="E14" s="22"/>
@@ -2059,10 +2086,6 @@
       <c r="G14" s="22"/>
       <c r="H14" s="22"/>
       <c r="I14" s="22"/>
-      <c r="J14" s="22"/>
-      <c r="K14" s="22"/>
-      <c r="L14" s="22"/>
-      <c r="M14" s="22"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="22" t="s">
@@ -2077,10 +2100,6 @@
       <c r="G15" s="22"/>
       <c r="H15" s="22"/>
       <c r="I15" s="22"/>
-      <c r="J15" s="22"/>
-      <c r="K15" s="22"/>
-      <c r="L15" s="22"/>
-      <c r="M15" s="22"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="22" t="s">
@@ -2095,10 +2114,6 @@
       <c r="G16" s="22"/>
       <c r="H16" s="22"/>
       <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
-      <c r="K16" s="22"/>
-      <c r="L16" s="22"/>
-      <c r="M16" s="22"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="22" t="s">
@@ -2113,15 +2128,10 @@
       <c r="G17" s="22"/>
       <c r="H17" s="22"/>
       <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
-      <c r="K17" s="22"/>
-      <c r="L17" s="22"/>
-      <c r="M17" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B12:M12"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Added some changed following th review
</commit_message>
<xml_diff>
--- a/Data/Test Suite Prerequisites.xlsx
+++ b/Data/Test Suite Prerequisites.xlsx
@@ -9,19 +9,20 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Patients" sheetId="1" r:id="rId1"/>
     <sheet name="Organizations" sheetId="2" r:id="rId2"/>
-    <sheet name="Practitioner" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
-    <sheet name="CustomAppointments" sheetId="5" r:id="rId5"/>
+    <sheet name="Locations" sheetId="6" r:id="rId3"/>
+    <sheet name="Practitioner" sheetId="3" r:id="rId4"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId5"/>
+    <sheet name="CustomAppointments" sheetId="5" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT">REPT(local_year_format,4)&amp;local_date_separator&amp;REPT(local_month_format,2)&amp;local_date_separator&amp;REPT(local_day_format,2)&amp;" "&amp;REPT(local_hour_format,2)&amp;local_time_separator&amp;REPT(local_minute_format,2)&amp;local_time_separator&amp;REPT(local_second_format,2)</definedName>
   </definedNames>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="161">
   <si>
     <t>Cells containing a '0' should not have any data for that section
 Cells containing an 'x' should have data for that section 
@@ -490,6 +491,81 @@
   </si>
   <si>
     <t>Priority</t>
+  </si>
+  <si>
+    <t>Number Of Locations</t>
+  </si>
+  <si>
+    <t>SIT4</t>
+  </si>
+  <si>
+    <t>Location Id</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>2,3</t>
+  </si>
+  <si>
+    <t>Building A</t>
+  </si>
+  <si>
+    <t>GPC001</t>
+  </si>
+  <si>
+    <t>GP Connect Demonstrator</t>
+  </si>
+  <si>
+    <t>Z26556</t>
+  </si>
+  <si>
+    <t>BUILDING A</t>
+  </si>
+  <si>
+    <t>ORG111</t>
+  </si>
+  <si>
+    <t>Z33432</t>
+  </si>
+  <si>
+    <t>ANNEX</t>
+  </si>
+  <si>
+    <t>SHED</t>
+  </si>
+  <si>
+    <t>Building 8</t>
+  </si>
+  <si>
+    <t>Building 6</t>
+  </si>
+  <si>
+    <t>ORG114</t>
+  </si>
+  <si>
+    <t>Z33433</t>
+  </si>
+  <si>
+    <t>BUILDING E</t>
+  </si>
+  <si>
+    <t>BUILDING F</t>
+  </si>
+  <si>
+    <t>BUILDING G</t>
+  </si>
+  <si>
+    <t>BUILDING H</t>
+  </si>
+  <si>
+    <t>BUILDING I</t>
+  </si>
+  <si>
+    <t>4,5,6,7,8,9</t>
+  </si>
+  <si>
+    <t>Location Ids(Location Spreadsheet)</t>
   </si>
 </sst>
 </file>
@@ -726,14 +802,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -834,6 +904,15 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1220,905 +1299,905 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.08984375" style="3" customWidth="1"/>
-    <col min="2" max="14" width="19.90625" style="4" customWidth="1"/>
-    <col min="15" max="15" width="25.54296875" style="3" customWidth="1"/>
-    <col min="16" max="1025" width="11.54296875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="13.08984375" style="1" customWidth="1"/>
+    <col min="2" max="14" width="19.90625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="25.54296875" style="1" customWidth="1"/>
+    <col min="16" max="1025" width="11.54296875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="43.9" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
+      <c r="A1" s="36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="36"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A3" s="5"/>
-      <c r="B3" s="6" t="s">
+      <c r="A3" s="3"/>
+      <c r="B3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="I3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="J3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="K3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="L3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="M3" s="7" t="s">
+      <c r="M3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="6" t="s">
+      <c r="N3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O3" s="8" t="s">
+      <c r="O3" s="6" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="10">
-        <v>0</v>
-      </c>
-      <c r="C4" s="11">
-        <v>0</v>
-      </c>
-      <c r="D4" s="11">
-        <v>0</v>
-      </c>
-      <c r="E4" s="10">
-        <v>0</v>
-      </c>
-      <c r="F4" s="11">
-        <v>0</v>
-      </c>
-      <c r="G4" s="10">
-        <v>0</v>
-      </c>
-      <c r="H4" s="11">
-        <v>0</v>
-      </c>
-      <c r="I4" s="11">
-        <v>0</v>
-      </c>
-      <c r="J4" s="11">
-        <v>0</v>
-      </c>
-      <c r="K4" s="10">
-        <v>0</v>
-      </c>
-      <c r="L4" s="11">
-        <v>0</v>
-      </c>
-      <c r="M4" s="11">
-        <v>0</v>
-      </c>
-      <c r="N4" s="10">
-        <v>0</v>
-      </c>
-      <c r="O4" s="12"/>
+      <c r="B4" s="8">
+        <v>0</v>
+      </c>
+      <c r="C4" s="9">
+        <v>0</v>
+      </c>
+      <c r="D4" s="9">
+        <v>0</v>
+      </c>
+      <c r="E4" s="8">
+        <v>0</v>
+      </c>
+      <c r="F4" s="9">
+        <v>0</v>
+      </c>
+      <c r="G4" s="8">
+        <v>0</v>
+      </c>
+      <c r="H4" s="9">
+        <v>0</v>
+      </c>
+      <c r="I4" s="9">
+        <v>0</v>
+      </c>
+      <c r="J4" s="9">
+        <v>0</v>
+      </c>
+      <c r="K4" s="8">
+        <v>0</v>
+      </c>
+      <c r="L4" s="9">
+        <v>0</v>
+      </c>
+      <c r="M4" s="9">
+        <v>0</v>
+      </c>
+      <c r="N4" s="8">
+        <v>0</v>
+      </c>
+      <c r="O4" s="10"/>
     </row>
     <row r="5" spans="1:15" ht="29" x14ac:dyDescent="0.35">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="G5" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="11" t="s">
+      <c r="H5" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="I5" s="11" t="s">
+      <c r="I5" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="J5" s="11" t="s">
+      <c r="J5" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="K5" s="10" t="s">
+      <c r="K5" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="L5" s="11" t="s">
+      <c r="L5" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="M5" s="11" t="s">
+      <c r="M5" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="N5" s="10" t="s">
+      <c r="N5" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="O5" s="12" t="s">
+      <c r="O5" s="10" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="11">
-        <v>0</v>
-      </c>
-      <c r="E6" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="H6" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I6" s="11">
-        <v>0</v>
-      </c>
-      <c r="J6" s="11">
-        <v>0</v>
-      </c>
-      <c r="K6" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="L6" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="M6" s="11">
-        <v>0</v>
-      </c>
-      <c r="N6" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="O6" s="12"/>
+      <c r="B6" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="9">
+        <v>0</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" s="9">
+        <v>0</v>
+      </c>
+      <c r="J6" s="9">
+        <v>0</v>
+      </c>
+      <c r="K6" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="L6" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="M6" s="9">
+        <v>0</v>
+      </c>
+      <c r="N6" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="O6" s="10"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="11">
-        <v>0</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="H7" s="11">
-        <v>0</v>
-      </c>
-      <c r="I7" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="J7" s="11">
-        <v>0</v>
-      </c>
-      <c r="K7" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="L7" s="11">
-        <v>0</v>
-      </c>
-      <c r="M7" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="N7" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="O7" s="12"/>
+      <c r="B7" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="9">
+        <v>0</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" s="9">
+        <v>0</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="J7" s="9">
+        <v>0</v>
+      </c>
+      <c r="K7" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="L7" s="9">
+        <v>0</v>
+      </c>
+      <c r="M7" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="N7" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="O7" s="10"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="F8" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="G8" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="H8" s="11">
-        <v>0</v>
-      </c>
-      <c r="I8" s="11">
-        <v>0</v>
-      </c>
-      <c r="J8" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="K8" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="L8" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="M8" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="N8" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="O8" s="12"/>
+      <c r="B8" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" s="9">
+        <v>0</v>
+      </c>
+      <c r="I8" s="9">
+        <v>0</v>
+      </c>
+      <c r="J8" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="K8" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="L8" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="M8" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="N8" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="O8" s="10"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="G9" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="H9" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I9" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="J9" s="11">
-        <v>0</v>
-      </c>
-      <c r="K9" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="L9" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="M9" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="N9" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="O9" s="12"/>
+      <c r="B9" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="J9" s="9">
+        <v>0</v>
+      </c>
+      <c r="K9" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="L9" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="M9" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="N9" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="O9" s="10"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="F10" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="G10" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="H10" s="11">
-        <v>0</v>
-      </c>
-      <c r="I10" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="J10" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="K10" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="L10" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="M10" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="N10" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="O10" s="12"/>
+      <c r="B10" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" s="9">
+        <v>0</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="J10" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="K10" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="L10" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="M10" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="N10" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="O10" s="10"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="F11" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="G11" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="H11" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I11" s="11">
-        <v>0</v>
-      </c>
-      <c r="J11" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="K11" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="L11" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="M11" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="N11" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="O11" s="12"/>
+      <c r="B11" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="I11" s="9">
+        <v>0</v>
+      </c>
+      <c r="J11" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="K11" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="L11" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="M11" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="N11" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="O11" s="10"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="G12" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="H12" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I12" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="J12" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="K12" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="L12" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="M12" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="N12" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="O12" s="8" t="s">
+      <c r="B12" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="J12" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="K12" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L12" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="M12" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="N12" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="O12" s="6" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A13" s="16" t="s">
+      <c r="A13" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="10">
-        <v>0</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" s="11">
-        <v>0</v>
-      </c>
-      <c r="E13" s="10">
-        <v>0</v>
-      </c>
-      <c r="F13" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="G13" s="10">
-        <v>0</v>
-      </c>
-      <c r="H13" s="11">
-        <v>0</v>
-      </c>
-      <c r="I13" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="J13" s="11">
-        <v>0</v>
-      </c>
-      <c r="K13" s="10">
-        <v>0</v>
-      </c>
-      <c r="L13" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="M13" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="N13" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="O13" s="8" t="s">
+      <c r="B13" s="8">
+        <v>0</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="9">
+        <v>0</v>
+      </c>
+      <c r="E13" s="8">
+        <v>0</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G13" s="8">
+        <v>0</v>
+      </c>
+      <c r="H13" s="9">
+        <v>0</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="J13" s="9">
+        <v>0</v>
+      </c>
+      <c r="K13" s="8">
+        <v>0</v>
+      </c>
+      <c r="L13" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="M13" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="N13" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="O13" s="6" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="G14" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="H14" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I14" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="J14" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="K14" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="L14" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="M14" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="N14" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="O14" s="8" t="s">
+      <c r="B14" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="J14" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="K14" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L14" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="M14" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="N14" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="O14" s="6" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A15" s="16" t="s">
+      <c r="A15" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="F15" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="G15" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="H15" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I15" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="J15" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="K15" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="L15" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="M15" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="N15" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="O15" s="8" t="s">
+      <c r="B15" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="I15" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="J15" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="K15" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L15" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="M15" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="N15" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="O15" s="6" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A16" s="16" t="s">
+      <c r="A16" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="F16" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="G16" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="H16" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I16" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="J16" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="K16" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="L16" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="M16" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="N16" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="O16" s="8" t="s">
+      <c r="B16" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="I16" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="J16" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="K16" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L16" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="M16" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="N16" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="O16" s="6" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:15" ht="29" x14ac:dyDescent="0.35">
-      <c r="A17" s="16" t="s">
+      <c r="A17" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B17" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="F17" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="G17" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="H17" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I17" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="J17" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="K17" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="L17" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="M17" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="N17" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="O17" s="8" t="s">
+      <c r="B17" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="I17" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="J17" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="K17" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L17" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="M17" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="N17" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="O17" s="6" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:15" ht="29" x14ac:dyDescent="0.35">
-      <c r="A18" s="16" t="s">
+      <c r="A18" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="B18" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="F18" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="G18" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="H18" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="I18" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="J18" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="K18" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="L18" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="M18" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="N18" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="O18" s="8" t="s">
+      <c r="B18" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="I18" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="J18" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="K18" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="L18" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="M18" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="N18" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="O18" s="6" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:15" ht="29" x14ac:dyDescent="0.35">
-      <c r="A19" s="16" t="s">
+      <c r="A19" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="B19" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="D19" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="E19" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="F19" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="G19" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="H19" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="I19" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="J19" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="K19" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="L19" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="M19" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="N19" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="O19" s="8" t="s">
+      <c r="B19" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F19" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="G19" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="H19" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="I19" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="J19" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="K19" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="L19" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="M19" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="N19" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="O19" s="6" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:15" ht="29" x14ac:dyDescent="0.35">
-      <c r="A20" s="16" t="s">
+      <c r="A20" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="B20" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="D20" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="E20" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="F20" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="G20" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="H20" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="I20" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="J20" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="K20" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="L20" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="M20" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="N20" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="O20" s="8" t="s">
+      <c r="B20" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F20" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="G20" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="H20" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="I20" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="J20" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="K20" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="L20" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="M20" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="N20" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="O20" s="6" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A21" s="16" t="s">
+      <c r="A21" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="B21" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="C21" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="D21" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="E21" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="F21" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="G21" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="H21" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="I21" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="J21" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="K21" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="L21" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="M21" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="N21" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="O21" s="8"/>
+      <c r="B21" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F21" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="G21" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="H21" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="I21" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="J21" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="K21" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="L21" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="M21" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="N21" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="O21" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2131,57 +2210,97 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.90625" customWidth="1"/>
     <col min="2" max="2" width="24.08984375" customWidth="1"/>
-    <col min="3" max="1025" width="8.6328125" customWidth="1"/>
+    <col min="3" max="3" width="41" customWidth="1"/>
+    <col min="4" max="4" width="29.54296875" customWidth="1"/>
+    <col min="5" max="1025" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>46</v>
       </c>
       <c r="B1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="19" t="s">
+      <c r="C1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="17" t="s">
         <v>48</v>
       </c>
       <c r="B2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>50</v>
       </c>
       <c r="B3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>52</v>
       </c>
       <c r="B4" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" s="20" t="s">
+      <c r="C4">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" t="s">
+        <v>137</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="18" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>46</v>
       </c>
@@ -2189,7 +2308,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>56</v>
       </c>
@@ -2209,6 +2328,214 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="18.54296875" customWidth="1"/>
+    <col min="2" max="2" width="22.453125" customWidth="1"/>
+    <col min="3" max="3" width="17.7265625" customWidth="1"/>
+    <col min="4" max="4" width="23" customWidth="1"/>
+    <col min="5" max="5" width="28.54296875" customWidth="1"/>
+    <col min="6" max="6" width="28.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="38" t="s">
+        <v>141</v>
+      </c>
+      <c r="C2" s="38" t="s">
+        <v>142</v>
+      </c>
+      <c r="D2" s="38" t="s">
+        <v>143</v>
+      </c>
+      <c r="E2" s="38" t="s">
+        <v>144</v>
+      </c>
+      <c r="F2" s="38" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="38" t="s">
+        <v>150</v>
+      </c>
+      <c r="C3" s="38" t="s">
+        <v>146</v>
+      </c>
+      <c r="D3" s="38" t="s">
+        <v>145</v>
+      </c>
+      <c r="E3" s="38" t="s">
+        <v>147</v>
+      </c>
+      <c r="F3" s="38" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="38" t="s">
+        <v>150</v>
+      </c>
+      <c r="C4" s="38" t="s">
+        <v>146</v>
+      </c>
+      <c r="D4" s="38" t="s">
+        <v>149</v>
+      </c>
+      <c r="E4" s="38" t="s">
+        <v>147</v>
+      </c>
+      <c r="F4" s="38" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="38" t="s">
+        <v>151</v>
+      </c>
+      <c r="C5" s="38" t="s">
+        <v>152</v>
+      </c>
+      <c r="D5" s="38" t="s">
+        <v>145</v>
+      </c>
+      <c r="E5" s="38" t="s">
+        <v>153</v>
+      </c>
+      <c r="F5" s="38" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="38" t="s">
+        <v>151</v>
+      </c>
+      <c r="C6" s="38" t="s">
+        <v>152</v>
+      </c>
+      <c r="D6" s="38" t="s">
+        <v>154</v>
+      </c>
+      <c r="E6" s="38" t="s">
+        <v>153</v>
+      </c>
+      <c r="F6" s="38" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="38" t="s">
+        <v>151</v>
+      </c>
+      <c r="C7" s="38" t="s">
+        <v>152</v>
+      </c>
+      <c r="D7" s="38" t="s">
+        <v>155</v>
+      </c>
+      <c r="E7" s="38" t="s">
+        <v>153</v>
+      </c>
+      <c r="F7" s="38" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="38" t="s">
+        <v>151</v>
+      </c>
+      <c r="C8" s="38" t="s">
+        <v>152</v>
+      </c>
+      <c r="D8" s="38" t="s">
+        <v>156</v>
+      </c>
+      <c r="E8" s="38" t="s">
+        <v>153</v>
+      </c>
+      <c r="F8" s="38" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="38" t="s">
+        <v>151</v>
+      </c>
+      <c r="C9" s="38" t="s">
+        <v>152</v>
+      </c>
+      <c r="D9" s="38" t="s">
+        <v>157</v>
+      </c>
+      <c r="E9" s="38" t="s">
+        <v>153</v>
+      </c>
+      <c r="F9" s="38" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="38" t="s">
+        <v>151</v>
+      </c>
+      <c r="C10" s="38" t="s">
+        <v>152</v>
+      </c>
+      <c r="D10" s="38" t="s">
+        <v>158</v>
+      </c>
+      <c r="E10" s="38" t="s">
+        <v>153</v>
+      </c>
+      <c r="F10" s="38" t="s">
+        <v>148</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK10"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -2217,16 +2544,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.08984375" style="19" customWidth="1"/>
-    <col min="2" max="2" width="15.26953125" style="19" customWidth="1"/>
-    <col min="3" max="1025" width="11.54296875" style="19"/>
+    <col min="1" max="1" width="16.08984375" style="17" customWidth="1"/>
+    <col min="2" max="2" width="15.26953125" style="17" customWidth="1"/>
+    <col min="3" max="1025" width="11.54296875" style="17"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="18" t="s">
         <v>59</v>
       </c>
     </row>
@@ -2236,10 +2563,10 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="17" t="s">
         <v>62</v>
       </c>
     </row>
@@ -2247,7 +2574,7 @@
       <c r="A4" t="s">
         <v>63</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="17" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2255,24 +2582,24 @@
       <c r="A5" t="s">
         <v>65</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="D5" s="18" t="s">
         <v>67</v>
       </c>
       <c r="E5"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="17" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="20" t="s">
+      <c r="A9" s="18" t="s">
         <v>54</v>
       </c>
     </row>
@@ -2291,7 +2618,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AMK17"/>
   <sheetViews>
@@ -2301,194 +2628,194 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.7265625" style="21" customWidth="1"/>
-    <col min="2" max="2" width="19.36328125" style="21" customWidth="1"/>
-    <col min="3" max="3" width="14.54296875" style="21" customWidth="1"/>
-    <col min="4" max="4" width="9.26953125" style="21" customWidth="1"/>
-    <col min="5" max="5" width="14.81640625" style="21" customWidth="1"/>
-    <col min="6" max="6" width="54.90625" style="21" customWidth="1"/>
-    <col min="7" max="1025" width="11.54296875" style="21"/>
+    <col min="1" max="1" width="4.7265625" style="19" customWidth="1"/>
+    <col min="2" max="2" width="19.36328125" style="19" customWidth="1"/>
+    <col min="3" max="3" width="14.54296875" style="19" customWidth="1"/>
+    <col min="4" max="4" width="9.26953125" style="19" customWidth="1"/>
+    <col min="5" max="5" width="14.81640625" style="19" customWidth="1"/>
+    <col min="6" max="6" width="54.90625" style="19" customWidth="1"/>
+    <col min="7" max="1025" width="11.54296875" style="19"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="17" x14ac:dyDescent="0.4">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="D4" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="E4" s="23" t="s">
+      <c r="E4" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="F4" s="23" t="s">
+      <c r="F4" s="21" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="C5" s="25">
+      <c r="C5" s="23">
         <v>42792</v>
       </c>
-      <c r="D5" s="26">
+      <c r="D5" s="24">
         <v>0.44097222222222199</v>
       </c>
-      <c r="E5" s="26" t="s">
+      <c r="E5" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="F5" s="26"/>
+      <c r="F5" s="24"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="C6" s="25">
+      <c r="C6" s="23">
         <v>42737</v>
       </c>
-      <c r="D6" s="26">
+      <c r="D6" s="24">
         <v>0.52777777777777801</v>
       </c>
-      <c r="E6" s="26" t="s">
+      <c r="E6" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="F6" s="26"/>
+      <c r="F6" s="24"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="C7" s="25">
+      <c r="C7" s="23">
         <v>43098</v>
       </c>
-      <c r="D7" s="26">
+      <c r="D7" s="24">
         <v>0.52777777777777801</v>
       </c>
-      <c r="E7" s="26" t="s">
+      <c r="E7" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="F7" s="26" t="s">
+      <c r="F7" s="24" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="10" spans="2:9" ht="17" x14ac:dyDescent="0.4">
-      <c r="B10" s="27" t="s">
+      <c r="B10" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="22"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B11" s="22"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="22"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="24"/>
-      <c r="H12" s="24"/>
-      <c r="I12" s="24"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B13" s="22"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="22"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="20"/>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B14" s="23" t="s">
+      <c r="B14" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="C14" s="23" t="s">
+      <c r="C14" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
-      <c r="I14" s="22"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="C15" s="22">
+      <c r="C15" s="20">
         <v>30</v>
       </c>
-      <c r="D15" s="22"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="22"/>
-      <c r="I15" s="22"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B16" s="22" t="s">
+      <c r="B16" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="C16" s="22">
+      <c r="C16" s="20">
         <v>20</v>
       </c>
-      <c r="D16" s="22"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="22"/>
-      <c r="G16" s="22"/>
-      <c r="H16" s="22"/>
-      <c r="I16" s="22"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="20"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B17" s="22" t="s">
+      <c r="B17" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="C17" s="22">
-        <v>0</v>
-      </c>
-      <c r="D17" s="22"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="22"/>
-      <c r="G17" s="22"/>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
+      <c r="C17" s="20">
+        <v>0</v>
+      </c>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
+      <c r="I17" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2503,11 +2830,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
@@ -2525,321 +2852,321 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="34.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="27" t="s">
         <v>127</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="28" t="s">
         <v>128</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="28" t="s">
         <v>129</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="D1" s="28" t="s">
         <v>130</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="E1" s="28" t="s">
         <v>131</v>
       </c>
-      <c r="F1" s="30" t="s">
+      <c r="F1" s="28" t="s">
         <v>132</v>
       </c>
-      <c r="G1" s="30" t="s">
+      <c r="G1" s="28" t="s">
         <v>133</v>
       </c>
-      <c r="H1" s="30" t="s">
+      <c r="H1" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="I1" s="30" t="s">
+      <c r="I1" s="28" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="72.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="D2" s="32" t="s">
+      <c r="D2" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="E2" s="32" t="s">
+      <c r="E2" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="F2" s="32" t="s">
+      <c r="F2" s="30" t="s">
         <v>82</v>
       </c>
-      <c r="G2" s="32" t="s">
+      <c r="G2" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="H2" s="32" t="s">
+      <c r="H2" s="30" t="s">
         <v>84</v>
       </c>
-      <c r="I2" s="32">
+      <c r="I2" s="30">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="96.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="34" t="s">
         <v>80</v>
       </c>
-      <c r="D3" s="35" t="s">
+      <c r="D3" s="33" t="s">
         <v>86</v>
       </c>
-      <c r="E3" s="35" t="s">
+      <c r="E3" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="F3" s="35" t="s">
+      <c r="F3" s="33" t="s">
         <v>87</v>
       </c>
-      <c r="G3" s="35" t="s">
+      <c r="G3" s="33" t="s">
         <v>88</v>
       </c>
-      <c r="H3" s="35" t="s">
+      <c r="H3" s="33" t="s">
         <v>89</v>
       </c>
-      <c r="I3" s="35">
+      <c r="I3" s="33">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="72.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="33" t="s">
         <v>91</v>
       </c>
-      <c r="C4" s="36" t="s">
+      <c r="C4" s="34" t="s">
         <v>80</v>
       </c>
-      <c r="D4" s="35" t="s">
+      <c r="D4" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="E4" s="35" t="s">
+      <c r="E4" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="F4" s="35" t="s">
+      <c r="F4" s="33" t="s">
         <v>92</v>
       </c>
-      <c r="G4" s="35" t="s">
+      <c r="G4" s="33" t="s">
         <v>93</v>
       </c>
-      <c r="H4" s="37" t="s">
+      <c r="H4" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="I4" s="35">
+      <c r="I4" s="33">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="96.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="C5" s="36" t="s">
+      <c r="C5" s="34" t="s">
         <v>80</v>
       </c>
-      <c r="D5" s="35" t="s">
+      <c r="D5" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="E5" s="35" t="s">
+      <c r="E5" s="33" t="s">
         <v>96</v>
       </c>
-      <c r="F5" s="35" t="s">
+      <c r="F5" s="33" t="s">
         <v>97</v>
       </c>
-      <c r="G5" s="35" t="s">
+      <c r="G5" s="33" t="s">
         <v>98</v>
       </c>
-      <c r="H5" s="35" t="s">
+      <c r="H5" s="33" t="s">
         <v>99</v>
       </c>
-      <c r="I5" s="35">
+      <c r="I5" s="33">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="96.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="32" t="s">
         <v>100</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="33" t="s">
         <v>101</v>
       </c>
-      <c r="C6" s="36" t="s">
+      <c r="C6" s="34" t="s">
         <v>102</v>
       </c>
-      <c r="D6" s="35" t="s">
+      <c r="D6" s="33" t="s">
         <v>103</v>
       </c>
-      <c r="E6" s="35" t="s">
+      <c r="E6" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="F6" s="35" t="s">
+      <c r="F6" s="33" t="s">
         <v>104</v>
       </c>
-      <c r="G6" s="35" t="s">
+      <c r="G6" s="33" t="s">
         <v>105</v>
       </c>
-      <c r="H6" s="35" t="s">
+      <c r="H6" s="33" t="s">
         <v>99</v>
       </c>
-      <c r="I6" s="35">
+      <c r="I6" s="33">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="96.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="34" t="s">
+      <c r="A7" s="32" t="s">
         <v>106</v>
       </c>
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="33" t="s">
         <v>107</v>
       </c>
-      <c r="C7" s="36" t="s">
+      <c r="C7" s="34" t="s">
         <v>108</v>
       </c>
-      <c r="D7" s="35" t="s">
+      <c r="D7" s="33" t="s">
         <v>109</v>
       </c>
-      <c r="E7" s="36" t="s">
+      <c r="E7" s="34" t="s">
         <v>80</v>
       </c>
-      <c r="F7" s="35" t="s">
+      <c r="F7" s="33" t="s">
         <v>110</v>
       </c>
-      <c r="G7" s="35" t="s">
+      <c r="G7" s="33" t="s">
         <v>105</v>
       </c>
-      <c r="H7" s="35" t="s">
+      <c r="H7" s="33" t="s">
         <v>99</v>
       </c>
-      <c r="I7" s="35">
+      <c r="I7" s="33">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="96.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="34" t="s">
+      <c r="A8" s="32" t="s">
         <v>111</v>
       </c>
-      <c r="B8" s="35" t="s">
+      <c r="B8" s="33" t="s">
         <v>112</v>
       </c>
-      <c r="C8" s="36" t="s">
+      <c r="C8" s="34" t="s">
         <v>113</v>
       </c>
-      <c r="D8" s="35" t="s">
+      <c r="D8" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="E8" s="35" t="s">
+      <c r="E8" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="F8" s="35" t="s">
+      <c r="F8" s="33" t="s">
         <v>115</v>
       </c>
-      <c r="G8" s="35" t="s">
+      <c r="G8" s="33" t="s">
         <v>105</v>
       </c>
-      <c r="H8" s="35" t="s">
+      <c r="H8" s="33" t="s">
         <v>99</v>
       </c>
-      <c r="I8" s="35">
+      <c r="I8" s="33">
         <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="96.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="34" t="s">
+      <c r="A9" s="32" t="s">
         <v>116</v>
       </c>
-      <c r="B9" s="35" t="s">
+      <c r="B9" s="33" t="s">
         <v>117</v>
       </c>
-      <c r="C9" s="36" t="s">
+      <c r="C9" s="34" t="s">
         <v>118</v>
       </c>
-      <c r="D9" s="35" t="s">
+      <c r="D9" s="33" t="s">
         <v>119</v>
       </c>
-      <c r="E9" s="35" t="s">
+      <c r="E9" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="F9" s="35" t="s">
+      <c r="F9" s="33" t="s">
         <v>120</v>
       </c>
-      <c r="G9" s="35" t="s">
+      <c r="G9" s="33" t="s">
         <v>105</v>
       </c>
-      <c r="H9" s="35" t="s">
+      <c r="H9" s="33" t="s">
         <v>99</v>
       </c>
-      <c r="I9" s="35">
+      <c r="I9" s="33">
         <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="96.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="34" t="s">
+      <c r="A10" s="32" t="s">
         <v>121</v>
       </c>
-      <c r="B10" s="35" t="s">
+      <c r="B10" s="33" t="s">
         <v>101</v>
       </c>
-      <c r="C10" s="36" t="s">
+      <c r="C10" s="34" t="s">
         <v>122</v>
       </c>
-      <c r="D10" s="35" t="s">
+      <c r="D10" s="33" t="s">
         <v>123</v>
       </c>
-      <c r="E10" s="35" t="s">
+      <c r="E10" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="F10" s="35" t="s">
+      <c r="F10" s="33" t="s">
         <v>124</v>
       </c>
-      <c r="G10" s="35" t="s">
+      <c r="G10" s="33" t="s">
         <v>105</v>
       </c>
-      <c r="H10" s="35" t="s">
+      <c r="H10" s="33" t="s">
         <v>99</v>
       </c>
-      <c r="I10" s="35">
+      <c r="I10" s="33">
         <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="96.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="34" t="s">
+      <c r="A11" s="32" t="s">
         <v>125</v>
       </c>
-      <c r="B11" s="35" t="s">
+      <c r="B11" s="33" t="s">
         <v>91</v>
       </c>
-      <c r="C11" s="36" t="s">
+      <c r="C11" s="34" t="s">
         <v>102</v>
       </c>
-      <c r="D11" s="35" t="s">
+      <c r="D11" s="33" t="s">
         <v>109</v>
       </c>
-      <c r="E11" s="35" t="s">
+      <c r="E11" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="F11" s="35" t="s">
+      <c r="F11" s="33" t="s">
         <v>126</v>
       </c>
-      <c r="G11" s="35" t="s">
+      <c r="G11" s="33" t="s">
         <v>105</v>
       </c>
-      <c r="H11" s="35" t="s">
+      <c r="H11" s="33" t="s">
         <v>99</v>
       </c>
-      <c r="I11" s="35">
+      <c r="I11" s="33">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Patient date changes non active
</commit_message>
<xml_diff>
--- a/Data/Test Suite Prerequisites.xlsx
+++ b/Data/Test Suite Prerequisites.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Patients" sheetId="1" r:id="rId1"/>
@@ -1002,8 +1002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK22"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1820,7 +1820,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="2:16" ht="29" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B21" s="14" t="s">
         <v>43</v>
       </c>
@@ -1863,11 +1863,9 @@
       <c r="O21" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="P21" s="6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.35">
+      <c r="P21" s="6"/>
+    </row>
+    <row r="22" spans="2:16" ht="29" x14ac:dyDescent="0.35">
       <c r="B22" s="14" t="s">
         <v>45</v>
       </c>
@@ -1910,7 +1908,9 @@
       <c r="O22" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="P22" s="6"/>
+      <c r="P22" s="6" t="s">
+        <v>44</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2614,7 +2614,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AMK17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fixed retrieve a patients appointments for patient where no appointments should be present. Also removed check for no appointments on successful response cache header test.
</commit_message>
<xml_diff>
--- a/Data/Test Suite Prerequisites.xlsx
+++ b/Data/Test Suite Prerequisites.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Patients" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="101">
   <si>
     <t xml:space="preserve">Cells containing a '0' should not have any data for that section
 Cells containing an 'x' should have data for that section 
@@ -169,6 +169,12 @@
   <si>
     <t xml:space="preserve">Deceased patient.
 Part of multiple birth.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">patientNoAppointments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patient should not have any appointments</t>
   </si>
   <si>
     <t xml:space="preserve">Required Organizations and Slots for testing</t>
@@ -971,17 +977,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:P22"/>
+  <dimension ref="B1:P23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P21" activeCellId="0" sqref="P21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="2.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="3" style="2" width="19.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="3" style="2" width="19.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="25.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="17" style="1" width="11.54"/>
   </cols>
@@ -1879,6 +1885,53 @@
       </c>
       <c r="P22" s="7" t="s">
         <v>45</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="23.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E23" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="F23" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="G23" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="H23" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="I23" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="J23" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="K23" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="L23" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="M23" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="N23" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="O23" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="P23" s="7" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1911,13 +1964,13 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="24.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="29.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="29.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="8.54"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="18.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="18" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C2" s="19"/>
       <c r="D2" s="19"/>
@@ -1932,7 +1985,7 @@
     </row>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="19" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C3" s="19"/>
       <c r="D3" s="19"/>
@@ -1947,13 +2000,13 @@
     </row>
     <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="20" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C5" s="20"/>
     </row>
     <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="21" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C6" s="19"/>
       <c r="D6" s="22"/>
@@ -1961,7 +2014,7 @@
     </row>
     <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="19" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C7" s="19"/>
       <c r="D7" s="22"/>
@@ -1969,7 +2022,7 @@
     </row>
     <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="19" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C8" s="19"/>
       <c r="D8" s="22"/>
@@ -1977,7 +2030,7 @@
     </row>
     <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="19" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C9" s="19"/>
       <c r="D9" s="22"/>
@@ -1993,7 +2046,7 @@
     </row>
     <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="23" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C12" s="19"/>
       <c r="D12" s="19"/>
@@ -2011,10 +2064,10 @@
     </row>
     <row r="14" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="20" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C14" s="20" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D14" s="19"/>
       <c r="E14" s="19"/>
@@ -2023,10 +2076,10 @@
     </row>
     <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="19" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D15" s="19"/>
       <c r="E15" s="19"/>
@@ -2057,7 +2110,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="24" width="3.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="24" width="3.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="24" width="12.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="24" width="16.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="24" width="15.72"/>
@@ -2074,7 +2127,7 @@
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="21.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B2" s="25" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C2" s="25"/>
       <c r="D2" s="25"/>
@@ -2101,28 +2154,28 @@
     <row r="4" customFormat="false" ht="31" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="28"/>
       <c r="C4" s="29" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D4" s="30" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E4" s="30" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="F4" s="30" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="G4" s="30" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="H4" s="29" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="I4" s="30" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="J4" s="29" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="K4" s="31" t="s">
         <v>14</v>
@@ -2130,10 +2183,10 @@
     </row>
     <row r="5" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="32" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C5" s="33" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D5" s="34" t="s">
         <v>21</v>
@@ -2160,10 +2213,10 @@
     </row>
     <row r="6" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="32" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C6" s="33" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D6" s="34" t="s">
         <v>21</v>
@@ -2190,10 +2243,10 @@
     </row>
     <row r="7" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="32" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C7" s="33" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D7" s="34" t="s">
         <v>21</v>
@@ -2220,10 +2273,10 @@
     </row>
     <row r="8" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="32" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C8" s="33" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D8" s="34" t="s">
         <v>21</v>
@@ -2250,10 +2303,10 @@
     </row>
     <row r="9" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="32" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C9" s="33" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D9" s="34" t="s">
         <v>21</v>
@@ -2280,10 +2333,10 @@
     </row>
     <row r="10" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="C10" s="33" t="s">
         <v>74</v>
-      </c>
-      <c r="C10" s="33" t="s">
-        <v>72</v>
       </c>
       <c r="D10" s="34" t="s">
         <v>21</v>
@@ -2310,10 +2363,10 @@
     </row>
     <row r="11" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="32" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C11" s="33" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D11" s="34" t="s">
         <v>21</v>
@@ -2340,10 +2393,10 @@
     </row>
     <row r="12" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="32" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C12" s="33" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D12" s="34" t="s">
         <v>21</v>
@@ -2370,10 +2423,10 @@
     </row>
     <row r="13" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="36" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C13" s="33" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D13" s="34" t="s">
         <v>21</v>
@@ -2400,10 +2453,10 @@
     </row>
     <row r="14" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="36" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C14" s="33" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D14" s="34" t="s">
         <v>21</v>
@@ -2430,10 +2483,10 @@
     </row>
     <row r="15" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="36" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C15" s="33" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D15" s="34" t="s">
         <v>21</v>
@@ -2479,17 +2532,17 @@
   </sheetPr>
   <dimension ref="B1:L12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J15" activeCellId="0" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="37" width="3.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="37" width="3.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="37" width="16.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="37" width="24.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="4" style="37" width="11.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="37" width="46.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="37" width="46.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="37" width="26.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="13" style="37" width="11.54"/>
   </cols>
@@ -2500,7 +2553,7 @@
     </row>
     <row r="2" customFormat="false" ht="18.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="18" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C2" s="19"/>
       <c r="D2" s="19"/>
@@ -2515,7 +2568,7 @@
     </row>
     <row r="3" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="39" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C3" s="39"/>
       <c r="D3" s="39"/>
@@ -2531,15 +2584,15 @@
     <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="20" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="21" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C6" s="40" t="n">
         <v>0</v>
@@ -2547,7 +2600,7 @@
     </row>
     <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="21" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C7" s="40" t="n">
         <v>1</v>
@@ -2555,7 +2608,7 @@
     </row>
     <row r="8" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="21" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C8" s="40" t="n">
         <v>2</v>
@@ -2563,7 +2616,7 @@
     </row>
     <row r="9" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="21" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C9" s="40" t="n">
         <v>1</v>
@@ -2572,13 +2625,13 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="20" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C11" s="39"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="21" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C12" s="21"/>
     </row>
@@ -2611,13 +2664,13 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="22" width="14.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="22" width="9.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="22" width="14.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="22" width="54.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="22" width="54.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="22" width="11.54"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="41" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C2" s="41"/>
       <c r="D2" s="41"/>
@@ -2633,16 +2686,16 @@
     </row>
     <row r="4" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="43" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C4" s="43" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D4" s="43" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="E4" s="43" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="F4" s="43" t="s">
         <v>14</v>
@@ -2650,7 +2703,7 @@
     </row>
     <row r="5" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="40" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C5" s="44" t="n">
         <v>42792</v>
@@ -2659,13 +2712,13 @@
         <v>0.440972222222222</v>
       </c>
       <c r="E5" s="45" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="F5" s="45"/>
     </row>
     <row r="6" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="40" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C6" s="44" t="n">
         <v>42737</v>
@@ -2674,13 +2727,13 @@
         <v>0.527777777777778</v>
       </c>
       <c r="E6" s="45" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="F6" s="45"/>
     </row>
     <row r="7" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="40" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C7" s="44" t="n">
         <v>43098</v>
@@ -2689,15 +2742,15 @@
         <v>0.527777777777778</v>
       </c>
       <c r="E7" s="45" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="F7" s="45" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="17" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="46" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C10" s="42"/>
       <c r="D10" s="42"/>
@@ -2719,7 +2772,7 @@
     </row>
     <row r="12" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="47" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C12" s="40"/>
       <c r="D12" s="40"/>
@@ -2741,10 +2794,10 @@
     </row>
     <row r="14" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="43" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C14" s="43" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D14" s="42"/>
       <c r="E14" s="42"/>
@@ -2755,7 +2808,7 @@
     </row>
     <row r="15" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="42" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C15" s="42" t="n">
         <v>30</v>
@@ -2769,7 +2822,7 @@
     </row>
     <row r="16" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="42" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C16" s="42" t="n">
         <v>20</v>
@@ -2783,7 +2836,7 @@
     </row>
     <row r="17" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="42" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C17" s="42" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
Updates for 1.2.2 appointments
Addresses Issues #108,#109,#111,#112,#115,#116.#117,#118,#119,#120,#121,#122,#123,#124,#125,#126,#131,#132,#133,#134,#135,#136
</commit_message>
<xml_diff>
--- a/Data/Test Suite Prerequisites.xlsx
+++ b/Data/Test Suite Prerequisites.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GPConnect\gpconnect-provider-testing-release-1.2.1\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{247A2DF9-23BF-4181-933B-B409098ABA4E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BE36DA8-73CB-47E6-B0BC-18A4582D4582}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="105">
   <si>
     <t>Required Organizations and Slots for testing</t>
   </si>
@@ -334,6 +334,15 @@
   </si>
   <si>
     <t>Patient has an AllergyIntolerance with no allergy EndReason</t>
+  </si>
+  <si>
+    <t>Patient 19</t>
+  </si>
+  <si>
+    <t>Inactive/not active Patient</t>
+  </si>
+  <si>
+    <t>Patient 21</t>
   </si>
 </sst>
 </file>
@@ -952,16 +961,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.7109375" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" customWidth="1"/>
     <col min="3" max="3" width="19.85546875" customWidth="1"/>
     <col min="4" max="4" width="54" customWidth="1"/>
     <col min="5" max="15" width="19.85546875" customWidth="1"/>
@@ -2116,9 +2125,9 @@
       <c r="Y22" s="6"/>
       <c r="Z22" s="6"/>
     </row>
-    <row r="23" spans="2:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:26" s="31" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="26" t="s">
-        <v>78</v>
+        <v>102</v>
       </c>
       <c r="C23" s="14" t="s">
         <v>29</v>
@@ -2132,36 +2141,34 @@
       <c r="F23" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="G23" s="15" t="s">
+      <c r="G23" s="22" t="s">
         <v>29</v>
       </c>
       <c r="H23" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="I23" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="J23" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="K23" s="15" t="s">
+      <c r="I23" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="J23" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="K23" s="22" t="s">
         <v>29</v>
       </c>
       <c r="L23" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="M23" s="15" t="s">
+      <c r="M23" s="22" t="s">
         <v>29</v>
       </c>
       <c r="N23" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="O23" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="P23" s="16" t="s">
-        <v>80</v>
-      </c>
+      <c r="O23" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="P23" s="16"/>
       <c r="Q23" s="6"/>
       <c r="R23" s="6"/>
       <c r="S23" s="6"/>
@@ -2174,21 +2181,51 @@
       <c r="Z23" s="6"/>
     </row>
     <row r="24" spans="2:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="6"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
-      <c r="L24" s="2"/>
-      <c r="M24" s="2"/>
-      <c r="N24" s="2"/>
-      <c r="O24" s="2"/>
-      <c r="P24" s="6"/>
+      <c r="B24" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D24" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="E24" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="F24" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G24" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="H24" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="I24" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="J24" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="K24" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="L24" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M24" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="N24" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="O24" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="P24" s="16" t="s">
+        <v>80</v>
+      </c>
       <c r="Q24" s="6"/>
       <c r="R24" s="6"/>
       <c r="S24" s="6"/>
@@ -2200,7 +2237,63 @@
       <c r="Y24" s="6"/>
       <c r="Z24" s="6"/>
     </row>
-    <row r="25" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="2:26" s="31" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D25" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="E25" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="F25" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G25" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="H25" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="I25" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="J25" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="K25" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="L25" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M25" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="N25" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="O25" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="P25" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q25" s="6"/>
+      <c r="R25" s="6"/>
+      <c r="S25" s="6"/>
+      <c r="T25" s="6"/>
+      <c r="U25" s="6"/>
+      <c r="V25" s="6"/>
+      <c r="W25" s="6"/>
+      <c r="X25" s="6"/>
+      <c r="Y25" s="6"/>
+      <c r="Z25" s="6"/>
+    </row>
     <row r="26" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="28" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3176,6 +3269,7 @@
     <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:P2"/>

</xml_diff>

<commit_message>
finalised new warning code tests all are targeted at pateint16 and have updated pateint16 data requirements
</commit_message>
<xml_diff>
--- a/Data/Test Suite Prerequisites.xlsx
+++ b/Data/Test Suite Prerequisites.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GPConnect\gpconnect-provider-testing-release-1.2.1\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\development\feature\1.2.4\gpconnect-provider-testing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BE36DA8-73CB-47E6-B0BC-18A4582D4582}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B88F7DD-E436-44EB-9628-9190CAB427D0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Patients" sheetId="1" r:id="rId1"/>
@@ -333,9 +333,6 @@
     <t>Number of slots</t>
   </si>
   <si>
-    <t>Patient has an AllergyIntolerance with no allergy EndReason</t>
-  </si>
-  <si>
     <t>Patient 19</t>
   </si>
   <si>
@@ -343,6 +340,10 @@
   </si>
   <si>
     <t>Patient 21</t>
+  </si>
+  <si>
+    <t>Patient has an AllergyIntolerance with no allergy EndReason
+Patient Has Warning Codes :  Data in Transit &amp;  Data Awaiting Filing &amp;  Confidential Items on  Allergies</t>
   </si>
 </sst>
 </file>
@@ -964,7 +965,7 @@
   <dimension ref="A1:Z1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1956,7 +1957,7 @@
       <c r="Y19" s="6"/>
       <c r="Z19" s="6"/>
     </row>
-    <row r="20" spans="2:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:26" ht="45" x14ac:dyDescent="0.25">
       <c r="B20" s="26" t="s">
         <v>71</v>
       </c>
@@ -2000,7 +2001,7 @@
         <v>29</v>
       </c>
       <c r="P20" s="39" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="Q20" s="6"/>
       <c r="R20" s="6"/>
@@ -2127,7 +2128,7 @@
     </row>
     <row r="23" spans="2:26" s="31" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="26" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C23" s="14" t="s">
         <v>29</v>
@@ -2239,7 +2240,7 @@
     </row>
     <row r="25" spans="2:26" s="31" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="26" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C25" s="14" t="s">
         <v>29</v>
@@ -2281,7 +2282,7 @@
         <v>29</v>
       </c>
       <c r="P25" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="Q25" s="6"/>
       <c r="R25" s="6"/>

</xml_diff>

<commit_message>
Update Test Suite Prerequisites.xlsx
Updated Pre Requisites spreadsheet
</commit_message>
<xml_diff>
--- a/Data/Test Suite Prerequisites.xlsx
+++ b/Data/Test Suite Prerequisites.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\development\feature\1.2.4\gpconnect-provider-testing\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\development\feature\1.3.1\1.3.1-imm-and-uncat\gpconnect-provider-testing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B88F7DD-E436-44EB-9628-9190CAB427D0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7EECDF4-097F-48F9-B4B0-234D405BCE8A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="106">
   <si>
     <t>Required Organizations and Slots for testing</t>
   </si>
@@ -74,9 +74,6 @@
     <t>Encounters</t>
   </si>
   <si>
-    <t>Immunisations</t>
-  </si>
-  <si>
     <t>Current Medications</t>
   </si>
   <si>
@@ -342,8 +339,14 @@
     <t>Patient 21</t>
   </si>
   <si>
+    <t>Immunizations</t>
+  </si>
+  <si>
+    <t>Uncategorised</t>
+  </si>
+  <si>
     <t>Patient has an AllergyIntolerance with no allergy EndReason
-Patient Has Warning Codes :  Data in Transit &amp;  Data Awaiting Filing &amp;  Confidential Items on  Allergies</t>
+Patient Has Warning Codes :  Data in Transit &amp;  Confidential Items on  Allergies</t>
   </si>
 </sst>
 </file>
@@ -507,7 +510,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -620,6 +623,7 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -962,10 +966,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1001"/>
+  <dimension ref="A1:AA1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -974,12 +978,13 @@
     <col min="2" max="2" width="22.5703125" customWidth="1"/>
     <col min="3" max="3" width="19.85546875" customWidth="1"/>
     <col min="4" max="4" width="54" customWidth="1"/>
-    <col min="5" max="15" width="19.85546875" customWidth="1"/>
-    <col min="16" max="16" width="62.7109375" customWidth="1"/>
-    <col min="17" max="26" width="11.5703125" customWidth="1"/>
+    <col min="5" max="14" width="19.85546875" customWidth="1"/>
+    <col min="15" max="16" width="19.85546875" style="31" customWidth="1"/>
+    <col min="17" max="17" width="62.7109375" customWidth="1"/>
+    <col min="18" max="27" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -1006,8 +1011,9 @@
       <c r="X1" s="2"/>
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
-    </row>
-    <row r="2" spans="1:26" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA1" s="2"/>
+    </row>
+    <row r="2" spans="1:27" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="40" t="s">
         <v>2</v>
       </c>
@@ -1023,9 +1029,9 @@
       <c r="L2" s="41"/>
       <c r="M2" s="41"/>
       <c r="N2" s="41"/>
-      <c r="O2" s="41"/>
-      <c r="P2" s="41"/>
-      <c r="Q2" s="6"/>
+      <c r="O2" s="44"/>
+      <c r="P2" s="44"/>
+      <c r="Q2" s="41"/>
       <c r="R2" s="6"/>
       <c r="S2" s="6"/>
       <c r="T2" s="6"/>
@@ -1035,8 +1041,9 @@
       <c r="X2" s="6"/>
       <c r="Y2" s="6"/>
       <c r="Z2" s="6"/>
-    </row>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA2" s="6"/>
+    </row>
+    <row r="3" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="6"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -1051,7 +1058,7 @@
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
-      <c r="P3" s="6"/>
+      <c r="P3" s="2"/>
       <c r="Q3" s="6"/>
       <c r="R3" s="6"/>
       <c r="S3" s="6"/>
@@ -1062,8 +1069,9 @@
       <c r="X3" s="6"/>
       <c r="Y3" s="6"/>
       <c r="Z3" s="6"/>
-    </row>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA3" s="6"/>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B4" s="8"/>
       <c r="C4" s="10" t="s">
         <v>5</v>
@@ -1080,34 +1088,36 @@
       <c r="G4" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="H4" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="I4" s="12" t="s">
+      <c r="I4" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="J4" s="12" t="s">
+      <c r="J4" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="K4" s="12" t="s">
+      <c r="K4" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="L4" s="10" t="s">
+      <c r="L4" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="M4" s="12" t="s">
+      <c r="M4" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="N4" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="O4" s="15" t="s">
+      <c r="N4" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="O4" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="P4" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="Q4" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="P4" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q4" s="6"/>
       <c r="R4" s="6"/>
       <c r="S4" s="6"/>
       <c r="T4" s="6"/>
@@ -1117,52 +1127,51 @@
       <c r="X4" s="6"/>
       <c r="Y4" s="6"/>
       <c r="Z4" s="6"/>
-    </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA4" s="6"/>
+    </row>
+    <row r="5" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C5" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="15" t="s">
         <v>29</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>30</v>
       </c>
       <c r="E5" s="15">
         <v>0</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G5" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="H5" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="I5" s="15">
+        <v>28</v>
+      </c>
+      <c r="H5" s="14">
         <v>0</v>
       </c>
-      <c r="J5" s="15">
+      <c r="I5" s="14">
         <v>0</v>
       </c>
-      <c r="K5" s="15">
+      <c r="J5" s="14">
         <v>0</v>
       </c>
+      <c r="K5" s="22" t="s">
+        <v>28</v>
+      </c>
       <c r="L5" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="M5" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="N5" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="O5" s="15">
+        <v>28</v>
+      </c>
+      <c r="M5" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="N5" s="22">
         <v>0</v>
       </c>
-      <c r="P5" s="20"/>
-      <c r="Q5" s="6"/>
+      <c r="O5" s="14"/>
+      <c r="P5" s="22"/>
+      <c r="Q5" s="20"/>
       <c r="R5" s="6"/>
       <c r="S5" s="6"/>
       <c r="T5" s="6"/>
@@ -1172,52 +1181,55 @@
       <c r="X5" s="6"/>
       <c r="Y5" s="6"/>
       <c r="Z5" s="6"/>
-    </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA5" s="6"/>
+    </row>
+    <row r="6" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" s="15" t="s">
+      <c r="E6" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="G6" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="H6" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="I6" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="J6" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="K6" s="15" t="s">
-        <v>33</v>
+      <c r="I6" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="J6" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="K6" s="22" t="s">
+        <v>28</v>
       </c>
       <c r="L6" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="M6" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="N6" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="O6" s="15">
+        <v>28</v>
+      </c>
+      <c r="M6" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="N6" s="22">
         <v>0</v>
       </c>
-      <c r="P6" s="20"/>
-      <c r="Q6" s="6"/>
+      <c r="O6" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="P6" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q6" s="20"/>
       <c r="R6" s="6"/>
       <c r="S6" s="6"/>
       <c r="T6" s="6"/>
@@ -1227,52 +1239,51 @@
       <c r="X6" s="6"/>
       <c r="Y6" s="6"/>
       <c r="Z6" s="6"/>
-    </row>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA6" s="6"/>
+    </row>
+    <row r="7" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G7" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="H7" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="I7" s="15">
+        <v>28</v>
+      </c>
+      <c r="H7" s="14">
         <v>0</v>
       </c>
-      <c r="J7" s="15">
+      <c r="I7" s="14">
         <v>0</v>
       </c>
-      <c r="K7" s="15" t="s">
-        <v>33</v>
+      <c r="J7" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="K7" s="22" t="s">
+        <v>28</v>
       </c>
       <c r="L7" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="M7" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="N7" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="O7" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="P7" s="20"/>
-      <c r="Q7" s="6"/>
+        <v>28</v>
+      </c>
+      <c r="M7" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="N7" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="O7" s="14"/>
+      <c r="P7" s="22"/>
+      <c r="Q7" s="20"/>
       <c r="R7" s="6"/>
       <c r="S7" s="6"/>
       <c r="T7" s="6"/>
@@ -1282,52 +1293,55 @@
       <c r="X7" s="6"/>
       <c r="Y7" s="6"/>
       <c r="Z7" s="6"/>
-    </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA7" s="6"/>
+    </row>
+    <row r="8" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G8" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="H8" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="I8" s="15">
+        <v>28</v>
+      </c>
+      <c r="H8" s="14">
         <v>0</v>
       </c>
-      <c r="J8" s="15">
+      <c r="I8" s="14">
         <v>0</v>
       </c>
-      <c r="K8" s="15">
+      <c r="J8" s="14">
         <v>0</v>
       </c>
+      <c r="K8" s="22" t="s">
+        <v>28</v>
+      </c>
       <c r="L8" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="M8" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="N8" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="O8" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="P8" s="20"/>
-      <c r="Q8" s="6"/>
+        <v>28</v>
+      </c>
+      <c r="M8" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="N8" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="O8" s="14">
+        <v>0</v>
+      </c>
+      <c r="P8" s="22">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="20"/>
       <c r="R8" s="6"/>
       <c r="S8" s="6"/>
       <c r="T8" s="6"/>
@@ -1337,52 +1351,51 @@
       <c r="X8" s="6"/>
       <c r="Y8" s="6"/>
       <c r="Z8" s="6"/>
-    </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA8" s="6"/>
+    </row>
+    <row r="9" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="15" t="s">
         <v>44</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>45</v>
       </c>
       <c r="E9" s="15">
         <v>0</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G9" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H9" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="I9" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="J9" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="K9" s="15">
+        <v>32</v>
+      </c>
+      <c r="I9" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="J9" s="14">
         <v>0</v>
       </c>
+      <c r="K9" s="22" t="s">
+        <v>28</v>
+      </c>
       <c r="L9" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="M9" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="N9" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="O9" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="P9" s="20"/>
-      <c r="Q9" s="6"/>
+        <v>28</v>
+      </c>
+      <c r="M9" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="N9" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="O9" s="14"/>
+      <c r="P9" s="22"/>
+      <c r="Q9" s="20"/>
       <c r="R9" s="6"/>
       <c r="S9" s="6"/>
       <c r="T9" s="6"/>
@@ -1392,52 +1405,51 @@
       <c r="X9" s="6"/>
       <c r="Y9" s="6"/>
       <c r="Z9" s="6"/>
-    </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA9" s="6"/>
+    </row>
+    <row r="10" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="18" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G10" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H10" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="I10" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="J10" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="K10" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="I10" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="J10" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="K10" s="22" t="s">
+        <v>28</v>
       </c>
       <c r="L10" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="M10" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="N10" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="O10" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="P10" s="20"/>
-      <c r="Q10" s="6"/>
+        <v>28</v>
+      </c>
+      <c r="M10" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="N10" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="O10" s="14"/>
+      <c r="P10" s="22"/>
+      <c r="Q10" s="20"/>
       <c r="R10" s="6"/>
       <c r="S10" s="6"/>
       <c r="T10" s="6"/>
@@ -1447,52 +1459,51 @@
       <c r="X10" s="6"/>
       <c r="Y10" s="6"/>
       <c r="Z10" s="6"/>
-    </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA10" s="6"/>
+    </row>
+    <row r="11" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G11" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H11" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="I11" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="J11" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="K11" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="I11" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="J11" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="K11" s="22" t="s">
+        <v>28</v>
       </c>
       <c r="L11" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="M11" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="N11" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="O11" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="P11" s="20"/>
-      <c r="Q11" s="6"/>
+        <v>28</v>
+      </c>
+      <c r="M11" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="N11" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="O11" s="14"/>
+      <c r="P11" s="22"/>
+      <c r="Q11" s="20"/>
       <c r="R11" s="6"/>
       <c r="S11" s="6"/>
       <c r="T11" s="6"/>
@@ -1502,52 +1513,51 @@
       <c r="X11" s="6"/>
       <c r="Y11" s="6"/>
       <c r="Z11" s="6"/>
-    </row>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA11" s="6"/>
+    </row>
+    <row r="12" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G12" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H12" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="I12" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="J12" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="K12" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="I12" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="J12" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="K12" s="22" t="s">
+        <v>28</v>
       </c>
       <c r="L12" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="M12" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="N12" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="O12" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="P12" s="20"/>
-      <c r="Q12" s="6"/>
+        <v>28</v>
+      </c>
+      <c r="M12" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="N12" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="O12" s="14"/>
+      <c r="P12" s="22"/>
+      <c r="Q12" s="20"/>
       <c r="R12" s="6"/>
       <c r="S12" s="6"/>
       <c r="T12" s="6"/>
@@ -1557,54 +1567,53 @@
       <c r="X12" s="6"/>
       <c r="Y12" s="6"/>
       <c r="Z12" s="6"/>
-    </row>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA12" s="6"/>
+    </row>
+    <row r="13" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="G13" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="H13" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="I13" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="J13" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="K13" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="L13" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="M13" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="N13" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="O13" s="14"/>
+      <c r="P13" s="22"/>
+      <c r="Q13" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="C13" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="E13" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="F13" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="G13" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="H13" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="I13" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="J13" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="K13" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="L13" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="M13" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="N13" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="O13" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="P13" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q13" s="6"/>
       <c r="R13" s="6"/>
       <c r="S13" s="6"/>
       <c r="T13" s="6"/>
@@ -1614,54 +1623,53 @@
       <c r="X13" s="6"/>
       <c r="Y13" s="6"/>
       <c r="Z13" s="6"/>
-    </row>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA13" s="6"/>
+    </row>
+    <row r="14" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="26" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G14" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H14" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="I14" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="J14" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="K14" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="I14" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="J14" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="K14" s="22" t="s">
+        <v>28</v>
       </c>
       <c r="L14" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="M14" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="N14" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="O14" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="P14" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q14" s="6"/>
+        <v>28</v>
+      </c>
+      <c r="M14" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="N14" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="O14" s="14"/>
+      <c r="P14" s="22"/>
+      <c r="Q14" s="16" t="s">
+        <v>50</v>
+      </c>
       <c r="R14" s="6"/>
       <c r="S14" s="6"/>
       <c r="T14" s="6"/>
@@ -1671,54 +1679,53 @@
       <c r="X14" s="6"/>
       <c r="Y14" s="6"/>
       <c r="Z14" s="6"/>
-    </row>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA14" s="6"/>
+    </row>
+    <row r="15" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="G15" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="H15" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="I15" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="J15" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="K15" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="L15" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="M15" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="N15" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="O15" s="14"/>
+      <c r="P15" s="22"/>
+      <c r="Q15" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="C15" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="E15" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="F15" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="G15" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="H15" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="I15" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="J15" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="K15" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="L15" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="M15" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="N15" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="O15" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="P15" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q15" s="6"/>
       <c r="R15" s="6"/>
       <c r="S15" s="6"/>
       <c r="T15" s="6"/>
@@ -1728,54 +1735,53 @@
       <c r="X15" s="6"/>
       <c r="Y15" s="6"/>
       <c r="Z15" s="6"/>
-    </row>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA15" s="6"/>
+    </row>
+    <row r="16" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="G16" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="H16" s="14">
+        <v>0</v>
+      </c>
+      <c r="I16" s="14">
+        <v>0</v>
+      </c>
+      <c r="J16" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="K16" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="L16" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="M16" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="N16" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="O16" s="14"/>
+      <c r="P16" s="22"/>
+      <c r="Q16" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="C16" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="D16" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="E16" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="F16" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="G16" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="H16" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="I16" s="15">
-        <v>0</v>
-      </c>
-      <c r="J16" s="15">
-        <v>0</v>
-      </c>
-      <c r="K16" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="L16" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="M16" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="N16" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="O16" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="P16" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q16" s="6"/>
       <c r="R16" s="6"/>
       <c r="S16" s="6"/>
       <c r="T16" s="6"/>
@@ -1785,54 +1791,53 @@
       <c r="X16" s="6"/>
       <c r="Y16" s="6"/>
       <c r="Z16" s="6"/>
-    </row>
-    <row r="17" spans="2:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA16" s="6"/>
+    </row>
+    <row r="17" spans="2:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="26" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F17" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G17" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H17" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="I17" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="J17" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="K17" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="I17" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="J17" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="K17" s="22" t="s">
+        <v>28</v>
       </c>
       <c r="L17" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="M17" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="N17" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="O17" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="P17" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q17" s="6"/>
+        <v>28</v>
+      </c>
+      <c r="M17" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="N17" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="O17" s="14"/>
+      <c r="P17" s="22"/>
+      <c r="Q17" s="16" t="s">
+        <v>59</v>
+      </c>
       <c r="R17" s="6"/>
       <c r="S17" s="6"/>
       <c r="T17" s="6"/>
@@ -1842,54 +1847,53 @@
       <c r="X17" s="6"/>
       <c r="Y17" s="6"/>
       <c r="Z17" s="6"/>
-    </row>
-    <row r="18" spans="2:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA17" s="6"/>
+    </row>
+    <row r="18" spans="2:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D18" s="22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F18" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G18" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H18" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="I18" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="J18" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="K18" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="I18" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="J18" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="K18" s="22" t="s">
+        <v>28</v>
       </c>
       <c r="L18" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="M18" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="N18" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="O18" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="P18" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q18" s="6"/>
+        <v>28</v>
+      </c>
+      <c r="M18" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="N18" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="O18" s="14"/>
+      <c r="P18" s="22"/>
+      <c r="Q18" s="16" t="s">
+        <v>65</v>
+      </c>
       <c r="R18" s="6"/>
       <c r="S18" s="6"/>
       <c r="T18" s="6"/>
@@ -1899,54 +1903,53 @@
       <c r="X18" s="6"/>
       <c r="Y18" s="6"/>
       <c r="Z18" s="6"/>
-    </row>
-    <row r="19" spans="2:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA18" s="6"/>
+    </row>
+    <row r="19" spans="2:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="26" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F19" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G19" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H19" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="I19" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="J19" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="K19" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="I19" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="J19" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="K19" s="22" t="s">
+        <v>28</v>
       </c>
       <c r="L19" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="M19" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="N19" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="O19" s="15">
+        <v>28</v>
+      </c>
+      <c r="M19" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="N19" s="22">
         <v>0</v>
       </c>
-      <c r="P19" s="16" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q19" s="6"/>
+      <c r="O19" s="14"/>
+      <c r="P19" s="22"/>
+      <c r="Q19" s="16" t="s">
+        <v>68</v>
+      </c>
       <c r="R19" s="6"/>
       <c r="S19" s="6"/>
       <c r="T19" s="6"/>
@@ -1956,54 +1959,53 @@
       <c r="X19" s="6"/>
       <c r="Y19" s="6"/>
       <c r="Z19" s="6"/>
-    </row>
-    <row r="20" spans="2:26" ht="45" x14ac:dyDescent="0.25">
+      <c r="AA19" s="6"/>
+    </row>
+    <row r="20" spans="2:27" ht="45" x14ac:dyDescent="0.25">
       <c r="B20" s="26" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D20" s="29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E20" s="29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F20" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G20" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H20" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="I20" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="J20" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="K20" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="I20" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="J20" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="K20" s="22" t="s">
+        <v>28</v>
       </c>
       <c r="L20" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="M20" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="N20" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="O20" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="P20" s="39" t="s">
-        <v>104</v>
-      </c>
-      <c r="Q20" s="6"/>
+        <v>28</v>
+      </c>
+      <c r="M20" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="N20" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="O20" s="14"/>
+      <c r="P20" s="22"/>
+      <c r="Q20" s="39" t="s">
+        <v>105</v>
+      </c>
       <c r="R20" s="6"/>
       <c r="S20" s="6"/>
       <c r="T20" s="6"/>
@@ -2013,52 +2015,51 @@
       <c r="X20" s="6"/>
       <c r="Y20" s="6"/>
       <c r="Z20" s="6"/>
-    </row>
-    <row r="21" spans="2:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA20" s="6"/>
+    </row>
+    <row r="21" spans="2:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D21" s="22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E21" s="29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F21" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G21" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H21" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="I21" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="J21" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="K21" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="I21" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="J21" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="K21" s="22" t="s">
+        <v>28</v>
       </c>
       <c r="L21" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="M21" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="N21" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="O21" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="P21" s="20"/>
-      <c r="Q21" s="6"/>
+        <v>28</v>
+      </c>
+      <c r="M21" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="N21" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="O21" s="14"/>
+      <c r="P21" s="22"/>
+      <c r="Q21" s="20"/>
       <c r="R21" s="6"/>
       <c r="S21" s="6"/>
       <c r="T21" s="6"/>
@@ -2068,54 +2069,53 @@
       <c r="X21" s="6"/>
       <c r="Y21" s="6"/>
       <c r="Z21" s="6"/>
-    </row>
-    <row r="22" spans="2:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA21" s="6"/>
+    </row>
+    <row r="22" spans="2:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="E22" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="G22" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="H22" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="I22" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="J22" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="K22" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="L22" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="M22" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="N22" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="O22" s="14"/>
+      <c r="P22" s="22"/>
+      <c r="Q22" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="C22" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="D22" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="E22" s="29" t="s">
-        <v>29</v>
-      </c>
-      <c r="F22" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="G22" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="H22" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="I22" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="J22" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="K22" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="L22" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="M22" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="N22" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="O22" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="P22" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q22" s="6"/>
       <c r="R22" s="6"/>
       <c r="S22" s="6"/>
       <c r="T22" s="6"/>
@@ -2125,52 +2125,51 @@
       <c r="X22" s="6"/>
       <c r="Y22" s="6"/>
       <c r="Z22" s="6"/>
-    </row>
-    <row r="23" spans="2:26" s="31" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA22" s="6"/>
+    </row>
+    <row r="23" spans="2:27" s="31" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="26" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D23" s="29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E23" s="29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F23" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G23" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H23" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="I23" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="J23" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="I23" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="J23" s="14" t="s">
+        <v>28</v>
       </c>
       <c r="K23" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L23" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="M23" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="N23" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="O23" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="P23" s="16"/>
-      <c r="Q23" s="6"/>
+        <v>28</v>
+      </c>
+      <c r="M23" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="N23" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="O23" s="14"/>
+      <c r="P23" s="22"/>
+      <c r="Q23" s="16"/>
       <c r="R23" s="6"/>
       <c r="S23" s="6"/>
       <c r="T23" s="6"/>
@@ -2180,54 +2179,53 @@
       <c r="X23" s="6"/>
       <c r="Y23" s="6"/>
       <c r="Z23" s="6"/>
-    </row>
-    <row r="24" spans="2:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA23" s="6"/>
+    </row>
+    <row r="24" spans="2:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="26" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D24" s="29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E24" s="29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F24" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G24" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H24" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="I24" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="J24" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="K24" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="I24" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="J24" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="K24" s="22" t="s">
+        <v>28</v>
       </c>
       <c r="L24" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="M24" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="N24" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="O24" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="P24" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="Q24" s="6"/>
+        <v>28</v>
+      </c>
+      <c r="M24" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="N24" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="O24" s="14"/>
+      <c r="P24" s="22"/>
+      <c r="Q24" s="16" t="s">
+        <v>79</v>
+      </c>
       <c r="R24" s="6"/>
       <c r="S24" s="6"/>
       <c r="T24" s="6"/>
@@ -2237,54 +2235,53 @@
       <c r="X24" s="6"/>
       <c r="Y24" s="6"/>
       <c r="Z24" s="6"/>
-    </row>
-    <row r="25" spans="2:26" s="31" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA24" s="6"/>
+    </row>
+    <row r="25" spans="2:27" s="31" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="26" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D25" s="29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E25" s="29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F25" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G25" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H25" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="I25" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="J25" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="I25" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="J25" s="14" t="s">
+        <v>28</v>
       </c>
       <c r="K25" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L25" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="M25" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="N25" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="O25" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="P25" s="16" t="s">
-        <v>102</v>
-      </c>
-      <c r="Q25" s="6"/>
+        <v>28</v>
+      </c>
+      <c r="M25" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="N25" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="O25" s="14"/>
+      <c r="P25" s="22"/>
+      <c r="Q25" s="16" t="s">
+        <v>101</v>
+      </c>
       <c r="R25" s="6"/>
       <c r="S25" s="6"/>
       <c r="T25" s="6"/>
@@ -2294,14 +2291,15 @@
       <c r="X25" s="6"/>
       <c r="Y25" s="6"/>
       <c r="Z25" s="6"/>
-    </row>
-    <row r="26" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="AA25" s="6"/>
+    </row>
+    <row r="26" spans="2:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="2:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="2:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="2:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="2:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="2:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="2:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3273,7 +3271,7 @@
     <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B2:P2"/>
+    <mergeCell ref="B2:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3396,7 +3394,7 @@
         <v>4</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
@@ -3405,10 +3403,10 @@
     </row>
     <row r="15" spans="2:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="7" t="s">
         <v>23</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>24</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
@@ -4507,31 +4505,31 @@
       <c r="A4" s="1"/>
       <c r="B4" s="17"/>
       <c r="C4" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E4" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="F4" s="21" t="s">
+      <c r="G4" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="G4" s="21" t="s">
+      <c r="H4" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="H4" s="19" t="s">
+      <c r="I4" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="I4" s="21" t="s">
+      <c r="J4" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="J4" s="19" t="s">
-        <v>40</v>
-      </c>
       <c r="K4" s="23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
@@ -4547,31 +4545,31 @@
     <row r="5" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D5" s="27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E5" s="27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F5" s="27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G5" s="27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H5" s="25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I5" s="27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J5" s="25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K5" s="28"/>
       <c r="L5" s="1"/>
@@ -4588,31 +4586,31 @@
     <row r="6" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="25" t="s">
-        <v>59</v>
-      </c>
       <c r="D6" s="27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E6" s="27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F6" s="27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G6" s="27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H6" s="25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I6" s="27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J6" s="25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K6" s="28"/>
       <c r="L6" s="1"/>
@@ -4629,31 +4627,31 @@
     <row r="7" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E7" s="27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F7" s="27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G7" s="27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H7" s="25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I7" s="27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J7" s="25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K7" s="28"/>
       <c r="L7" s="1"/>
@@ -4670,31 +4668,31 @@
     <row r="8" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="C8" s="25" t="s">
-        <v>65</v>
-      </c>
       <c r="D8" s="27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E8" s="27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F8" s="27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G8" s="27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H8" s="25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I8" s="27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J8" s="25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K8" s="28"/>
       <c r="L8" s="1"/>
@@ -4711,31 +4709,31 @@
     <row r="9" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="24" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D9" s="27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E9" s="27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F9" s="27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G9" s="27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H9" s="25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I9" s="27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J9" s="25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K9" s="28"/>
       <c r="L9" s="1"/>
@@ -4752,31 +4750,31 @@
     <row r="10" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="24" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D10" s="27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E10" s="27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F10" s="27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G10" s="27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H10" s="25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I10" s="27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J10" s="25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K10" s="28"/>
       <c r="L10" s="1"/>
@@ -4793,31 +4791,31 @@
     <row r="11" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="24" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D11" s="27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E11" s="27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F11" s="27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G11" s="27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H11" s="25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I11" s="27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J11" s="25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K11" s="28"/>
       <c r="L11" s="1"/>
@@ -4834,31 +4832,31 @@
     <row r="12" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="24" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D12" s="27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E12" s="27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F12" s="27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G12" s="27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H12" s="25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I12" s="27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J12" s="25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K12" s="28"/>
       <c r="L12" s="1"/>
@@ -4875,31 +4873,31 @@
     <row r="13" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="30" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D13" s="27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E13" s="27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F13" s="27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G13" s="27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H13" s="25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I13" s="27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J13" s="25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K13" s="23"/>
       <c r="L13" s="1"/>
@@ -4916,31 +4914,31 @@
     <row r="14" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="30" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D14" s="27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E14" s="27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F14" s="27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G14" s="27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H14" s="25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I14" s="27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J14" s="25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K14" s="23"/>
       <c r="L14" s="1"/>
@@ -4957,31 +4955,31 @@
     <row r="15" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="30" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D15" s="27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E15" s="27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F15" s="27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G15" s="27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H15" s="25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I15" s="27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J15" s="25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="K15" s="23"/>
       <c r="L15" s="1"/>
@@ -6156,7 +6154,7 @@
     <row r="2" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="31"/>
       <c r="B2" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
@@ -6173,7 +6171,7 @@
     <row r="3" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="31"/>
       <c r="B3" s="33" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C3" s="33"/>
       <c r="D3" s="33"/>
@@ -6205,10 +6203,10 @@
     <row r="5" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="31"/>
       <c r="B5" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C5" s="9" t="s">
         <v>85</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>86</v>
       </c>
       <c r="D5" s="31"/>
       <c r="E5" s="31"/>
@@ -6224,7 +6222,7 @@
     <row r="6" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="31"/>
       <c r="B6" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C6" s="34">
         <v>0</v>
@@ -6243,7 +6241,7 @@
     <row r="7" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="31"/>
       <c r="B7" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C7" s="34">
         <v>1</v>
@@ -6262,7 +6260,7 @@
     <row r="8" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="31"/>
       <c r="B8" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C8" s="34">
         <v>2</v>
@@ -6281,7 +6279,7 @@
     <row r="9" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="31"/>
       <c r="B9" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C9" s="34">
         <v>1</v>
@@ -6315,7 +6313,7 @@
     <row r="11" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="31"/>
       <c r="B11" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C11" s="33"/>
       <c r="D11" s="31"/>
@@ -6332,7 +6330,7 @@
     <row r="12" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="31"/>
       <c r="B12" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="31"/>
@@ -7508,7 +7506,7 @@
     <row r="2" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11"/>
       <c r="B2" s="43" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C2" s="41"/>
       <c r="D2" s="41"/>
@@ -7549,16 +7547,16 @@
         <v>4</v>
       </c>
       <c r="C4" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="D4" s="35" t="s">
         <v>93</v>
       </c>
-      <c r="D4" s="35" t="s">
+      <c r="E4" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="E4" s="35" t="s">
-        <v>95</v>
-      </c>
       <c r="F4" s="35" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G4" s="11"/>
       <c r="H4" s="11"/>
@@ -7583,7 +7581,7 @@
         <v>0.44097222222222199</v>
       </c>
       <c r="E5" s="37" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F5" s="37"/>
       <c r="G5" s="11"/>
@@ -7609,7 +7607,7 @@
         <v>0.52777777777777801</v>
       </c>
       <c r="E6" s="37" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F6" s="37"/>
       <c r="G6" s="11"/>
@@ -7635,10 +7633,10 @@
         <v>0.52777777777777801</v>
       </c>
       <c r="E7" s="37" t="s">
+        <v>95</v>
+      </c>
+      <c r="F7" s="37" t="s">
         <v>96</v>
-      </c>
-      <c r="F7" s="37" t="s">
-        <v>97</v>
       </c>
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
@@ -7690,7 +7688,7 @@
     <row r="10" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11"/>
       <c r="B10" s="38" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C10" s="34"/>
       <c r="D10" s="34"/>
@@ -7728,7 +7726,7 @@
     <row r="12" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11"/>
       <c r="B12" s="34" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C12" s="34"/>
       <c r="D12" s="34"/>
@@ -7769,7 +7767,7 @@
         <v>4</v>
       </c>
       <c r="C14" s="35" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D14" s="34"/>
       <c r="E14" s="34"/>

</xml_diff>

<commit_message>
Added new traits and started work on 1.3.2 changes
</commit_message>
<xml_diff>
--- a/Data/Test Suite Prerequisites.xlsx
+++ b/Data/Test Suite Prerequisites.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\development\feature\1.3.1\1.3.1\gpconnect-provider-testing\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\development\feature\1.3.2\gpconnect-provider-testing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02370DBF-9776-4BBB-8053-119AEB77EA3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{498194E6-594C-4EC0-8746-1DB9D4834465}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-26925" yWindow="690" windowWidth="25455" windowHeight="13440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Patients" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="106">
   <si>
     <t>Required Organizations and Slots for testing</t>
   </si>
@@ -77,12 +77,6 @@
     <t>Past Medications</t>
   </si>
   <si>
-    <t>Active Problems</t>
-  </si>
-  <si>
-    <t>Inactive Problems</t>
-  </si>
-  <si>
     <t>Site Code</t>
   </si>
   <si>
@@ -90,9 +84,6 @@
   </si>
   <si>
     <t>unknownSIT</t>
-  </si>
-  <si>
-    <t>Referrals</t>
   </si>
   <si>
     <t>Other Requirements</t>
@@ -343,19 +334,26 @@
     <t>Problems</t>
   </si>
   <si>
-    <t>Patient Must Have :
-Consultation that is linked to only clinical items
-Consultation That is only Linked to A topic that is only linked to clinical items (no heading)
-Consultation that linked to a Topic that is linked to clinical items and also to a heading list that is linked to clinical items
-Consultation that is linked to a topic that is linked to a problem
-Encounter linked to a problem but not linked to a topic or heading</t>
-  </si>
-  <si>
     <t>Consultations/Encounters</t>
   </si>
   <si>
     <t>x
 Meds TimePeriod Test Requires data from 3 years back from current system date</t>
+  </si>
+  <si>
+    <t>Patient Must Have :
+- Consultation that is linked to only clinical items
+- Consultation That is only Linked to A topic that is only linked to clinical items (no heading)
+- Consultation that linked to a Topic that is linked to clinical items and also to a heading list that is linked to clinical items
+- Consultation that is linked to a topic that is linked to a problem
+- Consultation linked to a problem but not linked to a topic or heading
+- A problem linked to a medRequest/Medication/MedStatement, AllergyIntollerance, Immunization,  Observation and another problem.</t>
+  </si>
+  <si>
+    <t>No Problems assocaited with Patient</t>
+  </si>
+  <si>
+    <t>No Data for new structurea areas(Imms, uncat, problems and consultations)</t>
   </si>
 </sst>
 </file>
@@ -975,10 +973,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1001"/>
+  <dimension ref="A1:W1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -987,13 +985,13 @@
     <col min="2" max="2" width="22.5703125" customWidth="1"/>
     <col min="3" max="3" width="19.85546875" customWidth="1"/>
     <col min="4" max="4" width="54" customWidth="1"/>
-    <col min="5" max="11" width="19.85546875" customWidth="1"/>
-    <col min="12" max="15" width="19.85546875" style="31" customWidth="1"/>
-    <col min="16" max="16" width="62.7109375" customWidth="1"/>
-    <col min="17" max="26" width="11.5703125" customWidth="1"/>
+    <col min="5" max="8" width="19.85546875" customWidth="1"/>
+    <col min="9" max="12" width="19.85546875" style="31" customWidth="1"/>
+    <col min="13" max="13" width="62.7109375" customWidth="1"/>
+    <col min="14" max="23" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -1017,11 +1015,8 @@
       <c r="U1" s="2"/>
       <c r="V1" s="2"/>
       <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
-      <c r="Z1" s="2"/>
-    </row>
-    <row r="2" spans="1:26" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:23" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="40" t="s">
         <v>2</v>
       </c>
@@ -1031,14 +1026,14 @@
       <c r="F2" s="41"/>
       <c r="G2" s="41"/>
       <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="41"/>
-      <c r="K2" s="41"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
       <c r="L2" s="42"/>
-      <c r="M2" s="42"/>
-      <c r="N2" s="42"/>
-      <c r="O2" s="42"/>
-      <c r="P2" s="41"/>
+      <c r="M2" s="41"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
       <c r="Q2" s="6"/>
       <c r="R2" s="6"/>
       <c r="S2" s="6"/>
@@ -1046,11 +1041,8 @@
       <c r="U2" s="6"/>
       <c r="V2" s="6"/>
       <c r="W2" s="6"/>
-      <c r="X2" s="6"/>
-      <c r="Y2" s="6"/>
-      <c r="Z2" s="6"/>
-    </row>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="6"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -1062,9 +1054,9 @@
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
       <c r="P3" s="6"/>
       <c r="Q3" s="6"/>
       <c r="R3" s="6"/>
@@ -1073,11 +1065,8 @@
       <c r="U3" s="6"/>
       <c r="V3" s="6"/>
       <c r="W3" s="6"/>
-      <c r="X3" s="6"/>
-      <c r="Y3" s="6"/>
-      <c r="Z3" s="6"/>
-    </row>
-    <row r="4" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="B4" s="8"/>
       <c r="C4" s="10" t="s">
         <v>5</v>
@@ -1098,29 +1087,23 @@
         <v>15</v>
       </c>
       <c r="I4" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="J4" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="K4" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="L4" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="J4" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="K4" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="M4" s="22" t="s">
+      <c r="L4" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="N4" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="O4" s="22" t="s">
-        <v>105</v>
-      </c>
-      <c r="P4" s="16" t="s">
-        <v>22</v>
-      </c>
+      <c r="M4" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
       <c r="Q4" s="6"/>
       <c r="R4" s="6"/>
       <c r="S4" s="6"/>
@@ -1128,19 +1111,16 @@
       <c r="U4" s="6"/>
       <c r="V4" s="6"/>
       <c r="W4" s="6"/>
-      <c r="X4" s="6"/>
-      <c r="Y4" s="6"/>
-      <c r="Z4" s="6"/>
-    </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="15" t="s">
         <v>23</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>26</v>
       </c>
       <c r="E5" s="15">
         <v>0</v>
@@ -1154,20 +1134,14 @@
       <c r="H5" s="14">
         <v>0</v>
       </c>
-      <c r="I5" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="J5" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="K5" s="22">
-        <v>0</v>
-      </c>
-      <c r="L5" s="14"/>
-      <c r="M5" s="22"/>
-      <c r="N5" s="14"/>
-      <c r="O5" s="22"/>
-      <c r="P5" s="20"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="22"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="22"/>
+      <c r="M5" s="20"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6"/>
       <c r="Q5" s="6"/>
       <c r="R5" s="6"/>
       <c r="S5" s="6"/>
@@ -1175,56 +1149,47 @@
       <c r="U5" s="6"/>
       <c r="V5" s="6"/>
       <c r="W5" s="6"/>
-      <c r="X5" s="6"/>
-      <c r="Y5" s="6"/>
-      <c r="Z5" s="6"/>
-    </row>
-    <row r="6" spans="1:26" ht="120" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:23" ht="180" x14ac:dyDescent="0.25">
       <c r="B6" s="18" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="H6" s="14" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="J6" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="K6" s="22">
-        <v>0</v>
-      </c>
-      <c r="L6" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="M6" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="N6" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="O6" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="P6" s="20" t="s">
-        <v>104</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="J6" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="K6" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="L6" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="M6" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="6"/>
       <c r="Q6" s="6"/>
       <c r="R6" s="6"/>
       <c r="S6" s="6"/>
@@ -1232,22 +1197,19 @@
       <c r="U6" s="6"/>
       <c r="V6" s="6"/>
       <c r="W6" s="6"/>
-      <c r="X6" s="6"/>
-      <c r="Y6" s="6"/>
-      <c r="Z6" s="6"/>
-    </row>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="18" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F7" s="14">
         <v>0</v>
@@ -1256,22 +1218,18 @@
         <v>0</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="I7" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="J7" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="K7" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="L7" s="14"/>
-      <c r="M7" s="22"/>
-      <c r="N7" s="14"/>
-      <c r="O7" s="22"/>
-      <c r="P7" s="20"/>
+        <v>26</v>
+      </c>
+      <c r="I7" s="14"/>
+      <c r="J7" s="22"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="22"/>
+      <c r="M7" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6"/>
       <c r="Q7" s="6"/>
       <c r="R7" s="6"/>
       <c r="S7" s="6"/>
@@ -1279,22 +1237,19 @@
       <c r="U7" s="6"/>
       <c r="V7" s="6"/>
       <c r="W7" s="6"/>
-      <c r="X7" s="6"/>
-      <c r="Y7" s="6"/>
-      <c r="Z7" s="6"/>
-    </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="B8" s="18" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F8" s="14">
         <v>0</v>
@@ -1305,28 +1260,24 @@
       <c r="H8" s="14">
         <v>0</v>
       </c>
-      <c r="I8" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="J8" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="K8" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="L8" s="14">
+      <c r="I8" s="14">
         <v>0</v>
       </c>
-      <c r="M8" s="22">
+      <c r="J8" s="22">
         <v>0</v>
       </c>
-      <c r="N8" s="14">
+      <c r="K8" s="14">
         <v>0</v>
       </c>
-      <c r="O8" s="22">
+      <c r="L8" s="22">
         <v>0</v>
       </c>
-      <c r="P8" s="20"/>
+      <c r="M8" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
       <c r="Q8" s="6"/>
       <c r="R8" s="6"/>
       <c r="S8" s="6"/>
@@ -1334,46 +1285,37 @@
       <c r="U8" s="6"/>
       <c r="V8" s="6"/>
       <c r="W8" s="6"/>
-      <c r="X8" s="6"/>
-      <c r="Y8" s="6"/>
-      <c r="Z8" s="6"/>
-    </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="18" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E9" s="15">
         <v>0</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="H9" s="14">
         <v>0</v>
       </c>
-      <c r="I9" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="J9" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="K9" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="L9" s="14"/>
-      <c r="M9" s="22"/>
-      <c r="N9" s="14"/>
-      <c r="O9" s="22"/>
-      <c r="P9" s="20"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="22"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="22"/>
+      <c r="M9" s="20"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
       <c r="Q9" s="6"/>
       <c r="R9" s="6"/>
       <c r="S9" s="6"/>
@@ -1381,46 +1323,37 @@
       <c r="U9" s="6"/>
       <c r="V9" s="6"/>
       <c r="W9" s="6"/>
-      <c r="X9" s="6"/>
-      <c r="Y9" s="6"/>
-      <c r="Z9" s="6"/>
-    </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="18" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G10" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H10" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="I10" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="J10" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="K10" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="L10" s="14"/>
-      <c r="M10" s="22"/>
-      <c r="N10" s="14"/>
-      <c r="O10" s="22"/>
-      <c r="P10" s="20"/>
+        <v>22</v>
+      </c>
+      <c r="I10" s="14"/>
+      <c r="J10" s="22"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="22"/>
+      <c r="M10" s="20"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
       <c r="Q10" s="6"/>
       <c r="R10" s="6"/>
       <c r="S10" s="6"/>
@@ -1428,46 +1361,37 @@
       <c r="U10" s="6"/>
       <c r="V10" s="6"/>
       <c r="W10" s="6"/>
-      <c r="X10" s="6"/>
-      <c r="Y10" s="6"/>
-      <c r="Z10" s="6"/>
-    </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="18" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G11" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H11" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="I11" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="J11" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="K11" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="L11" s="14"/>
-      <c r="M11" s="22"/>
-      <c r="N11" s="14"/>
-      <c r="O11" s="22"/>
-      <c r="P11" s="20"/>
+        <v>22</v>
+      </c>
+      <c r="I11" s="14"/>
+      <c r="J11" s="22"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="22"/>
+      <c r="M11" s="20"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="6"/>
       <c r="Q11" s="6"/>
       <c r="R11" s="6"/>
       <c r="S11" s="6"/>
@@ -1475,46 +1399,37 @@
       <c r="U11" s="6"/>
       <c r="V11" s="6"/>
       <c r="W11" s="6"/>
-      <c r="X11" s="6"/>
-      <c r="Y11" s="6"/>
-      <c r="Z11" s="6"/>
-    </row>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="18" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G12" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H12" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="I12" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="J12" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="K12" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="L12" s="14"/>
-      <c r="M12" s="22"/>
-      <c r="N12" s="14"/>
-      <c r="O12" s="22"/>
-      <c r="P12" s="20"/>
+        <v>22</v>
+      </c>
+      <c r="I12" s="14"/>
+      <c r="J12" s="22"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="22"/>
+      <c r="M12" s="20"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="6"/>
       <c r="Q12" s="6"/>
       <c r="R12" s="6"/>
       <c r="S12" s="6"/>
@@ -1522,48 +1437,39 @@
       <c r="U12" s="6"/>
       <c r="V12" s="6"/>
       <c r="W12" s="6"/>
-      <c r="X12" s="6"/>
-      <c r="Y12" s="6"/>
-      <c r="Z12" s="6"/>
-    </row>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="26" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F13" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G13" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H13" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="I13" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="J13" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="K13" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="L13" s="14"/>
-      <c r="M13" s="22"/>
-      <c r="N13" s="14"/>
-      <c r="O13" s="22"/>
-      <c r="P13" s="16" t="s">
-        <v>47</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="I13" s="14"/>
+      <c r="J13" s="22"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="22"/>
+      <c r="M13" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+      <c r="P13" s="6"/>
       <c r="Q13" s="6"/>
       <c r="R13" s="6"/>
       <c r="S13" s="6"/>
@@ -1571,48 +1477,39 @@
       <c r="U13" s="6"/>
       <c r="V13" s="6"/>
       <c r="W13" s="6"/>
-      <c r="X13" s="6"/>
-      <c r="Y13" s="6"/>
-      <c r="Z13" s="6"/>
-    </row>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="26" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G14" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H14" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="I14" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="J14" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="K14" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="L14" s="14"/>
-      <c r="M14" s="22"/>
-      <c r="N14" s="14"/>
-      <c r="O14" s="22"/>
-      <c r="P14" s="16" t="s">
-        <v>47</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="I14" s="14"/>
+      <c r="J14" s="22"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="22"/>
+      <c r="M14" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="N14" s="6"/>
+      <c r="O14" s="6"/>
+      <c r="P14" s="6"/>
       <c r="Q14" s="6"/>
       <c r="R14" s="6"/>
       <c r="S14" s="6"/>
@@ -1620,48 +1517,39 @@
       <c r="U14" s="6"/>
       <c r="V14" s="6"/>
       <c r="W14" s="6"/>
-      <c r="X14" s="6"/>
-      <c r="Y14" s="6"/>
-      <c r="Z14" s="6"/>
-    </row>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="26" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G15" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H15" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="I15" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="J15" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="K15" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="L15" s="14"/>
-      <c r="M15" s="22"/>
-      <c r="N15" s="14"/>
-      <c r="O15" s="22"/>
-      <c r="P15" s="16" t="s">
-        <v>50</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="I15" s="14"/>
+      <c r="J15" s="22"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="22"/>
+      <c r="M15" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="N15" s="6"/>
+      <c r="O15" s="6"/>
+      <c r="P15" s="6"/>
       <c r="Q15" s="6"/>
       <c r="R15" s="6"/>
       <c r="S15" s="6"/>
@@ -1669,22 +1557,19 @@
       <c r="U15" s="6"/>
       <c r="V15" s="6"/>
       <c r="W15" s="6"/>
-      <c r="X15" s="6"/>
-      <c r="Y15" s="6"/>
-      <c r="Z15" s="6"/>
-    </row>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="26" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F16" s="14">
         <v>0</v>
@@ -1693,24 +1578,18 @@
         <v>0</v>
       </c>
       <c r="H16" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="I16" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="J16" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="K16" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="L16" s="14"/>
-      <c r="M16" s="22"/>
-      <c r="N16" s="14"/>
-      <c r="O16" s="22"/>
-      <c r="P16" s="16" t="s">
-        <v>52</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="I16" s="14"/>
+      <c r="J16" s="22"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="22"/>
+      <c r="M16" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="N16" s="6"/>
+      <c r="O16" s="6"/>
+      <c r="P16" s="6"/>
       <c r="Q16" s="6"/>
       <c r="R16" s="6"/>
       <c r="S16" s="6"/>
@@ -1718,48 +1597,39 @@
       <c r="U16" s="6"/>
       <c r="V16" s="6"/>
       <c r="W16" s="6"/>
-      <c r="X16" s="6"/>
-      <c r="Y16" s="6"/>
-      <c r="Z16" s="6"/>
-    </row>
-    <row r="17" spans="2:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="2:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G17" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="H17" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="I17" s="14"/>
+      <c r="J17" s="22"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="22"/>
+      <c r="M17" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="C17" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="D17" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="E17" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="F17" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="G17" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="H17" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="I17" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="J17" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="K17" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="L17" s="14"/>
-      <c r="M17" s="22"/>
-      <c r="N17" s="14"/>
-      <c r="O17" s="22"/>
-      <c r="P17" s="16" t="s">
-        <v>56</v>
-      </c>
+      <c r="N17" s="6"/>
+      <c r="O17" s="6"/>
+      <c r="P17" s="6"/>
       <c r="Q17" s="6"/>
       <c r="R17" s="6"/>
       <c r="S17" s="6"/>
@@ -1767,48 +1637,39 @@
       <c r="U17" s="6"/>
       <c r="V17" s="6"/>
       <c r="W17" s="6"/>
-      <c r="X17" s="6"/>
-      <c r="Y17" s="6"/>
-      <c r="Z17" s="6"/>
-    </row>
-    <row r="18" spans="2:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="2:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="26" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D18" s="22" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F18" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G18" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H18" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="I18" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="J18" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="K18" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="L18" s="14"/>
-      <c r="M18" s="22"/>
-      <c r="N18" s="14"/>
-      <c r="O18" s="22"/>
-      <c r="P18" s="16" t="s">
-        <v>62</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="I18" s="14"/>
+      <c r="J18" s="22"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="22"/>
+      <c r="M18" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="N18" s="6"/>
+      <c r="O18" s="6"/>
+      <c r="P18" s="6"/>
       <c r="Q18" s="6"/>
       <c r="R18" s="6"/>
       <c r="S18" s="6"/>
@@ -1816,48 +1677,39 @@
       <c r="U18" s="6"/>
       <c r="V18" s="6"/>
       <c r="W18" s="6"/>
-      <c r="X18" s="6"/>
-      <c r="Y18" s="6"/>
-      <c r="Z18" s="6"/>
-    </row>
-    <row r="19" spans="2:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="2:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="26" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E19" s="15" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F19" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G19" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H19" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="I19" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="J19" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="K19" s="22">
-        <v>0</v>
-      </c>
-      <c r="L19" s="14"/>
-      <c r="M19" s="22"/>
-      <c r="N19" s="14"/>
-      <c r="O19" s="22"/>
-      <c r="P19" s="16" t="s">
-        <v>65</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="I19" s="14"/>
+      <c r="J19" s="22"/>
+      <c r="K19" s="14"/>
+      <c r="L19" s="22"/>
+      <c r="M19" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="N19" s="6"/>
+      <c r="O19" s="6"/>
+      <c r="P19" s="6"/>
       <c r="Q19" s="6"/>
       <c r="R19" s="6"/>
       <c r="S19" s="6"/>
@@ -1865,48 +1717,39 @@
       <c r="U19" s="6"/>
       <c r="V19" s="6"/>
       <c r="W19" s="6"/>
-      <c r="X19" s="6"/>
-      <c r="Y19" s="6"/>
-      <c r="Z19" s="6"/>
-    </row>
-    <row r="20" spans="2:26" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="2:23" ht="45" x14ac:dyDescent="0.25">
       <c r="B20" s="26" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D20" s="29" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E20" s="29" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F20" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G20" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H20" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="I20" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="J20" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="K20" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="L20" s="14"/>
-      <c r="M20" s="22"/>
-      <c r="N20" s="14"/>
-      <c r="O20" s="22"/>
-      <c r="P20" s="39" t="s">
-        <v>102</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="I20" s="14"/>
+      <c r="J20" s="22"/>
+      <c r="K20" s="14"/>
+      <c r="L20" s="22"/>
+      <c r="M20" s="39" t="s">
+        <v>99</v>
+      </c>
+      <c r="N20" s="6"/>
+      <c r="O20" s="6"/>
+      <c r="P20" s="6"/>
       <c r="Q20" s="6"/>
       <c r="R20" s="6"/>
       <c r="S20" s="6"/>
@@ -1914,46 +1757,37 @@
       <c r="U20" s="6"/>
       <c r="V20" s="6"/>
       <c r="W20" s="6"/>
-      <c r="X20" s="6"/>
-      <c r="Y20" s="6"/>
-      <c r="Z20" s="6"/>
-    </row>
-    <row r="21" spans="2:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="2:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="26" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D21" s="22" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E21" s="29" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F21" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G21" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H21" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="I21" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="J21" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="K21" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="L21" s="14"/>
-      <c r="M21" s="22"/>
-      <c r="N21" s="14"/>
-      <c r="O21" s="22"/>
-      <c r="P21" s="20"/>
+        <v>22</v>
+      </c>
+      <c r="I21" s="14"/>
+      <c r="J21" s="22"/>
+      <c r="K21" s="14"/>
+      <c r="L21" s="22"/>
+      <c r="M21" s="20"/>
+      <c r="N21" s="6"/>
+      <c r="O21" s="6"/>
+      <c r="P21" s="6"/>
       <c r="Q21" s="6"/>
       <c r="R21" s="6"/>
       <c r="S21" s="6"/>
@@ -1961,48 +1795,39 @@
       <c r="U21" s="6"/>
       <c r="V21" s="6"/>
       <c r="W21" s="6"/>
-      <c r="X21" s="6"/>
-      <c r="Y21" s="6"/>
-      <c r="Z21" s="6"/>
-    </row>
-    <row r="22" spans="2:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="2:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="26" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D22" s="29" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E22" s="29" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F22" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G22" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H22" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="I22" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="J22" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="K22" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="L22" s="14"/>
-      <c r="M22" s="22"/>
-      <c r="N22" s="14"/>
-      <c r="O22" s="22"/>
-      <c r="P22" s="16" t="s">
-        <v>73</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="I22" s="14"/>
+      <c r="J22" s="22"/>
+      <c r="K22" s="14"/>
+      <c r="L22" s="22"/>
+      <c r="M22" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="N22" s="6"/>
+      <c r="O22" s="6"/>
+      <c r="P22" s="6"/>
       <c r="Q22" s="6"/>
       <c r="R22" s="6"/>
       <c r="S22" s="6"/>
@@ -2010,46 +1835,37 @@
       <c r="U22" s="6"/>
       <c r="V22" s="6"/>
       <c r="W22" s="6"/>
-      <c r="X22" s="6"/>
-      <c r="Y22" s="6"/>
-      <c r="Z22" s="6"/>
-    </row>
-    <row r="23" spans="2:26" s="31" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="2:23" s="31" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="26" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D23" s="29" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E23" s="29" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F23" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G23" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H23" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="I23" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="J23" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="K23" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="L23" s="14"/>
-      <c r="M23" s="22"/>
-      <c r="N23" s="14"/>
-      <c r="O23" s="22"/>
-      <c r="P23" s="16"/>
+        <v>22</v>
+      </c>
+      <c r="I23" s="14"/>
+      <c r="J23" s="22"/>
+      <c r="K23" s="14"/>
+      <c r="L23" s="22"/>
+      <c r="M23" s="16"/>
+      <c r="N23" s="6"/>
+      <c r="O23" s="6"/>
+      <c r="P23" s="6"/>
       <c r="Q23" s="6"/>
       <c r="R23" s="6"/>
       <c r="S23" s="6"/>
@@ -2057,48 +1873,39 @@
       <c r="U23" s="6"/>
       <c r="V23" s="6"/>
       <c r="W23" s="6"/>
-      <c r="X23" s="6"/>
-      <c r="Y23" s="6"/>
-      <c r="Z23" s="6"/>
-    </row>
-    <row r="24" spans="2:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="2:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="26" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D24" s="29" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E24" s="29" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F24" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G24" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H24" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="I24" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="J24" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="K24" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="L24" s="14"/>
-      <c r="M24" s="22"/>
-      <c r="N24" s="14"/>
-      <c r="O24" s="22"/>
-      <c r="P24" s="16" t="s">
-        <v>76</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="I24" s="14"/>
+      <c r="J24" s="22"/>
+      <c r="K24" s="14"/>
+      <c r="L24" s="22"/>
+      <c r="M24" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="N24" s="6"/>
+      <c r="O24" s="6"/>
+      <c r="P24" s="6"/>
       <c r="Q24" s="6"/>
       <c r="R24" s="6"/>
       <c r="S24" s="6"/>
@@ -2106,48 +1913,39 @@
       <c r="U24" s="6"/>
       <c r="V24" s="6"/>
       <c r="W24" s="6"/>
-      <c r="X24" s="6"/>
-      <c r="Y24" s="6"/>
-      <c r="Z24" s="6"/>
-    </row>
-    <row r="25" spans="2:26" s="31" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="2:23" s="31" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="26" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D25" s="29" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E25" s="29" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F25" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G25" s="14" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H25" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="I25" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="J25" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="K25" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="L25" s="14"/>
-      <c r="M25" s="22"/>
-      <c r="N25" s="14"/>
-      <c r="O25" s="22"/>
-      <c r="P25" s="16" t="s">
-        <v>98</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="I25" s="14"/>
+      <c r="J25" s="22"/>
+      <c r="K25" s="14"/>
+      <c r="L25" s="22"/>
+      <c r="M25" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="N25" s="6"/>
+      <c r="O25" s="6"/>
+      <c r="P25" s="6"/>
       <c r="Q25" s="6"/>
       <c r="R25" s="6"/>
       <c r="S25" s="6"/>
@@ -2155,17 +1953,14 @@
       <c r="U25" s="6"/>
       <c r="V25" s="6"/>
       <c r="W25" s="6"/>
-      <c r="X25" s="6"/>
-      <c r="Y25" s="6"/>
-      <c r="Z25" s="6"/>
-    </row>
-    <row r="26" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    </row>
+    <row r="26" spans="2:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="2:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="2:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="2:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="2:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="2:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="2:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3137,7 +2932,7 @@
     <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B2:P2"/>
+    <mergeCell ref="B2:M2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3260,7 +3055,7 @@
         <v>4</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
@@ -3269,10 +3064,10 @@
     </row>
     <row r="15" spans="2:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
@@ -4371,31 +4166,31 @@
       <c r="A4" s="1"/>
       <c r="B4" s="17"/>
       <c r="C4" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="21" t="s">
-        <v>27</v>
-      </c>
       <c r="E4" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="F4" s="21" t="s">
+      <c r="I4" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="G4" s="21" t="s">
+      <c r="J4" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="H4" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="I4" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="J4" s="19" t="s">
-        <v>36</v>
-      </c>
       <c r="K4" s="23" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
@@ -4411,31 +4206,31 @@
     <row r="5" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="24" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D5" s="27" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E5" s="27" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F5" s="27" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G5" s="27" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H5" s="25" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="I5" s="27" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="J5" s="25" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="K5" s="28"/>
       <c r="L5" s="1"/>
@@ -4452,31 +4247,31 @@
     <row r="6" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="24" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D6" s="27" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E6" s="27" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F6" s="27" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G6" s="27" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H6" s="25" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="I6" s="27" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="J6" s="25" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="K6" s="28"/>
       <c r="L6" s="1"/>
@@ -4493,31 +4288,31 @@
     <row r="7" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="24" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E7" s="27" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F7" s="27" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G7" s="27" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H7" s="25" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="I7" s="27" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="J7" s="25" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="K7" s="28"/>
       <c r="L7" s="1"/>
@@ -4534,31 +4329,31 @@
     <row r="8" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="24" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D8" s="27" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E8" s="27" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F8" s="27" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G8" s="27" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H8" s="25" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="I8" s="27" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="J8" s="25" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="K8" s="28"/>
       <c r="L8" s="1"/>
@@ -4575,31 +4370,31 @@
     <row r="9" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="24" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D9" s="27" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E9" s="27" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F9" s="27" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G9" s="27" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H9" s="25" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="I9" s="27" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="J9" s="25" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="K9" s="28"/>
       <c r="L9" s="1"/>
@@ -4616,31 +4411,31 @@
     <row r="10" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="24" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D10" s="27" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E10" s="27" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F10" s="27" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G10" s="27" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H10" s="25" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="I10" s="27" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="J10" s="25" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="K10" s="28"/>
       <c r="L10" s="1"/>
@@ -4657,31 +4452,31 @@
     <row r="11" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="24" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D11" s="27" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E11" s="27" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F11" s="27" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G11" s="27" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H11" s="25" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="I11" s="27" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="J11" s="25" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="K11" s="28"/>
       <c r="L11" s="1"/>
@@ -4698,31 +4493,31 @@
     <row r="12" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="24" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D12" s="27" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E12" s="27" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F12" s="27" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G12" s="27" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H12" s="25" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="I12" s="27" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="J12" s="25" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="K12" s="28"/>
       <c r="L12" s="1"/>
@@ -4739,31 +4534,31 @@
     <row r="13" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="30" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D13" s="27" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E13" s="27" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F13" s="27" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G13" s="27" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H13" s="25" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="I13" s="27" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="J13" s="25" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="K13" s="23"/>
       <c r="L13" s="1"/>
@@ -4780,31 +4575,31 @@
     <row r="14" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="30" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D14" s="27" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E14" s="27" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F14" s="27" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G14" s="27" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H14" s="25" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="I14" s="27" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="J14" s="25" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="K14" s="23"/>
       <c r="L14" s="1"/>
@@ -4821,31 +4616,31 @@
     <row r="15" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="30" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D15" s="27" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E15" s="27" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F15" s="27" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G15" s="27" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H15" s="25" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="I15" s="27" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="J15" s="25" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="K15" s="23"/>
       <c r="L15" s="1"/>
@@ -6020,7 +5815,7 @@
     <row r="2" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="31"/>
       <c r="B2" s="5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
@@ -6037,7 +5832,7 @@
     <row r="3" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="31"/>
       <c r="B3" s="33" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C3" s="33"/>
       <c r="D3" s="33"/>
@@ -6069,10 +5864,10 @@
     <row r="5" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="31"/>
       <c r="B5" s="9" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D5" s="31"/>
       <c r="E5" s="31"/>
@@ -6088,7 +5883,7 @@
     <row r="6" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="31"/>
       <c r="B6" s="7" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C6" s="34">
         <v>0</v>
@@ -6107,7 +5902,7 @@
     <row r="7" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="31"/>
       <c r="B7" s="7" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C7" s="34">
         <v>1</v>
@@ -6126,7 +5921,7 @@
     <row r="8" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="31"/>
       <c r="B8" s="7" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C8" s="34">
         <v>2</v>
@@ -6145,7 +5940,7 @@
     <row r="9" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="31"/>
       <c r="B9" s="7" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C9" s="34">
         <v>1</v>
@@ -6179,7 +5974,7 @@
     <row r="11" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="31"/>
       <c r="B11" s="9" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C11" s="33"/>
       <c r="D11" s="31"/>
@@ -6196,7 +5991,7 @@
     <row r="12" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="31"/>
       <c r="B12" s="7" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="31"/>
@@ -7372,7 +7167,7 @@
     <row r="2" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11"/>
       <c r="B2" s="44" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C2" s="41"/>
       <c r="D2" s="41"/>
@@ -7413,16 +7208,16 @@
         <v>4</v>
       </c>
       <c r="C4" s="35" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D4" s="35" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E4" s="35" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="F4" s="35" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="G4" s="11"/>
       <c r="H4" s="11"/>
@@ -7447,7 +7242,7 @@
         <v>0.44097222222222199</v>
       </c>
       <c r="E5" s="37" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F5" s="37"/>
       <c r="G5" s="11"/>
@@ -7473,7 +7268,7 @@
         <v>0.52777777777777801</v>
       </c>
       <c r="E6" s="37" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F6" s="37"/>
       <c r="G6" s="11"/>
@@ -7499,10 +7294,10 @@
         <v>0.52777777777777801</v>
       </c>
       <c r="E7" s="37" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="F7" s="37" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
@@ -7554,7 +7349,7 @@
     <row r="10" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11"/>
       <c r="B10" s="38" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C10" s="34"/>
       <c r="D10" s="34"/>
@@ -7592,7 +7387,7 @@
     <row r="12" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11"/>
       <c r="B12" s="34" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C12" s="34"/>
       <c r="D12" s="34"/>
@@ -7633,7 +7428,7 @@
         <v>4</v>
       </c>
       <c r="C14" s="35" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D14" s="34"/>
       <c r="E14" s="34"/>

</xml_diff>

<commit_message>
Main Problems test now updated to check 1.3.2 new list and linkages requirements
</commit_message>
<xml_diff>
--- a/Data/Test Suite Prerequisites.xlsx
+++ b/Data/Test Suite Prerequisites.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\development\feature\1.3.2\gpconnect-provider-testing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{498194E6-594C-4EC0-8746-1DB9D4834465}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6CF8E0B-2B47-4366-8156-F073CCD9BD55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26925" yWindow="690" windowWidth="25455" windowHeight="13440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Patients" sheetId="1" r:id="rId1"/>
@@ -341,19 +341,19 @@
 Meds TimePeriod Test Requires data from 3 years back from current system date</t>
   </si>
   <si>
+    <t>No Problems assocaited with Patient</t>
+  </si>
+  <si>
+    <t>No Data for new structurea areas(Imms, uncat, problems and consultations)</t>
+  </si>
+  <si>
     <t>Patient Must Have :
 - Consultation that is linked to only clinical items
 - Consultation That is only Linked to A topic that is only linked to clinical items (no heading)
 - Consultation that linked to a Topic that is linked to clinical items and also to a heading list that is linked to clinical items
 - Consultation that is linked to a topic that is linked to a problem
 - Consultation linked to a problem but not linked to a topic or heading
-- A problem linked to a medRequest/Medication/MedStatement, AllergyIntollerance, Immunization,  Observation and another problem.</t>
-  </si>
-  <si>
-    <t>No Problems assocaited with Patient</t>
-  </si>
-  <si>
-    <t>No Data for new structurea areas(Imms, uncat, problems and consultations)</t>
+- A problem linked to a medRequest/Medication/MedStatement, AllergyIntollerance, Immunization &amp;  Observation</t>
   </si>
 </sst>
 </file>
@@ -976,7 +976,7 @@
   <dimension ref="A1:W1001"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1150,7 +1150,7 @@
       <c r="V5" s="6"/>
       <c r="W5" s="6"/>
     </row>
-    <row r="6" spans="1:23" ht="180" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" ht="165" x14ac:dyDescent="0.25">
       <c r="B6" s="18" t="s">
         <v>25</v>
       </c>
@@ -1185,7 +1185,7 @@
         <v>26</v>
       </c>
       <c r="M6" s="20" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="N6" s="6"/>
       <c r="O6" s="6"/>
@@ -1225,7 +1225,7 @@
       <c r="K7" s="14"/>
       <c r="L7" s="22"/>
       <c r="M7" s="20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="N7" s="6"/>
       <c r="O7" s="6"/>
@@ -1273,7 +1273,7 @@
         <v>0</v>
       </c>
       <c r="M8" s="20" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="N8" s="6"/>
       <c r="O8" s="6"/>

</xml_diff>

<commit_message>
Updated main consultations test for 1.3.2 to check for new lists and clincal items. updated data requirements
</commit_message>
<xml_diff>
--- a/Data/Test Suite Prerequisites.xlsx
+++ b/Data/Test Suite Prerequisites.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\development\feature\1.3.2\gpconnect-provider-testing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6CF8E0B-2B47-4366-8156-F073CCD9BD55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A236474D-07EE-4CD7-836A-74CDCF2D91DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Patients" sheetId="1" r:id="rId1"/>
@@ -350,7 +350,7 @@
     <t>Patient Must Have :
 - Consultation that is linked to only clinical items
 - Consultation That is only Linked to A topic that is only linked to clinical items (no heading)
-- Consultation that linked to a Topic that is linked to clinical items and also to a heading list that is linked to clinical items
+- Consultation that is linked to a Topic or Heading  that is linked to all supported Clinical items 
 - Consultation that is linked to a topic that is linked to a problem
 - Consultation linked to a problem but not linked to a topic or heading
 - A problem linked to a medRequest/Medication/MedStatement, AllergyIntollerance, Immunization &amp;  Observation</t>
@@ -976,7 +976,7 @@
   <dimension ref="A1:W1001"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
updated data requirements and split main uncat test
</commit_message>
<xml_diff>
--- a/Data/Test Suite Prerequisites.xlsx
+++ b/Data/Test Suite Prerequisites.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\development\feature\1.3.2\gpconnect-provider-testing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A236474D-07EE-4CD7-836A-74CDCF2D91DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8A3FD80-C5C9-47EE-BC2D-18F3A2DED8FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Patients" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="106">
   <si>
     <t>Required Organizations and Slots for testing</t>
   </si>
@@ -339,9 +339,6 @@
   <si>
     <t>x
 Meds TimePeriod Test Requires data from 3 years back from current system date</t>
-  </si>
-  <si>
-    <t>No Problems assocaited with Patient</t>
   </si>
   <si>
     <t>No Data for new structurea areas(Imms, uncat, problems and consultations)</t>
@@ -354,6 +351,15 @@
 - Consultation that is linked to a topic that is linked to a problem
 - Consultation linked to a problem but not linked to a topic or heading
 - A problem linked to a medRequest/Medication/MedStatement, AllergyIntollerance, Immunization &amp;  Observation</t>
+  </si>
+  <si>
+    <t>Patient Must Have :
+No Problems associated with Patient/Clinical Items but has data for new structured areas
+- Consultation that is linked to only clinical items
+- Consultation That is only Linked to A topic that is only linked to clinical items (no heading)
+- Consultation that is linked to a Topic or Heading  that is linked to all supported Clinical items 
+- Consultation that is linked to a topic that is linked to a problem
+- Consultation linked to a problem but not linked to a topic or heading</t>
   </si>
 </sst>
 </file>
@@ -975,8 +981,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView tabSelected="1" topLeftCell="E3" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1185,7 +1191,7 @@
         <v>26</v>
       </c>
       <c r="M6" s="20" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="N6" s="6"/>
       <c r="O6" s="6"/>
@@ -1198,7 +1204,7 @@
       <c r="V6" s="6"/>
       <c r="W6" s="6"/>
     </row>
-    <row r="7" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" ht="165" x14ac:dyDescent="0.25">
       <c r="B7" s="18" t="s">
         <v>34</v>
       </c>
@@ -1220,12 +1226,20 @@
       <c r="H7" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="I7" s="14"/>
-      <c r="J7" s="22"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="22"/>
+      <c r="I7" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="J7" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="K7" s="14">
+        <v>0</v>
+      </c>
+      <c r="L7" s="22" t="s">
+        <v>26</v>
+      </c>
       <c r="M7" s="20" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="N7" s="6"/>
       <c r="O7" s="6"/>
@@ -1273,7 +1287,7 @@
         <v>0</v>
       </c>
       <c r="M8" s="20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="N8" s="6"/>
       <c r="O8" s="6"/>

</xml_diff>

<commit_message>
Big update for investigations and referrals
</commit_message>
<xml_diff>
--- a/Data/Test Suite Prerequisites.xlsx
+++ b/Data/Test Suite Prerequisites.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\development\feature\1.3.2\gpconnect-provider-testing\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\development\feature\1.5.0\gpconnect-provider-testing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8A3FD80-C5C9-47EE-BC2D-18F3A2DED8FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF3F6879-B37A-4913-B05E-0355A83B80D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Patients" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="112">
   <si>
     <t>Required Organizations and Slots for testing</t>
   </si>
@@ -360,6 +360,28 @@
 - Consultation that is linked to a Topic or Heading  that is linked to all supported Clinical items 
 - Consultation that is linked to a topic that is linked to a problem
 - Consultation linked to a problem but not linked to a topic or heading</t>
+  </si>
+  <si>
+    <t>Investigations</t>
+  </si>
+  <si>
+    <t>Referrals</t>
+  </si>
+  <si>
+    <t>x
+Patient Linked to DiagnosticReport, ProcedureRequests and specimens and a NO problems linked</t>
+  </si>
+  <si>
+    <t>x
+Patient Linked to ReferralRequests and  linked to a problem</t>
+  </si>
+  <si>
+    <t>x
+Patient Linked to ReferralRequests and  NOT linked to a problem</t>
+  </si>
+  <si>
+    <t>x
+Patient Linked to DiagnosticReport, ProcedureRequests,  specimens and a problem linked</t>
   </si>
 </sst>
 </file>
@@ -979,10 +1001,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W1001"/>
+  <dimension ref="A1:Y1001"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E3" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -992,12 +1014,12 @@
     <col min="3" max="3" width="19.85546875" customWidth="1"/>
     <col min="4" max="4" width="54" customWidth="1"/>
     <col min="5" max="8" width="19.85546875" customWidth="1"/>
-    <col min="9" max="12" width="19.85546875" style="31" customWidth="1"/>
-    <col min="13" max="13" width="62.7109375" customWidth="1"/>
-    <col min="14" max="23" width="11.5703125" customWidth="1"/>
+    <col min="9" max="14" width="19.85546875" style="31" customWidth="1"/>
+    <col min="15" max="15" width="62.7109375" customWidth="1"/>
+    <col min="16" max="25" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -1021,8 +1043,10 @@
       <c r="U1" s="2"/>
       <c r="V1" s="2"/>
       <c r="W1" s="2"/>
-    </row>
-    <row r="2" spans="1:23" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+    </row>
+    <row r="2" spans="1:25" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="40" t="s">
         <v>2</v>
       </c>
@@ -1036,9 +1060,9 @@
       <c r="J2" s="42"/>
       <c r="K2" s="42"/>
       <c r="L2" s="42"/>
-      <c r="M2" s="41"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6"/>
+      <c r="M2" s="42"/>
+      <c r="N2" s="42"/>
+      <c r="O2" s="41"/>
       <c r="P2" s="6"/>
       <c r="Q2" s="6"/>
       <c r="R2" s="6"/>
@@ -1047,8 +1071,10 @@
       <c r="U2" s="6"/>
       <c r="V2" s="6"/>
       <c r="W2" s="6"/>
-    </row>
-    <row r="3" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X2" s="6"/>
+      <c r="Y2" s="6"/>
+    </row>
+    <row r="3" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="6"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -1060,8 +1086,8 @@
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
       <c r="O3" s="6"/>
       <c r="P3" s="6"/>
       <c r="Q3" s="6"/>
@@ -1071,8 +1097,10 @@
       <c r="U3" s="6"/>
       <c r="V3" s="6"/>
       <c r="W3" s="6"/>
-    </row>
-    <row r="4" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+      <c r="X3" s="6"/>
+      <c r="Y3" s="6"/>
+    </row>
+    <row r="4" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="B4" s="8"/>
       <c r="C4" s="10" t="s">
         <v>5</v>
@@ -1104,11 +1132,15 @@
       <c r="L4" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="M4" s="16" t="s">
+      <c r="M4" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="N4" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="O4" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="N4" s="6"/>
-      <c r="O4" s="6"/>
       <c r="P4" s="6"/>
       <c r="Q4" s="6"/>
       <c r="R4" s="6"/>
@@ -1117,8 +1149,10 @@
       <c r="U4" s="6"/>
       <c r="V4" s="6"/>
       <c r="W4" s="6"/>
-    </row>
-    <row r="5" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X4" s="6"/>
+      <c r="Y4" s="6"/>
+    </row>
+    <row r="5" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="18" t="s">
         <v>20</v>
       </c>
@@ -1144,9 +1178,9 @@
       <c r="J5" s="22"/>
       <c r="K5" s="14"/>
       <c r="L5" s="22"/>
-      <c r="M5" s="20"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="6"/>
+      <c r="M5" s="22"/>
+      <c r="N5" s="22"/>
+      <c r="O5" s="20"/>
       <c r="P5" s="6"/>
       <c r="Q5" s="6"/>
       <c r="R5" s="6"/>
@@ -1155,8 +1189,10 @@
       <c r="U5" s="6"/>
       <c r="V5" s="6"/>
       <c r="W5" s="6"/>
-    </row>
-    <row r="6" spans="1:23" ht="165" x14ac:dyDescent="0.25">
+      <c r="X5" s="6"/>
+      <c r="Y5" s="6"/>
+    </row>
+    <row r="6" spans="1:25" ht="165" x14ac:dyDescent="0.25">
       <c r="B6" s="18" t="s">
         <v>25</v>
       </c>
@@ -1190,11 +1226,15 @@
       <c r="L6" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="M6" s="20" t="s">
+      <c r="M6" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="N6" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="O6" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="N6" s="6"/>
-      <c r="O6" s="6"/>
       <c r="P6" s="6"/>
       <c r="Q6" s="6"/>
       <c r="R6" s="6"/>
@@ -1203,8 +1243,10 @@
       <c r="U6" s="6"/>
       <c r="V6" s="6"/>
       <c r="W6" s="6"/>
-    </row>
-    <row r="7" spans="1:23" ht="165" x14ac:dyDescent="0.25">
+      <c r="X6" s="6"/>
+      <c r="Y6" s="6"/>
+    </row>
+    <row r="7" spans="1:25" ht="165" x14ac:dyDescent="0.25">
       <c r="B7" s="18" t="s">
         <v>34</v>
       </c>
@@ -1238,11 +1280,15 @@
       <c r="L7" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="M7" s="20" t="s">
+      <c r="M7" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="N7" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="O7" s="20" t="s">
         <v>105</v>
       </c>
-      <c r="N7" s="6"/>
-      <c r="O7" s="6"/>
       <c r="P7" s="6"/>
       <c r="Q7" s="6"/>
       <c r="R7" s="6"/>
@@ -1251,8 +1297,10 @@
       <c r="U7" s="6"/>
       <c r="V7" s="6"/>
       <c r="W7" s="6"/>
-    </row>
-    <row r="8" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+      <c r="X7" s="6"/>
+      <c r="Y7" s="6"/>
+    </row>
+    <row r="8" spans="1:25" ht="30" x14ac:dyDescent="0.25">
       <c r="B8" s="18" t="s">
         <v>35</v>
       </c>
@@ -1286,11 +1334,15 @@
       <c r="L8" s="22">
         <v>0</v>
       </c>
-      <c r="M8" s="20" t="s">
+      <c r="M8" s="22">
+        <v>0</v>
+      </c>
+      <c r="N8" s="22">
+        <v>0</v>
+      </c>
+      <c r="O8" s="20" t="s">
         <v>103</v>
       </c>
-      <c r="N8" s="6"/>
-      <c r="O8" s="6"/>
       <c r="P8" s="6"/>
       <c r="Q8" s="6"/>
       <c r="R8" s="6"/>
@@ -1299,8 +1351,10 @@
       <c r="U8" s="6"/>
       <c r="V8" s="6"/>
       <c r="W8" s="6"/>
-    </row>
-    <row r="9" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X8" s="6"/>
+      <c r="Y8" s="6"/>
+    </row>
+    <row r="9" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="18" t="s">
         <v>37</v>
       </c>
@@ -1326,9 +1380,9 @@
       <c r="J9" s="22"/>
       <c r="K9" s="14"/>
       <c r="L9" s="22"/>
-      <c r="M9" s="20"/>
-      <c r="N9" s="6"/>
-      <c r="O9" s="6"/>
+      <c r="M9" s="22"/>
+      <c r="N9" s="22"/>
+      <c r="O9" s="20"/>
       <c r="P9" s="6"/>
       <c r="Q9" s="6"/>
       <c r="R9" s="6"/>
@@ -1337,8 +1391,10 @@
       <c r="U9" s="6"/>
       <c r="V9" s="6"/>
       <c r="W9" s="6"/>
-    </row>
-    <row r="10" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X9" s="6"/>
+      <c r="Y9" s="6"/>
+    </row>
+    <row r="10" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="18" t="s">
         <v>39</v>
       </c>
@@ -1364,9 +1420,9 @@
       <c r="J10" s="22"/>
       <c r="K10" s="14"/>
       <c r="L10" s="22"/>
-      <c r="M10" s="20"/>
-      <c r="N10" s="6"/>
-      <c r="O10" s="6"/>
+      <c r="M10" s="22"/>
+      <c r="N10" s="22"/>
+      <c r="O10" s="20"/>
       <c r="P10" s="6"/>
       <c r="Q10" s="6"/>
       <c r="R10" s="6"/>
@@ -1375,8 +1431,10 @@
       <c r="U10" s="6"/>
       <c r="V10" s="6"/>
       <c r="W10" s="6"/>
-    </row>
-    <row r="11" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X10" s="6"/>
+      <c r="Y10" s="6"/>
+    </row>
+    <row r="11" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="18" t="s">
         <v>40</v>
       </c>
@@ -1402,9 +1460,9 @@
       <c r="J11" s="22"/>
       <c r="K11" s="14"/>
       <c r="L11" s="22"/>
-      <c r="M11" s="20"/>
-      <c r="N11" s="6"/>
-      <c r="O11" s="6"/>
+      <c r="M11" s="22"/>
+      <c r="N11" s="22"/>
+      <c r="O11" s="20"/>
       <c r="P11" s="6"/>
       <c r="Q11" s="6"/>
       <c r="R11" s="6"/>
@@ -1413,8 +1471,10 @@
       <c r="U11" s="6"/>
       <c r="V11" s="6"/>
       <c r="W11" s="6"/>
-    </row>
-    <row r="12" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X11" s="6"/>
+      <c r="Y11" s="6"/>
+    </row>
+    <row r="12" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="18" t="s">
         <v>41</v>
       </c>
@@ -1440,9 +1500,9 @@
       <c r="J12" s="22"/>
       <c r="K12" s="14"/>
       <c r="L12" s="22"/>
-      <c r="M12" s="20"/>
-      <c r="N12" s="6"/>
-      <c r="O12" s="6"/>
+      <c r="M12" s="22"/>
+      <c r="N12" s="22"/>
+      <c r="O12" s="20"/>
       <c r="P12" s="6"/>
       <c r="Q12" s="6"/>
       <c r="R12" s="6"/>
@@ -1451,8 +1511,10 @@
       <c r="U12" s="6"/>
       <c r="V12" s="6"/>
       <c r="W12" s="6"/>
-    </row>
-    <row r="13" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X12" s="6"/>
+      <c r="Y12" s="6"/>
+    </row>
+    <row r="13" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="26" t="s">
         <v>43</v>
       </c>
@@ -1478,11 +1540,11 @@
       <c r="J13" s="22"/>
       <c r="K13" s="14"/>
       <c r="L13" s="22"/>
-      <c r="M13" s="16" t="s">
+      <c r="M13" s="22"/>
+      <c r="N13" s="22"/>
+      <c r="O13" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="N13" s="6"/>
-      <c r="O13" s="6"/>
       <c r="P13" s="6"/>
       <c r="Q13" s="6"/>
       <c r="R13" s="6"/>
@@ -1491,8 +1553,10 @@
       <c r="U13" s="6"/>
       <c r="V13" s="6"/>
       <c r="W13" s="6"/>
-    </row>
-    <row r="14" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X13" s="6"/>
+      <c r="Y13" s="6"/>
+    </row>
+    <row r="14" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="26" t="s">
         <v>45</v>
       </c>
@@ -1518,11 +1582,11 @@
       <c r="J14" s="22"/>
       <c r="K14" s="14"/>
       <c r="L14" s="22"/>
-      <c r="M14" s="16" t="s">
+      <c r="M14" s="22"/>
+      <c r="N14" s="22"/>
+      <c r="O14" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="N14" s="6"/>
-      <c r="O14" s="6"/>
       <c r="P14" s="6"/>
       <c r="Q14" s="6"/>
       <c r="R14" s="6"/>
@@ -1531,8 +1595,10 @@
       <c r="U14" s="6"/>
       <c r="V14" s="6"/>
       <c r="W14" s="6"/>
-    </row>
-    <row r="15" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X14" s="6"/>
+      <c r="Y14" s="6"/>
+    </row>
+    <row r="15" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="26" t="s">
         <v>46</v>
       </c>
@@ -1558,11 +1624,11 @@
       <c r="J15" s="22"/>
       <c r="K15" s="14"/>
       <c r="L15" s="22"/>
-      <c r="M15" s="16" t="s">
+      <c r="M15" s="22"/>
+      <c r="N15" s="22"/>
+      <c r="O15" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="N15" s="6"/>
-      <c r="O15" s="6"/>
       <c r="P15" s="6"/>
       <c r="Q15" s="6"/>
       <c r="R15" s="6"/>
@@ -1571,8 +1637,10 @@
       <c r="U15" s="6"/>
       <c r="V15" s="6"/>
       <c r="W15" s="6"/>
-    </row>
-    <row r="16" spans="1:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X15" s="6"/>
+      <c r="Y15" s="6"/>
+    </row>
+    <row r="16" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="26" t="s">
         <v>48</v>
       </c>
@@ -1598,11 +1666,11 @@
       <c r="J16" s="22"/>
       <c r="K16" s="14"/>
       <c r="L16" s="22"/>
-      <c r="M16" s="16" t="s">
+      <c r="M16" s="22"/>
+      <c r="N16" s="22"/>
+      <c r="O16" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="N16" s="6"/>
-      <c r="O16" s="6"/>
       <c r="P16" s="6"/>
       <c r="Q16" s="6"/>
       <c r="R16" s="6"/>
@@ -1611,8 +1679,10 @@
       <c r="U16" s="6"/>
       <c r="V16" s="6"/>
       <c r="W16" s="6"/>
-    </row>
-    <row r="17" spans="2:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X16" s="6"/>
+      <c r="Y16" s="6"/>
+    </row>
+    <row r="17" spans="2:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="26" t="s">
         <v>50</v>
       </c>
@@ -1638,11 +1708,11 @@
       <c r="J17" s="22"/>
       <c r="K17" s="14"/>
       <c r="L17" s="22"/>
-      <c r="M17" s="16" t="s">
+      <c r="M17" s="22"/>
+      <c r="N17" s="22"/>
+      <c r="O17" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="N17" s="6"/>
-      <c r="O17" s="6"/>
       <c r="P17" s="6"/>
       <c r="Q17" s="6"/>
       <c r="R17" s="6"/>
@@ -1651,8 +1721,10 @@
       <c r="U17" s="6"/>
       <c r="V17" s="6"/>
       <c r="W17" s="6"/>
-    </row>
-    <row r="18" spans="2:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X17" s="6"/>
+      <c r="Y17" s="6"/>
+    </row>
+    <row r="18" spans="2:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="26" t="s">
         <v>55</v>
       </c>
@@ -1678,11 +1750,11 @@
       <c r="J18" s="22"/>
       <c r="K18" s="14"/>
       <c r="L18" s="22"/>
-      <c r="M18" s="16" t="s">
+      <c r="M18" s="22"/>
+      <c r="N18" s="22"/>
+      <c r="O18" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="N18" s="6"/>
-      <c r="O18" s="6"/>
       <c r="P18" s="6"/>
       <c r="Q18" s="6"/>
       <c r="R18" s="6"/>
@@ -1691,8 +1763,10 @@
       <c r="U18" s="6"/>
       <c r="V18" s="6"/>
       <c r="W18" s="6"/>
-    </row>
-    <row r="19" spans="2:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X18" s="6"/>
+      <c r="Y18" s="6"/>
+    </row>
+    <row r="19" spans="2:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="26" t="s">
         <v>60</v>
       </c>
@@ -1718,11 +1792,11 @@
       <c r="J19" s="22"/>
       <c r="K19" s="14"/>
       <c r="L19" s="22"/>
-      <c r="M19" s="16" t="s">
+      <c r="M19" s="22"/>
+      <c r="N19" s="22"/>
+      <c r="O19" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="N19" s="6"/>
-      <c r="O19" s="6"/>
       <c r="P19" s="6"/>
       <c r="Q19" s="6"/>
       <c r="R19" s="6"/>
@@ -1731,8 +1805,10 @@
       <c r="U19" s="6"/>
       <c r="V19" s="6"/>
       <c r="W19" s="6"/>
-    </row>
-    <row r="20" spans="2:23" ht="45" x14ac:dyDescent="0.25">
+      <c r="X19" s="6"/>
+      <c r="Y19" s="6"/>
+    </row>
+    <row r="20" spans="2:25" ht="45" x14ac:dyDescent="0.25">
       <c r="B20" s="26" t="s">
         <v>64</v>
       </c>
@@ -1758,11 +1834,11 @@
       <c r="J20" s="22"/>
       <c r="K20" s="14"/>
       <c r="L20" s="22"/>
-      <c r="M20" s="39" t="s">
+      <c r="M20" s="22"/>
+      <c r="N20" s="22"/>
+      <c r="O20" s="39" t="s">
         <v>99</v>
       </c>
-      <c r="N20" s="6"/>
-      <c r="O20" s="6"/>
       <c r="P20" s="6"/>
       <c r="Q20" s="6"/>
       <c r="R20" s="6"/>
@@ -1771,8 +1847,10 @@
       <c r="U20" s="6"/>
       <c r="V20" s="6"/>
       <c r="W20" s="6"/>
-    </row>
-    <row r="21" spans="2:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X20" s="6"/>
+      <c r="Y20" s="6"/>
+    </row>
+    <row r="21" spans="2:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="26" t="s">
         <v>68</v>
       </c>
@@ -1798,9 +1876,9 @@
       <c r="J21" s="22"/>
       <c r="K21" s="14"/>
       <c r="L21" s="22"/>
-      <c r="M21" s="20"/>
-      <c r="N21" s="6"/>
-      <c r="O21" s="6"/>
+      <c r="M21" s="22"/>
+      <c r="N21" s="22"/>
+      <c r="O21" s="20"/>
       <c r="P21" s="6"/>
       <c r="Q21" s="6"/>
       <c r="R21" s="6"/>
@@ -1809,8 +1887,10 @@
       <c r="U21" s="6"/>
       <c r="V21" s="6"/>
       <c r="W21" s="6"/>
-    </row>
-    <row r="22" spans="2:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X21" s="6"/>
+      <c r="Y21" s="6"/>
+    </row>
+    <row r="22" spans="2:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="26" t="s">
         <v>69</v>
       </c>
@@ -1836,11 +1916,11 @@
       <c r="J22" s="22"/>
       <c r="K22" s="14"/>
       <c r="L22" s="22"/>
-      <c r="M22" s="16" t="s">
+      <c r="M22" s="22"/>
+      <c r="N22" s="22"/>
+      <c r="O22" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="N22" s="6"/>
-      <c r="O22" s="6"/>
       <c r="P22" s="6"/>
       <c r="Q22" s="6"/>
       <c r="R22" s="6"/>
@@ -1849,8 +1929,10 @@
       <c r="U22" s="6"/>
       <c r="V22" s="6"/>
       <c r="W22" s="6"/>
-    </row>
-    <row r="23" spans="2:23" s="31" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X22" s="6"/>
+      <c r="Y22" s="6"/>
+    </row>
+    <row r="23" spans="2:25" s="31" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="26" t="s">
         <v>94</v>
       </c>
@@ -1876,9 +1958,9 @@
       <c r="J23" s="22"/>
       <c r="K23" s="14"/>
       <c r="L23" s="22"/>
-      <c r="M23" s="16"/>
-      <c r="N23" s="6"/>
-      <c r="O23" s="6"/>
+      <c r="M23" s="22"/>
+      <c r="N23" s="22"/>
+      <c r="O23" s="16"/>
       <c r="P23" s="6"/>
       <c r="Q23" s="6"/>
       <c r="R23" s="6"/>
@@ -1887,8 +1969,10 @@
       <c r="U23" s="6"/>
       <c r="V23" s="6"/>
       <c r="W23" s="6"/>
-    </row>
-    <row r="24" spans="2:23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X23" s="6"/>
+      <c r="Y23" s="6"/>
+    </row>
+    <row r="24" spans="2:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="26" t="s">
         <v>71</v>
       </c>
@@ -1914,11 +1998,11 @@
       <c r="J24" s="22"/>
       <c r="K24" s="14"/>
       <c r="L24" s="22"/>
-      <c r="M24" s="16" t="s">
+      <c r="M24" s="22"/>
+      <c r="N24" s="22"/>
+      <c r="O24" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="N24" s="6"/>
-      <c r="O24" s="6"/>
       <c r="P24" s="6"/>
       <c r="Q24" s="6"/>
       <c r="R24" s="6"/>
@@ -1927,8 +2011,10 @@
       <c r="U24" s="6"/>
       <c r="V24" s="6"/>
       <c r="W24" s="6"/>
-    </row>
-    <row r="25" spans="2:23" s="31" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X24" s="6"/>
+      <c r="Y24" s="6"/>
+    </row>
+    <row r="25" spans="2:25" s="31" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="26" t="s">
         <v>96</v>
       </c>
@@ -1954,11 +2040,11 @@
       <c r="J25" s="22"/>
       <c r="K25" s="14"/>
       <c r="L25" s="22"/>
-      <c r="M25" s="16" t="s">
+      <c r="M25" s="22"/>
+      <c r="N25" s="22"/>
+      <c r="O25" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="N25" s="6"/>
-      <c r="O25" s="6"/>
       <c r="P25" s="6"/>
       <c r="Q25" s="6"/>
       <c r="R25" s="6"/>
@@ -1967,14 +2053,16 @@
       <c r="U25" s="6"/>
       <c r="V25" s="6"/>
       <c r="W25" s="6"/>
-    </row>
-    <row r="26" spans="2:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="2:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="2:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="2:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="2:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="2:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="X25" s="6"/>
+      <c r="Y25" s="6"/>
+    </row>
+    <row r="26" spans="2:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="2:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="2:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="2:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="2:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="2:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="2:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2946,7 +3034,7 @@
     <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B2:M2"/>
+    <mergeCell ref="B2:O2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
added code to check problem linked to a diagnostic report
</commit_message>
<xml_diff>
--- a/Data/Test Suite Prerequisites.xlsx
+++ b/Data/Test Suite Prerequisites.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\development\feature\1.5.0\gpconnect-provider-testing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF3F6879-B37A-4913-B05E-0355A83B80D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00BABB6F-686C-4E2F-9F2B-A0E5DC230B3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27765" yWindow="405" windowWidth="19920" windowHeight="13515" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Patients" sheetId="1" r:id="rId1"/>
@@ -381,7 +381,7 @@
   </si>
   <si>
     <t>x
-Patient Linked to DiagnosticReport, ProcedureRequests,  specimens and a problem linked</t>
+Patient Linked to DiagnosticReport, ProcedureRequests,  specimens and a problem linked to a diagnostic report</t>
   </si>
 </sst>
 </file>
@@ -1003,8 +1003,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E3" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView tabSelected="1" topLeftCell="I3" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
updated investigations tests to include detailed checks for test report filings
</commit_message>
<xml_diff>
--- a/Data/Test Suite Prerequisites.xlsx
+++ b/Data/Test Suite Prerequisites.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\development\feature\1.5.0\gpconnect-provider-testing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00BABB6F-686C-4E2F-9F2B-A0E5DC230B3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC6E9E38-B393-4B5A-AE86-6674972ACFE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27765" yWindow="405" windowWidth="19920" windowHeight="13515" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Patients" sheetId="1" r:id="rId1"/>
@@ -341,9 +341,6 @@
 Meds TimePeriod Test Requires data from 3 years back from current system date</t>
   </si>
   <si>
-    <t>No Data for new structurea areas(Imms, uncat, problems and consultations)</t>
-  </si>
-  <si>
     <t>Patient Must Have :
 - Consultation that is linked to only clinical items
 - Consultation That is only Linked to A topic that is only linked to clinical items (no heading)
@@ -369,10 +366,6 @@
   </si>
   <si>
     <t>x
-Patient Linked to DiagnosticReport, ProcedureRequests and specimens and a NO problems linked</t>
-  </si>
-  <si>
-    <t>x
 Patient Linked to ReferralRequests and  linked to a problem</t>
   </si>
   <si>
@@ -380,8 +373,15 @@
 Patient Linked to ReferralRequests and  NOT linked to a problem</t>
   </si>
   <si>
+    <t>No Data for new structurea areas(Imms, uncat, problems and consultations, investigations, referrals)</t>
+  </si>
+  <si>
     <t>x
-Patient Linked to DiagnosticReport, ProcedureRequests,  specimens and a problem linked to a diagnostic report</t>
+Patient Linked to DiagnosticReport linked to a  ProcedureRequest,  specimen, test group, test report filing and also a problem linked to a diagnostic report</t>
+  </si>
+  <si>
+    <t>x
+Patient Linked to DiagnosticReport linked to a  ProcedureRequest,  specimen, test group, test report filing BUT NOT linked to any problems</t>
   </si>
 </sst>
 </file>
@@ -1004,7 +1004,7 @@
   <dimension ref="A1:Y1001"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I3" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1133,10 +1133,10 @@
         <v>101</v>
       </c>
       <c r="M4" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="N4" s="22" t="s">
         <v>106</v>
-      </c>
-      <c r="N4" s="22" t="s">
-        <v>107</v>
       </c>
       <c r="O4" s="16" t="s">
         <v>19</v>
@@ -1227,13 +1227,13 @@
         <v>26</v>
       </c>
       <c r="M6" s="22" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="N6" s="22" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="O6" s="20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="P6" s="6"/>
       <c r="Q6" s="6"/>
@@ -1281,13 +1281,13 @@
         <v>26</v>
       </c>
       <c r="M7" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="N7" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="N7" s="22" t="s">
-        <v>110</v>
-      </c>
       <c r="O7" s="20" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="P7" s="6"/>
       <c r="Q7" s="6"/>
@@ -1341,7 +1341,7 @@
         <v>0</v>
       </c>
       <c r="O8" s="20" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="P8" s="6"/>
       <c r="Q8" s="6"/>

</xml_diff>

<commit_message>
Added remaining 1.2.7 tests and changed new search for slots test around serviceCategory and ServiceType
</commit_message>
<xml_diff>
--- a/Data/Test Suite Prerequisites.xlsx
+++ b/Data/Test Suite Prerequisites.xlsx
@@ -1,30 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\development\feature\1.2.4\gpconnect-provider-testing\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\development\feature\1.2.7\gpconnect-provider-testing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B88F7DD-E436-44EB-9628-9190CAB427D0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E637B9E2-F998-4FDF-97DE-69F33F8FD00C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Patients" sheetId="1" r:id="rId1"/>
     <sheet name="Organizations" sheetId="2" r:id="rId2"/>
     <sheet name="Locations" sheetId="3" r:id="rId3"/>
     <sheet name="Practitioner" sheetId="4" r:id="rId4"/>
-    <sheet name="Slots" sheetId="5" r:id="rId5"/>
+    <sheet name="Schedule and Slots" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="114">
   <si>
     <t>Required Organizations and Slots for testing</t>
   </si>
@@ -344,6 +344,33 @@
   <si>
     <t>Patient has an AllergyIntolerance with no allergy EndReason
 Patient Has Warning Codes :  Data in Transit &amp;  Data Awaiting Filing &amp;  Confidential Items on  Allergies</t>
+  </si>
+  <si>
+    <t>Requirements for Schedule and Slots for Tests relating to serviceCategory and serviceType</t>
+  </si>
+  <si>
+    <t>Schedule Day 1</t>
+  </si>
+  <si>
+    <t>Slots on Day 1</t>
+  </si>
+  <si>
+    <t>Slots on Day 2</t>
+  </si>
+  <si>
+    <t>Schedule Day 2</t>
+  </si>
+  <si>
+    <t>Schedule Should have NO serviceCategory set</t>
+  </si>
+  <si>
+    <t>Schedule Should have serviceCategory set to something</t>
+  </si>
+  <si>
+    <t>Slots Should have NO serviceType set</t>
+  </si>
+  <si>
+    <t>Slots Should have serviceType set to something</t>
   </si>
 </sst>
 </file>
@@ -353,7 +380,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -397,8 +424,15 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -445,6 +479,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFBE5D6"/>
         <bgColor rgb="FFFBE5D6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -507,7 +547,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -618,6 +658,16 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -964,7 +1014,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
@@ -973,7 +1023,7 @@
     <col min="1" max="1" width="2.7109375" customWidth="1"/>
     <col min="2" max="2" width="22.5703125" customWidth="1"/>
     <col min="3" max="3" width="19.85546875" customWidth="1"/>
-    <col min="4" max="4" width="54" customWidth="1"/>
+    <col min="4" max="4" width="35.42578125" customWidth="1"/>
     <col min="5" max="15" width="19.85546875" customWidth="1"/>
     <col min="16" max="16" width="62.7109375" customWidth="1"/>
     <col min="17" max="26" width="11.5703125" customWidth="1"/>
@@ -7474,7 +7524,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:P1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7889,11 +7941,13 @@
     </row>
     <row r="20" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
+      <c r="B20" s="46" t="s">
+        <v>105</v>
+      </c>
+      <c r="C20" s="46"/>
+      <c r="D20" s="46"/>
+      <c r="E20" s="46"/>
+      <c r="F20" s="46"/>
       <c r="G20" s="11"/>
       <c r="H20" s="11"/>
       <c r="I20" s="11"/>
@@ -7907,11 +7961,15 @@
     </row>
     <row r="21" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="11"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
+      <c r="B21" s="44" t="s">
+        <v>106</v>
+      </c>
+      <c r="C21" s="47" t="s">
+        <v>110</v>
+      </c>
+      <c r="D21" s="47"/>
+      <c r="E21" s="47"/>
+      <c r="F21" s="47"/>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
       <c r="I21" s="11"/>
@@ -7923,10 +7981,46 @@
       <c r="O21" s="11"/>
       <c r="P21" s="11"/>
     </row>
-    <row r="22" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="44" t="s">
+        <v>109</v>
+      </c>
+      <c r="C22" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="D22" s="47"/>
+      <c r="E22" s="47"/>
+      <c r="F22" s="47"/>
+    </row>
+    <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="44" t="s">
+        <v>107</v>
+      </c>
+      <c r="C23" s="47" t="s">
+        <v>112</v>
+      </c>
+      <c r="D23" s="47"/>
+      <c r="E23" s="47"/>
+      <c r="F23" s="47"/>
+    </row>
+    <row r="24" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="44" t="s">
+        <v>108</v>
+      </c>
+      <c r="C24" s="47" t="s">
+        <v>113</v>
+      </c>
+      <c r="D24" s="47"/>
+      <c r="E24" s="47"/>
+      <c r="F24" s="47"/>
+    </row>
+    <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="45"/>
+      <c r="C25" s="45"/>
+      <c r="D25" s="45"/>
+      <c r="E25" s="45"/>
+      <c r="F25" s="45"/>
+    </row>
     <row r="26" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="28" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -8903,11 +8997,16 @@
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="6">
+    <mergeCell ref="C24:F24"/>
     <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="C23:F23"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0" footer="0"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>

<commit_message>
updated tests based on providers not supporting both elements
</commit_message>
<xml_diff>
--- a/Data/Test Suite Prerequisites.xlsx
+++ b/Data/Test Suite Prerequisites.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\development\feature\1.2.7\gpconnect-provider-testing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E637B9E2-F998-4FDF-97DE-69F33F8FD00C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DB6678D-0C7F-4FE1-A5EB-002B958E9AD0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24840" yWindow="1800" windowWidth="21600" windowHeight="11385" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Patients" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="108">
   <si>
     <t>Required Organizations and Slots for testing</t>
   </si>
@@ -349,28 +349,32 @@
     <t>Requirements for Schedule and Slots for Tests relating to serviceCategory and serviceType</t>
   </si>
   <si>
-    <t>Schedule Day 1</t>
-  </si>
-  <si>
-    <t>Slots on Day 1</t>
-  </si>
-  <si>
-    <t>Slots on Day 2</t>
-  </si>
-  <si>
-    <t>Schedule Day 2</t>
-  </si>
-  <si>
-    <t>Schedule Should have NO serviceCategory set</t>
-  </si>
-  <si>
-    <t>Schedule Should have serviceCategory set to something</t>
-  </si>
-  <si>
-    <t>Slots Should have NO serviceType set</t>
-  </si>
-  <si>
-    <t>Slots Should have serviceType set to something</t>
+    <r>
+      <t xml:space="preserve">If supported : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>Schedule contains a serviceCategory and the slots will have a serviceType</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">If supported : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.5"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>Appointments contains serviceCategory and a serviceType</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -380,7 +384,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -430,6 +434,12 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9.5"/>
+      <color rgb="FF000000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="10">
@@ -547,7 +557,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -650,6 +660,7 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -660,14 +671,7 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1058,23 +1062,23 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2" spans="1:26" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="41"/>
-      <c r="K2" s="41"/>
-      <c r="L2" s="41"/>
-      <c r="M2" s="41"/>
-      <c r="N2" s="41"/>
-      <c r="O2" s="41"/>
-      <c r="P2" s="41"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="42"/>
+      <c r="N2" s="42"/>
+      <c r="O2" s="42"/>
+      <c r="P2" s="42"/>
       <c r="Q2" s="6"/>
       <c r="R2" s="6"/>
       <c r="S2" s="6"/>
@@ -4507,18 +4511,18 @@
     </row>
     <row r="2" spans="1:21" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="41"/>
-      <c r="K2" s="41"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
@@ -7522,10 +7526,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:P1000"/>
+  <dimension ref="A1:P997"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20:F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -7559,11 +7563,11 @@
     </row>
     <row r="2" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11"/>
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="44" t="s">
         <v>83</v>
       </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
       <c r="E2" s="34"/>
       <c r="F2" s="34"/>
       <c r="G2" s="11"/>
@@ -7941,13 +7945,13 @@
     </row>
     <row r="20" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11"/>
-      <c r="B20" s="46" t="s">
+      <c r="B20" s="45" t="s">
         <v>105</v>
       </c>
-      <c r="C20" s="46"/>
-      <c r="D20" s="46"/>
-      <c r="E20" s="46"/>
-      <c r="F20" s="46"/>
+      <c r="C20" s="45"/>
+      <c r="D20" s="45"/>
+      <c r="E20" s="45"/>
+      <c r="F20" s="45"/>
       <c r="G20" s="11"/>
       <c r="H20" s="11"/>
       <c r="I20" s="11"/>
@@ -7961,15 +7965,13 @@
     </row>
     <row r="21" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="11"/>
-      <c r="B21" s="44" t="s">
+      <c r="B21" s="40" t="s">
         <v>106</v>
       </c>
-      <c r="C21" s="47" t="s">
-        <v>110</v>
-      </c>
-      <c r="D21" s="47"/>
-      <c r="E21" s="47"/>
-      <c r="F21" s="47"/>
+      <c r="C21" s="40"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="40"/>
+      <c r="F21" s="40"/>
       <c r="G21" s="11"/>
       <c r="H21" s="11"/>
       <c r="I21" s="11"/>
@@ -7982,45 +7984,17 @@
       <c r="P21" s="11"/>
     </row>
     <row r="22" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="44" t="s">
-        <v>109</v>
-      </c>
-      <c r="C22" s="47" t="s">
-        <v>111</v>
-      </c>
-      <c r="D22" s="47"/>
-      <c r="E22" s="47"/>
-      <c r="F22" s="47"/>
-    </row>
-    <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="44" t="s">
+      <c r="B22" s="40" t="s">
         <v>107</v>
       </c>
-      <c r="C23" s="47" t="s">
-        <v>112</v>
-      </c>
-      <c r="D23" s="47"/>
-      <c r="E23" s="47"/>
-      <c r="F23" s="47"/>
-    </row>
-    <row r="24" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="44" t="s">
-        <v>108</v>
-      </c>
-      <c r="C24" s="47" t="s">
-        <v>113</v>
-      </c>
-      <c r="D24" s="47"/>
-      <c r="E24" s="47"/>
-      <c r="F24" s="47"/>
-    </row>
-    <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="45"/>
-      <c r="C25" s="45"/>
-      <c r="D25" s="45"/>
-      <c r="E25" s="45"/>
-      <c r="F25" s="45"/>
-    </row>
+      <c r="C22" s="40"/>
+      <c r="D22" s="40"/>
+      <c r="E22" s="40"/>
+      <c r="F22" s="40"/>
+    </row>
+    <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="26" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="28" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -8993,17 +8967,10 @@
     <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="C24:F24"/>
+  <mergeCells count="2">
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B20:F20"/>
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="C22:F22"/>
-    <mergeCell ref="C23:F23"/>
   </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
updated data requirements spreadsheet and app.config
</commit_message>
<xml_diff>
--- a/Data/Test Suite Prerequisites.xlsx
+++ b/Data/Test Suite Prerequisites.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\development\Merge\1.2.7 to 1.5.0\1.5.0\1.5.0-gpconnect-provider-testing\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\development\feature\1.5.0\gpconnect-provider-testing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EEB7322-266B-483F-8D6B-B59C795005F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2E421D8-3019-4E1C-AAF0-EA50483C144F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Patients" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="116">
   <si>
     <t>Required Organizations and Slots for testing</t>
   </si>
@@ -413,6 +413,9 @@
       </rPr>
       <t>Appointments contains serviceCategory and a serviceType</t>
     </r>
+  </si>
+  <si>
+    <t>Documents</t>
   </si>
 </sst>
 </file>
@@ -698,6 +701,11 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -709,14 +717,9 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1059,10 +1062,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y1001"/>
+  <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView topLeftCell="I3" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1073,11 +1076,12 @@
     <col min="4" max="4" width="54" customWidth="1"/>
     <col min="5" max="8" width="19.85546875" customWidth="1"/>
     <col min="9" max="14" width="19.85546875" style="31" customWidth="1"/>
-    <col min="15" max="15" width="62.7109375" customWidth="1"/>
-    <col min="16" max="25" width="11.5703125" customWidth="1"/>
+    <col min="15" max="15" width="13.7109375" style="31" customWidth="1"/>
+    <col min="16" max="16" width="62.7109375" customWidth="1"/>
+    <col min="17" max="26" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -1103,25 +1107,26 @@
       <c r="W1" s="2"/>
       <c r="X1" s="2"/>
       <c r="Y1" s="2"/>
-    </row>
-    <row r="2" spans="1:25" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="40" t="s">
+      <c r="Z1" s="2"/>
+    </row>
+    <row r="2" spans="1:26" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="42"/>
-      <c r="J2" s="42"/>
-      <c r="K2" s="42"/>
-      <c r="L2" s="42"/>
-      <c r="M2" s="42"/>
-      <c r="N2" s="42"/>
-      <c r="O2" s="41"/>
-      <c r="P2" s="6"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
+      <c r="K2" s="45"/>
+      <c r="L2" s="45"/>
+      <c r="M2" s="45"/>
+      <c r="N2" s="45"/>
+      <c r="O2" s="45"/>
+      <c r="P2" s="44"/>
       <c r="Q2" s="6"/>
       <c r="R2" s="6"/>
       <c r="S2" s="6"/>
@@ -1131,8 +1136,9 @@
       <c r="W2" s="6"/>
       <c r="X2" s="6"/>
       <c r="Y2" s="6"/>
-    </row>
-    <row r="3" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z2" s="6"/>
+    </row>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="6"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -1146,7 +1152,7 @@
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
-      <c r="O3" s="6"/>
+      <c r="O3" s="2"/>
       <c r="P3" s="6"/>
       <c r="Q3" s="6"/>
       <c r="R3" s="6"/>
@@ -1157,8 +1163,9 @@
       <c r="W3" s="6"/>
       <c r="X3" s="6"/>
       <c r="Y3" s="6"/>
-    </row>
-    <row r="4" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+      <c r="Z3" s="6"/>
+    </row>
+    <row r="4" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="B4" s="8"/>
       <c r="C4" s="10" t="s">
         <v>5</v>
@@ -1196,10 +1203,12 @@
       <c r="N4" s="22" t="s">
         <v>106</v>
       </c>
-      <c r="O4" s="16" t="s">
+      <c r="O4" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="P4" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="P4" s="6"/>
       <c r="Q4" s="6"/>
       <c r="R4" s="6"/>
       <c r="S4" s="6"/>
@@ -1209,8 +1218,9 @@
       <c r="W4" s="6"/>
       <c r="X4" s="6"/>
       <c r="Y4" s="6"/>
-    </row>
-    <row r="5" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z4" s="6"/>
+    </row>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="18" t="s">
         <v>20</v>
       </c>
@@ -1238,8 +1248,8 @@
       <c r="L5" s="22"/>
       <c r="M5" s="22"/>
       <c r="N5" s="22"/>
-      <c r="O5" s="20"/>
-      <c r="P5" s="6"/>
+      <c r="O5" s="22"/>
+      <c r="P5" s="20"/>
       <c r="Q5" s="6"/>
       <c r="R5" s="6"/>
       <c r="S5" s="6"/>
@@ -1249,8 +1259,9 @@
       <c r="W5" s="6"/>
       <c r="X5" s="6"/>
       <c r="Y5" s="6"/>
-    </row>
-    <row r="6" spans="1:25" ht="165" x14ac:dyDescent="0.25">
+      <c r="Z5" s="6"/>
+    </row>
+    <row r="6" spans="1:26" ht="165" x14ac:dyDescent="0.25">
       <c r="B6" s="18" t="s">
         <v>25</v>
       </c>
@@ -1290,10 +1301,12 @@
       <c r="N6" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="O6" s="20" t="s">
+      <c r="O6" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="P6" s="20" t="s">
         <v>103</v>
       </c>
-      <c r="P6" s="6"/>
       <c r="Q6" s="6"/>
       <c r="R6" s="6"/>
       <c r="S6" s="6"/>
@@ -1303,8 +1316,9 @@
       <c r="W6" s="6"/>
       <c r="X6" s="6"/>
       <c r="Y6" s="6"/>
-    </row>
-    <row r="7" spans="1:25" ht="165" x14ac:dyDescent="0.25">
+      <c r="Z6" s="6"/>
+    </row>
+    <row r="7" spans="1:26" ht="165" x14ac:dyDescent="0.25">
       <c r="B7" s="18" t="s">
         <v>34</v>
       </c>
@@ -1344,10 +1358,10 @@
       <c r="N7" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="O7" s="20" t="s">
+      <c r="O7" s="22"/>
+      <c r="P7" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="P7" s="6"/>
       <c r="Q7" s="6"/>
       <c r="R7" s="6"/>
       <c r="S7" s="6"/>
@@ -1357,8 +1371,9 @@
       <c r="W7" s="6"/>
       <c r="X7" s="6"/>
       <c r="Y7" s="6"/>
-    </row>
-    <row r="8" spans="1:25" ht="30" x14ac:dyDescent="0.25">
+      <c r="Z7" s="6"/>
+    </row>
+    <row r="8" spans="1:26" ht="30" x14ac:dyDescent="0.25">
       <c r="B8" s="18" t="s">
         <v>35</v>
       </c>
@@ -1398,10 +1413,10 @@
       <c r="N8" s="22">
         <v>0</v>
       </c>
-      <c r="O8" s="20" t="s">
+      <c r="O8" s="22"/>
+      <c r="P8" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="P8" s="6"/>
       <c r="Q8" s="6"/>
       <c r="R8" s="6"/>
       <c r="S8" s="6"/>
@@ -1411,8 +1426,9 @@
       <c r="W8" s="6"/>
       <c r="X8" s="6"/>
       <c r="Y8" s="6"/>
-    </row>
-    <row r="9" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z8" s="6"/>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="18" t="s">
         <v>37</v>
       </c>
@@ -1440,8 +1456,8 @@
       <c r="L9" s="22"/>
       <c r="M9" s="22"/>
       <c r="N9" s="22"/>
-      <c r="O9" s="20"/>
-      <c r="P9" s="6"/>
+      <c r="O9" s="22"/>
+      <c r="P9" s="20"/>
       <c r="Q9" s="6"/>
       <c r="R9" s="6"/>
       <c r="S9" s="6"/>
@@ -1451,8 +1467,9 @@
       <c r="W9" s="6"/>
       <c r="X9" s="6"/>
       <c r="Y9" s="6"/>
-    </row>
-    <row r="10" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z9" s="6"/>
+    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="18" t="s">
         <v>39</v>
       </c>
@@ -1480,8 +1497,8 @@
       <c r="L10" s="22"/>
       <c r="M10" s="22"/>
       <c r="N10" s="22"/>
-      <c r="O10" s="20"/>
-      <c r="P10" s="6"/>
+      <c r="O10" s="22"/>
+      <c r="P10" s="20"/>
       <c r="Q10" s="6"/>
       <c r="R10" s="6"/>
       <c r="S10" s="6"/>
@@ -1491,8 +1508,9 @@
       <c r="W10" s="6"/>
       <c r="X10" s="6"/>
       <c r="Y10" s="6"/>
-    </row>
-    <row r="11" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z10" s="6"/>
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="18" t="s">
         <v>40</v>
       </c>
@@ -1520,8 +1538,8 @@
       <c r="L11" s="22"/>
       <c r="M11" s="22"/>
       <c r="N11" s="22"/>
-      <c r="O11" s="20"/>
-      <c r="P11" s="6"/>
+      <c r="O11" s="22"/>
+      <c r="P11" s="20"/>
       <c r="Q11" s="6"/>
       <c r="R11" s="6"/>
       <c r="S11" s="6"/>
@@ -1531,8 +1549,9 @@
       <c r="W11" s="6"/>
       <c r="X11" s="6"/>
       <c r="Y11" s="6"/>
-    </row>
-    <row r="12" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z11" s="6"/>
+    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="18" t="s">
         <v>41</v>
       </c>
@@ -1560,8 +1579,8 @@
       <c r="L12" s="22"/>
       <c r="M12" s="22"/>
       <c r="N12" s="22"/>
-      <c r="O12" s="20"/>
-      <c r="P12" s="6"/>
+      <c r="O12" s="22"/>
+      <c r="P12" s="20"/>
       <c r="Q12" s="6"/>
       <c r="R12" s="6"/>
       <c r="S12" s="6"/>
@@ -1571,8 +1590,9 @@
       <c r="W12" s="6"/>
       <c r="X12" s="6"/>
       <c r="Y12" s="6"/>
-    </row>
-    <row r="13" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z12" s="6"/>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="26" t="s">
         <v>43</v>
       </c>
@@ -1600,10 +1620,10 @@
       <c r="L13" s="22"/>
       <c r="M13" s="22"/>
       <c r="N13" s="22"/>
-      <c r="O13" s="16" t="s">
+      <c r="O13" s="22"/>
+      <c r="P13" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="P13" s="6"/>
       <c r="Q13" s="6"/>
       <c r="R13" s="6"/>
       <c r="S13" s="6"/>
@@ -1613,8 +1633,9 @@
       <c r="W13" s="6"/>
       <c r="X13" s="6"/>
       <c r="Y13" s="6"/>
-    </row>
-    <row r="14" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z13" s="6"/>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="26" t="s">
         <v>45</v>
       </c>
@@ -1642,10 +1663,10 @@
       <c r="L14" s="22"/>
       <c r="M14" s="22"/>
       <c r="N14" s="22"/>
-      <c r="O14" s="16" t="s">
+      <c r="O14" s="22"/>
+      <c r="P14" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="P14" s="6"/>
       <c r="Q14" s="6"/>
       <c r="R14" s="6"/>
       <c r="S14" s="6"/>
@@ -1655,8 +1676,9 @@
       <c r="W14" s="6"/>
       <c r="X14" s="6"/>
       <c r="Y14" s="6"/>
-    </row>
-    <row r="15" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z14" s="6"/>
+    </row>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="26" t="s">
         <v>46</v>
       </c>
@@ -1684,10 +1706,10 @@
       <c r="L15" s="22"/>
       <c r="M15" s="22"/>
       <c r="N15" s="22"/>
-      <c r="O15" s="16" t="s">
+      <c r="O15" s="22"/>
+      <c r="P15" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="P15" s="6"/>
       <c r="Q15" s="6"/>
       <c r="R15" s="6"/>
       <c r="S15" s="6"/>
@@ -1697,8 +1719,9 @@
       <c r="W15" s="6"/>
       <c r="X15" s="6"/>
       <c r="Y15" s="6"/>
-    </row>
-    <row r="16" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z15" s="6"/>
+    </row>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="26" t="s">
         <v>48</v>
       </c>
@@ -1726,10 +1749,10 @@
       <c r="L16" s="22"/>
       <c r="M16" s="22"/>
       <c r="N16" s="22"/>
-      <c r="O16" s="16" t="s">
+      <c r="O16" s="22"/>
+      <c r="P16" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="P16" s="6"/>
       <c r="Q16" s="6"/>
       <c r="R16" s="6"/>
       <c r="S16" s="6"/>
@@ -1739,8 +1762,9 @@
       <c r="W16" s="6"/>
       <c r="X16" s="6"/>
       <c r="Y16" s="6"/>
-    </row>
-    <row r="17" spans="2:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z16" s="6"/>
+    </row>
+    <row r="17" spans="2:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="26" t="s">
         <v>50</v>
       </c>
@@ -1768,10 +1792,10 @@
       <c r="L17" s="22"/>
       <c r="M17" s="22"/>
       <c r="N17" s="22"/>
-      <c r="O17" s="16" t="s">
+      <c r="O17" s="22"/>
+      <c r="P17" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="P17" s="6"/>
       <c r="Q17" s="6"/>
       <c r="R17" s="6"/>
       <c r="S17" s="6"/>
@@ -1781,8 +1805,9 @@
       <c r="W17" s="6"/>
       <c r="X17" s="6"/>
       <c r="Y17" s="6"/>
-    </row>
-    <row r="18" spans="2:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z17" s="6"/>
+    </row>
+    <row r="18" spans="2:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="26" t="s">
         <v>55</v>
       </c>
@@ -1810,10 +1835,10 @@
       <c r="L18" s="22"/>
       <c r="M18" s="22"/>
       <c r="N18" s="22"/>
-      <c r="O18" s="16" t="s">
+      <c r="O18" s="22"/>
+      <c r="P18" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="P18" s="6"/>
       <c r="Q18" s="6"/>
       <c r="R18" s="6"/>
       <c r="S18" s="6"/>
@@ -1823,8 +1848,9 @@
       <c r="W18" s="6"/>
       <c r="X18" s="6"/>
       <c r="Y18" s="6"/>
-    </row>
-    <row r="19" spans="2:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z18" s="6"/>
+    </row>
+    <row r="19" spans="2:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="26" t="s">
         <v>60</v>
       </c>
@@ -1852,10 +1878,10 @@
       <c r="L19" s="22"/>
       <c r="M19" s="22"/>
       <c r="N19" s="22"/>
-      <c r="O19" s="16" t="s">
+      <c r="O19" s="22"/>
+      <c r="P19" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="P19" s="6"/>
       <c r="Q19" s="6"/>
       <c r="R19" s="6"/>
       <c r="S19" s="6"/>
@@ -1865,8 +1891,9 @@
       <c r="W19" s="6"/>
       <c r="X19" s="6"/>
       <c r="Y19" s="6"/>
-    </row>
-    <row r="20" spans="2:25" ht="45" x14ac:dyDescent="0.25">
+      <c r="Z19" s="6"/>
+    </row>
+    <row r="20" spans="2:26" ht="45" x14ac:dyDescent="0.25">
       <c r="B20" s="26" t="s">
         <v>64</v>
       </c>
@@ -1894,10 +1921,10 @@
       <c r="L20" s="22"/>
       <c r="M20" s="22"/>
       <c r="N20" s="22"/>
-      <c r="O20" s="39" t="s">
+      <c r="O20" s="22"/>
+      <c r="P20" s="39" t="s">
         <v>99</v>
       </c>
-      <c r="P20" s="6"/>
       <c r="Q20" s="6"/>
       <c r="R20" s="6"/>
       <c r="S20" s="6"/>
@@ -1907,8 +1934,9 @@
       <c r="W20" s="6"/>
       <c r="X20" s="6"/>
       <c r="Y20" s="6"/>
-    </row>
-    <row r="21" spans="2:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z20" s="6"/>
+    </row>
+    <row r="21" spans="2:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="26" t="s">
         <v>68</v>
       </c>
@@ -1936,8 +1964,8 @@
       <c r="L21" s="22"/>
       <c r="M21" s="22"/>
       <c r="N21" s="22"/>
-      <c r="O21" s="20"/>
-      <c r="P21" s="6"/>
+      <c r="O21" s="22"/>
+      <c r="P21" s="20"/>
       <c r="Q21" s="6"/>
       <c r="R21" s="6"/>
       <c r="S21" s="6"/>
@@ -1947,8 +1975,9 @@
       <c r="W21" s="6"/>
       <c r="X21" s="6"/>
       <c r="Y21" s="6"/>
-    </row>
-    <row r="22" spans="2:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z21" s="6"/>
+    </row>
+    <row r="22" spans="2:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="26" t="s">
         <v>69</v>
       </c>
@@ -1976,10 +2005,10 @@
       <c r="L22" s="22"/>
       <c r="M22" s="22"/>
       <c r="N22" s="22"/>
-      <c r="O22" s="16" t="s">
+      <c r="O22" s="22"/>
+      <c r="P22" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="P22" s="6"/>
       <c r="Q22" s="6"/>
       <c r="R22" s="6"/>
       <c r="S22" s="6"/>
@@ -1989,8 +2018,9 @@
       <c r="W22" s="6"/>
       <c r="X22" s="6"/>
       <c r="Y22" s="6"/>
-    </row>
-    <row r="23" spans="2:25" s="31" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z22" s="6"/>
+    </row>
+    <row r="23" spans="2:26" s="31" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="26" t="s">
         <v>94</v>
       </c>
@@ -2018,8 +2048,8 @@
       <c r="L23" s="22"/>
       <c r="M23" s="22"/>
       <c r="N23" s="22"/>
-      <c r="O23" s="16"/>
-      <c r="P23" s="6"/>
+      <c r="O23" s="22"/>
+      <c r="P23" s="16"/>
       <c r="Q23" s="6"/>
       <c r="R23" s="6"/>
       <c r="S23" s="6"/>
@@ -2029,8 +2059,9 @@
       <c r="W23" s="6"/>
       <c r="X23" s="6"/>
       <c r="Y23" s="6"/>
-    </row>
-    <row r="24" spans="2:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z23" s="6"/>
+    </row>
+    <row r="24" spans="2:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="26" t="s">
         <v>71</v>
       </c>
@@ -2058,10 +2089,10 @@
       <c r="L24" s="22"/>
       <c r="M24" s="22"/>
       <c r="N24" s="22"/>
-      <c r="O24" s="16" t="s">
+      <c r="O24" s="22"/>
+      <c r="P24" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="P24" s="6"/>
       <c r="Q24" s="6"/>
       <c r="R24" s="6"/>
       <c r="S24" s="6"/>
@@ -2071,8 +2102,9 @@
       <c r="W24" s="6"/>
       <c r="X24" s="6"/>
       <c r="Y24" s="6"/>
-    </row>
-    <row r="25" spans="2:25" s="31" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Z24" s="6"/>
+    </row>
+    <row r="25" spans="2:26" s="31" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="26" t="s">
         <v>96</v>
       </c>
@@ -2100,10 +2132,10 @@
       <c r="L25" s="22"/>
       <c r="M25" s="22"/>
       <c r="N25" s="22"/>
-      <c r="O25" s="16" t="s">
+      <c r="O25" s="22"/>
+      <c r="P25" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="P25" s="6"/>
       <c r="Q25" s="6"/>
       <c r="R25" s="6"/>
       <c r="S25" s="6"/>
@@ -2113,14 +2145,15 @@
       <c r="W25" s="6"/>
       <c r="X25" s="6"/>
       <c r="Y25" s="6"/>
-    </row>
-    <row r="26" spans="2:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="2:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="2:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="2:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="2:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="2:25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="Z25" s="6"/>
+    </row>
+    <row r="26" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3092,7 +3125,7 @@
     <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B2:O2"/>
+    <mergeCell ref="B2:P2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4276,18 +4309,18 @@
     </row>
     <row r="2" spans="1:21" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="41"/>
-      <c r="K2" s="41"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="44"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
@@ -7293,7 +7326,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:P1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
@@ -7328,11 +7361,11 @@
     </row>
     <row r="2" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11"/>
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="47" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
       <c r="E2" s="34"/>
       <c r="F2" s="34"/>
       <c r="G2" s="11"/>
@@ -7708,54 +7741,54 @@
       <c r="O19" s="11"/>
       <c r="P19" s="11"/>
     </row>
-    <row r="20" spans="1:16" s="47" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="45"/>
-      <c r="B20" s="46" t="s">
+    <row r="20" spans="1:16" s="41" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="40"/>
+      <c r="B20" s="48" t="s">
         <v>112</v>
       </c>
-      <c r="C20" s="46"/>
-      <c r="D20" s="46"/>
-      <c r="E20" s="46"/>
-      <c r="F20" s="46"/>
-      <c r="G20" s="45"/>
-      <c r="H20" s="45"/>
-      <c r="I20" s="45"/>
-      <c r="J20" s="45"/>
-      <c r="K20" s="45"/>
-      <c r="L20" s="45"/>
-      <c r="M20" s="45"/>
-      <c r="N20" s="45"/>
-      <c r="O20" s="45"/>
-      <c r="P20" s="45"/>
-    </row>
-    <row r="21" spans="1:16" s="47" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="45"/>
-      <c r="B21" s="48" t="s">
+      <c r="C20" s="48"/>
+      <c r="D20" s="48"/>
+      <c r="E20" s="48"/>
+      <c r="F20" s="48"/>
+      <c r="G20" s="40"/>
+      <c r="H20" s="40"/>
+      <c r="I20" s="40"/>
+      <c r="J20" s="40"/>
+      <c r="K20" s="40"/>
+      <c r="L20" s="40"/>
+      <c r="M20" s="40"/>
+      <c r="N20" s="40"/>
+      <c r="O20" s="40"/>
+      <c r="P20" s="40"/>
+    </row>
+    <row r="21" spans="1:16" s="41" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="40"/>
+      <c r="B21" s="42" t="s">
         <v>113</v>
       </c>
-      <c r="C21" s="48"/>
-      <c r="D21" s="48"/>
-      <c r="E21" s="48"/>
-      <c r="F21" s="48"/>
-      <c r="G21" s="45"/>
-      <c r="H21" s="45"/>
-      <c r="I21" s="45"/>
-      <c r="J21" s="45"/>
-      <c r="K21" s="45"/>
-      <c r="L21" s="45"/>
-      <c r="M21" s="45"/>
-      <c r="N21" s="45"/>
-      <c r="O21" s="45"/>
-      <c r="P21" s="45"/>
-    </row>
-    <row r="22" spans="1:16" s="47" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="48" t="s">
+      <c r="C21" s="42"/>
+      <c r="D21" s="42"/>
+      <c r="E21" s="42"/>
+      <c r="F21" s="42"/>
+      <c r="G21" s="40"/>
+      <c r="H21" s="40"/>
+      <c r="I21" s="40"/>
+      <c r="J21" s="40"/>
+      <c r="K21" s="40"/>
+      <c r="L21" s="40"/>
+      <c r="M21" s="40"/>
+      <c r="N21" s="40"/>
+      <c r="O21" s="40"/>
+      <c r="P21" s="40"/>
+    </row>
+    <row r="22" spans="1:16" s="41" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="42" t="s">
         <v>114</v>
       </c>
-      <c r="C22" s="48"/>
-      <c r="D22" s="48"/>
-      <c r="E22" s="48"/>
-      <c r="F22" s="48"/>
+      <c r="C22" s="42"/>
+      <c r="D22" s="42"/>
+      <c r="E22" s="42"/>
+      <c r="F22" s="42"/>
     </row>
     <row r="23" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="24" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated Data Requirements Spreadsheet
</commit_message>
<xml_diff>
--- a/Data/Test Suite Prerequisites.xlsx
+++ b/Data/Test Suite Prerequisites.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\development\feature\1.5.0\gpconnect-provider-testing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2E421D8-3019-4E1C-AAF0-EA50483C144F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62B8C3E0-2BC6-41CC-8035-10B1E9B9B5DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Patients" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="120">
   <si>
     <t>Required Organizations and Slots for testing</t>
   </si>
@@ -341,24 +341,6 @@
 Meds TimePeriod Test Requires data from 3 years back from current system date</t>
   </si>
   <si>
-    <t>Patient Must Have :
-- Consultation that is linked to only clinical items
-- Consultation That is only Linked to A topic that is only linked to clinical items (no heading)
-- Consultation that is linked to a Topic or Heading  that is linked to all supported Clinical items 
-- Consultation that is linked to a topic that is linked to a problem
-- Consultation linked to a problem but not linked to a topic or heading
-- A problem linked to a medRequest/Medication/MedStatement, AllergyIntollerance, Immunization &amp;  Observation</t>
-  </si>
-  <si>
-    <t>Patient Must Have :
-No Problems associated with Patient/Clinical Items but has data for new structured areas
-- Consultation that is linked to only clinical items
-- Consultation That is only Linked to A topic that is only linked to clinical items (no heading)
-- Consultation that is linked to a Topic or Heading  that is linked to all supported Clinical items 
-- Consultation that is linked to a topic that is linked to a problem
-- Consultation linked to a problem but not linked to a topic or heading</t>
-  </si>
-  <si>
     <t>Investigations</t>
   </si>
   <si>
@@ -371,9 +353,6 @@
   <si>
     <t>x
 Patient Linked to ReferralRequests and  NOT linked to a problem</t>
-  </si>
-  <si>
-    <t>No Data for new structurea areas(Imms, uncat, problems and consultations, investigations, referrals)</t>
   </si>
   <si>
     <t>x
@@ -416,6 +395,43 @@
   </si>
   <si>
     <t>Documents</t>
+  </si>
+  <si>
+    <t>Diary</t>
+  </si>
+  <si>
+    <t>x
+With Problems Associated to the Patients Diary Entry</t>
+  </si>
+  <si>
+    <t>x
+With NO Problems Associated to the Patients Diary Entry
+&amp;
+Diary Occurrence should atleast 20 days prior to current date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x
+</t>
+  </si>
+  <si>
+    <t>Other Requirements / Comments</t>
+  </si>
+  <si>
+    <t>x
+- Consultation that is linked to only clinical items
+- Consultation That is only Linked to A topic that is only linked to clinical items (no heading)
+- Consultation that is linked to a Topic or Heading  that is linked to all supported Clinical items 
+- Consultation that is linked to a topic that is linked to a problem
+- Consultation linked to a problem but not linked to a topic or heading
+-  A Consultation linked to a problem linked and to a Medication,  AllergyIntollerance, Immunization &amp;  Observation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x
+- Consultation that is linked to only clinical items 
+ - Consultation That is only Linked to A topic that is only linked to clinical items (no heading)
+- Consultation that is linked to a Topic or Heading  that is linked to all supported Clinical items 
+- Consultations linked to clincal Items ( Medication,  AllergyIntollerance, Immunization &amp;  Observation) 
+- No Problems associated with Patient/Consultations/Topics/Headings or Clinical Items </t>
   </si>
 </sst>
 </file>
@@ -1062,11 +1078,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1001"/>
+  <dimension ref="A1:AA1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1075,13 +1089,19 @@
     <col min="3" max="3" width="19.85546875" customWidth="1"/>
     <col min="4" max="4" width="54" customWidth="1"/>
     <col min="5" max="8" width="19.85546875" customWidth="1"/>
-    <col min="9" max="14" width="19.85546875" style="31" customWidth="1"/>
+    <col min="9" max="10" width="19.85546875" style="31" customWidth="1"/>
+    <col min="11" max="11" width="25" style="31" customWidth="1"/>
+    <col min="12" max="12" width="54.140625" style="31" customWidth="1"/>
+    <col min="13" max="13" width="24.7109375" style="31" customWidth="1"/>
+    <col min="14" max="14" width="19.85546875" style="31" customWidth="1"/>
     <col min="15" max="15" width="13.7109375" style="31" customWidth="1"/>
-    <col min="16" max="16" width="62.7109375" customWidth="1"/>
-    <col min="17" max="26" width="11.5703125" customWidth="1"/>
+    <col min="16" max="16" width="19.42578125" style="31" customWidth="1"/>
+    <col min="17" max="17" width="36.28515625" customWidth="1"/>
+    <col min="18" max="18" width="24.5703125" customWidth="1"/>
+    <col min="19" max="27" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -1108,8 +1128,9 @@
       <c r="X1" s="2"/>
       <c r="Y1" s="2"/>
       <c r="Z1" s="2"/>
-    </row>
-    <row r="2" spans="1:26" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA1" s="2"/>
+    </row>
+    <row r="2" spans="1:27" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="43" t="s">
         <v>2</v>
       </c>
@@ -1126,8 +1147,8 @@
       <c r="M2" s="45"/>
       <c r="N2" s="45"/>
       <c r="O2" s="45"/>
-      <c r="P2" s="44"/>
-      <c r="Q2" s="6"/>
+      <c r="P2" s="45"/>
+      <c r="Q2" s="44"/>
       <c r="R2" s="6"/>
       <c r="S2" s="6"/>
       <c r="T2" s="6"/>
@@ -1137,8 +1158,9 @@
       <c r="X2" s="6"/>
       <c r="Y2" s="6"/>
       <c r="Z2" s="6"/>
-    </row>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA2" s="6"/>
+    </row>
+    <row r="3" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="6"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -1153,7 +1175,7 @@
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
-      <c r="P3" s="6"/>
+      <c r="P3" s="2"/>
       <c r="Q3" s="6"/>
       <c r="R3" s="6"/>
       <c r="S3" s="6"/>
@@ -1164,8 +1186,9 @@
       <c r="X3" s="6"/>
       <c r="Y3" s="6"/>
       <c r="Z3" s="6"/>
-    </row>
-    <row r="4" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+      <c r="AA3" s="6"/>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B4" s="8"/>
       <c r="C4" s="10" t="s">
         <v>5</v>
@@ -1198,18 +1221,20 @@
         <v>101</v>
       </c>
       <c r="M4" s="22" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="N4" s="22" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="O4" s="22" t="s">
-        <v>115</v>
-      </c>
-      <c r="P4" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q4" s="6"/>
+        <v>112</v>
+      </c>
+      <c r="P4" s="22" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q4" s="16" t="s">
+        <v>117</v>
+      </c>
       <c r="R4" s="6"/>
       <c r="S4" s="6"/>
       <c r="T4" s="6"/>
@@ -1219,8 +1244,9 @@
       <c r="X4" s="6"/>
       <c r="Y4" s="6"/>
       <c r="Z4" s="6"/>
-    </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA4" s="6"/>
+    </row>
+    <row r="5" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="18" t="s">
         <v>20</v>
       </c>
@@ -1249,9 +1275,11 @@
       <c r="M5" s="22"/>
       <c r="N5" s="22"/>
       <c r="O5" s="22"/>
-      <c r="P5" s="20"/>
-      <c r="Q5" s="6"/>
-      <c r="R5" s="6"/>
+      <c r="P5" s="22"/>
+      <c r="Q5" s="20"/>
+      <c r="R5" s="18" t="s">
+        <v>20</v>
+      </c>
       <c r="S5" s="6"/>
       <c r="T5" s="6"/>
       <c r="U5" s="6"/>
@@ -1260,8 +1288,9 @@
       <c r="X5" s="6"/>
       <c r="Y5" s="6"/>
       <c r="Z5" s="6"/>
-    </row>
-    <row r="6" spans="1:26" ht="165" x14ac:dyDescent="0.25">
+      <c r="AA5" s="6"/>
+    </row>
+    <row r="6" spans="1:27" ht="195" x14ac:dyDescent="0.25">
       <c r="B6" s="18" t="s">
         <v>25</v>
       </c>
@@ -1290,25 +1319,27 @@
         <v>26</v>
       </c>
       <c r="K6" s="14" t="s">
-        <v>26</v>
+        <v>116</v>
       </c>
       <c r="L6" s="22" t="s">
-        <v>26</v>
+        <v>118</v>
       </c>
       <c r="M6" s="22" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="N6" s="22" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="O6" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="P6" s="20" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q6" s="6"/>
-      <c r="R6" s="6"/>
+      <c r="P6" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="Q6" s="20"/>
+      <c r="R6" s="18" t="s">
+        <v>25</v>
+      </c>
       <c r="S6" s="6"/>
       <c r="T6" s="6"/>
       <c r="U6" s="6"/>
@@ -1317,8 +1348,9 @@
       <c r="X6" s="6"/>
       <c r="Y6" s="6"/>
       <c r="Z6" s="6"/>
-    </row>
-    <row r="7" spans="1:26" ht="165" x14ac:dyDescent="0.25">
+      <c r="AA6" s="6"/>
+    </row>
+    <row r="7" spans="1:27" ht="150" x14ac:dyDescent="0.25">
       <c r="B7" s="18" t="s">
         <v>34</v>
       </c>
@@ -1350,20 +1382,24 @@
         <v>0</v>
       </c>
       <c r="L7" s="22" t="s">
-        <v>26</v>
+        <v>119</v>
       </c>
       <c r="M7" s="22" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="N7" s="22" t="s">
-        <v>108</v>
-      </c>
-      <c r="O7" s="22"/>
-      <c r="P7" s="20" t="s">
-        <v>104</v>
-      </c>
-      <c r="Q7" s="6"/>
-      <c r="R7" s="6"/>
+        <v>106</v>
+      </c>
+      <c r="O7" s="22">
+        <v>0</v>
+      </c>
+      <c r="P7" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q7" s="20"/>
+      <c r="R7" s="18" t="s">
+        <v>34</v>
+      </c>
       <c r="S7" s="6"/>
       <c r="T7" s="6"/>
       <c r="U7" s="6"/>
@@ -1372,8 +1408,9 @@
       <c r="X7" s="6"/>
       <c r="Y7" s="6"/>
       <c r="Z7" s="6"/>
-    </row>
-    <row r="8" spans="1:26" ht="30" x14ac:dyDescent="0.25">
+      <c r="AA7" s="6"/>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B8" s="18" t="s">
         <v>35</v>
       </c>
@@ -1414,11 +1451,13 @@
         <v>0</v>
       </c>
       <c r="O8" s="22"/>
-      <c r="P8" s="20" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q8" s="6"/>
-      <c r="R8" s="6"/>
+      <c r="P8" s="22">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="20"/>
+      <c r="R8" s="18" t="s">
+        <v>35</v>
+      </c>
       <c r="S8" s="6"/>
       <c r="T8" s="6"/>
       <c r="U8" s="6"/>
@@ -1427,8 +1466,9 @@
       <c r="X8" s="6"/>
       <c r="Y8" s="6"/>
       <c r="Z8" s="6"/>
-    </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA8" s="6"/>
+    </row>
+    <row r="9" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="18" t="s">
         <v>37</v>
       </c>
@@ -1457,9 +1497,11 @@
       <c r="M9" s="22"/>
       <c r="N9" s="22"/>
       <c r="O9" s="22"/>
-      <c r="P9" s="20"/>
-      <c r="Q9" s="6"/>
-      <c r="R9" s="6"/>
+      <c r="P9" s="22"/>
+      <c r="Q9" s="20"/>
+      <c r="R9" s="18" t="s">
+        <v>37</v>
+      </c>
       <c r="S9" s="6"/>
       <c r="T9" s="6"/>
       <c r="U9" s="6"/>
@@ -1468,8 +1510,9 @@
       <c r="X9" s="6"/>
       <c r="Y9" s="6"/>
       <c r="Z9" s="6"/>
-    </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA9" s="6"/>
+    </row>
+    <row r="10" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="18" t="s">
         <v>39</v>
       </c>
@@ -1498,9 +1541,11 @@
       <c r="M10" s="22"/>
       <c r="N10" s="22"/>
       <c r="O10" s="22"/>
-      <c r="P10" s="20"/>
-      <c r="Q10" s="6"/>
-      <c r="R10" s="6"/>
+      <c r="P10" s="22"/>
+      <c r="Q10" s="20"/>
+      <c r="R10" s="18" t="s">
+        <v>39</v>
+      </c>
       <c r="S10" s="6"/>
       <c r="T10" s="6"/>
       <c r="U10" s="6"/>
@@ -1509,8 +1554,9 @@
       <c r="X10" s="6"/>
       <c r="Y10" s="6"/>
       <c r="Z10" s="6"/>
-    </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA10" s="6"/>
+    </row>
+    <row r="11" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="18" t="s">
         <v>40</v>
       </c>
@@ -1539,9 +1585,11 @@
       <c r="M11" s="22"/>
       <c r="N11" s="22"/>
       <c r="O11" s="22"/>
-      <c r="P11" s="20"/>
-      <c r="Q11" s="6"/>
-      <c r="R11" s="6"/>
+      <c r="P11" s="22"/>
+      <c r="Q11" s="20"/>
+      <c r="R11" s="18" t="s">
+        <v>40</v>
+      </c>
       <c r="S11" s="6"/>
       <c r="T11" s="6"/>
       <c r="U11" s="6"/>
@@ -1550,8 +1598,9 @@
       <c r="X11" s="6"/>
       <c r="Y11" s="6"/>
       <c r="Z11" s="6"/>
-    </row>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA11" s="6"/>
+    </row>
+    <row r="12" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="18" t="s">
         <v>41</v>
       </c>
@@ -1580,9 +1629,11 @@
       <c r="M12" s="22"/>
       <c r="N12" s="22"/>
       <c r="O12" s="22"/>
-      <c r="P12" s="20"/>
-      <c r="Q12" s="6"/>
-      <c r="R12" s="6"/>
+      <c r="P12" s="22"/>
+      <c r="Q12" s="20"/>
+      <c r="R12" s="18" t="s">
+        <v>41</v>
+      </c>
       <c r="S12" s="6"/>
       <c r="T12" s="6"/>
       <c r="U12" s="6"/>
@@ -1591,8 +1642,9 @@
       <c r="X12" s="6"/>
       <c r="Y12" s="6"/>
       <c r="Z12" s="6"/>
-    </row>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA12" s="6"/>
+    </row>
+    <row r="13" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="26" t="s">
         <v>43</v>
       </c>
@@ -1621,11 +1673,13 @@
       <c r="M13" s="22"/>
       <c r="N13" s="22"/>
       <c r="O13" s="22"/>
-      <c r="P13" s="16" t="s">
+      <c r="P13" s="22"/>
+      <c r="Q13" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="Q13" s="6"/>
-      <c r="R13" s="6"/>
+      <c r="R13" s="26" t="s">
+        <v>43</v>
+      </c>
       <c r="S13" s="6"/>
       <c r="T13" s="6"/>
       <c r="U13" s="6"/>
@@ -1634,8 +1688,9 @@
       <c r="X13" s="6"/>
       <c r="Y13" s="6"/>
       <c r="Z13" s="6"/>
-    </row>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA13" s="6"/>
+    </row>
+    <row r="14" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="26" t="s">
         <v>45</v>
       </c>
@@ -1664,11 +1719,13 @@
       <c r="M14" s="22"/>
       <c r="N14" s="22"/>
       <c r="O14" s="22"/>
-      <c r="P14" s="16" t="s">
+      <c r="P14" s="22"/>
+      <c r="Q14" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="Q14" s="6"/>
-      <c r="R14" s="6"/>
+      <c r="R14" s="26" t="s">
+        <v>45</v>
+      </c>
       <c r="S14" s="6"/>
       <c r="T14" s="6"/>
       <c r="U14" s="6"/>
@@ -1677,8 +1734,9 @@
       <c r="X14" s="6"/>
       <c r="Y14" s="6"/>
       <c r="Z14" s="6"/>
-    </row>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA14" s="6"/>
+    </row>
+    <row r="15" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="26" t="s">
         <v>46</v>
       </c>
@@ -1707,11 +1765,13 @@
       <c r="M15" s="22"/>
       <c r="N15" s="22"/>
       <c r="O15" s="22"/>
-      <c r="P15" s="16" t="s">
+      <c r="P15" s="22"/>
+      <c r="Q15" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="Q15" s="6"/>
-      <c r="R15" s="6"/>
+      <c r="R15" s="26" t="s">
+        <v>46</v>
+      </c>
       <c r="S15" s="6"/>
       <c r="T15" s="6"/>
       <c r="U15" s="6"/>
@@ -1720,8 +1780,9 @@
       <c r="X15" s="6"/>
       <c r="Y15" s="6"/>
       <c r="Z15" s="6"/>
-    </row>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA15" s="6"/>
+    </row>
+    <row r="16" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="26" t="s">
         <v>48</v>
       </c>
@@ -1750,11 +1811,13 @@
       <c r="M16" s="22"/>
       <c r="N16" s="22"/>
       <c r="O16" s="22"/>
-      <c r="P16" s="16" t="s">
+      <c r="P16" s="22"/>
+      <c r="Q16" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="Q16" s="6"/>
-      <c r="R16" s="6"/>
+      <c r="R16" s="26" t="s">
+        <v>48</v>
+      </c>
       <c r="S16" s="6"/>
       <c r="T16" s="6"/>
       <c r="U16" s="6"/>
@@ -1763,8 +1826,9 @@
       <c r="X16" s="6"/>
       <c r="Y16" s="6"/>
       <c r="Z16" s="6"/>
-    </row>
-    <row r="17" spans="2:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA16" s="6"/>
+    </row>
+    <row r="17" spans="2:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="26" t="s">
         <v>50</v>
       </c>
@@ -1793,11 +1857,13 @@
       <c r="M17" s="22"/>
       <c r="N17" s="22"/>
       <c r="O17" s="22"/>
-      <c r="P17" s="16" t="s">
+      <c r="P17" s="22"/>
+      <c r="Q17" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="Q17" s="6"/>
-      <c r="R17" s="6"/>
+      <c r="R17" s="26" t="s">
+        <v>50</v>
+      </c>
       <c r="S17" s="6"/>
       <c r="T17" s="6"/>
       <c r="U17" s="6"/>
@@ -1806,8 +1872,9 @@
       <c r="X17" s="6"/>
       <c r="Y17" s="6"/>
       <c r="Z17" s="6"/>
-    </row>
-    <row r="18" spans="2:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA17" s="6"/>
+    </row>
+    <row r="18" spans="2:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="26" t="s">
         <v>55</v>
       </c>
@@ -1836,11 +1903,13 @@
       <c r="M18" s="22"/>
       <c r="N18" s="22"/>
       <c r="O18" s="22"/>
-      <c r="P18" s="16" t="s">
+      <c r="P18" s="22"/>
+      <c r="Q18" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="Q18" s="6"/>
-      <c r="R18" s="6"/>
+      <c r="R18" s="26" t="s">
+        <v>55</v>
+      </c>
       <c r="S18" s="6"/>
       <c r="T18" s="6"/>
       <c r="U18" s="6"/>
@@ -1849,8 +1918,9 @@
       <c r="X18" s="6"/>
       <c r="Y18" s="6"/>
       <c r="Z18" s="6"/>
-    </row>
-    <row r="19" spans="2:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA18" s="6"/>
+    </row>
+    <row r="19" spans="2:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="26" t="s">
         <v>60</v>
       </c>
@@ -1879,11 +1949,13 @@
       <c r="M19" s="22"/>
       <c r="N19" s="22"/>
       <c r="O19" s="22"/>
-      <c r="P19" s="16" t="s">
+      <c r="P19" s="22"/>
+      <c r="Q19" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="Q19" s="6"/>
-      <c r="R19" s="6"/>
+      <c r="R19" s="26" t="s">
+        <v>60</v>
+      </c>
       <c r="S19" s="6"/>
       <c r="T19" s="6"/>
       <c r="U19" s="6"/>
@@ -1892,8 +1964,9 @@
       <c r="X19" s="6"/>
       <c r="Y19" s="6"/>
       <c r="Z19" s="6"/>
-    </row>
-    <row r="20" spans="2:26" ht="45" x14ac:dyDescent="0.25">
+      <c r="AA19" s="6"/>
+    </row>
+    <row r="20" spans="2:27" ht="75" x14ac:dyDescent="0.25">
       <c r="B20" s="26" t="s">
         <v>64</v>
       </c>
@@ -1922,11 +1995,13 @@
       <c r="M20" s="22"/>
       <c r="N20" s="22"/>
       <c r="O20" s="22"/>
-      <c r="P20" s="39" t="s">
+      <c r="P20" s="22"/>
+      <c r="Q20" s="39" t="s">
         <v>99</v>
       </c>
-      <c r="Q20" s="6"/>
-      <c r="R20" s="6"/>
+      <c r="R20" s="26" t="s">
+        <v>64</v>
+      </c>
       <c r="S20" s="6"/>
       <c r="T20" s="6"/>
       <c r="U20" s="6"/>
@@ -1935,8 +2010,9 @@
       <c r="X20" s="6"/>
       <c r="Y20" s="6"/>
       <c r="Z20" s="6"/>
-    </row>
-    <row r="21" spans="2:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA20" s="6"/>
+    </row>
+    <row r="21" spans="2:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="26" t="s">
         <v>68</v>
       </c>
@@ -1965,9 +2041,11 @@
       <c r="M21" s="22"/>
       <c r="N21" s="22"/>
       <c r="O21" s="22"/>
-      <c r="P21" s="20"/>
-      <c r="Q21" s="6"/>
-      <c r="R21" s="6"/>
+      <c r="P21" s="22"/>
+      <c r="Q21" s="20"/>
+      <c r="R21" s="26" t="s">
+        <v>68</v>
+      </c>
       <c r="S21" s="6"/>
       <c r="T21" s="6"/>
       <c r="U21" s="6"/>
@@ -1976,8 +2054,9 @@
       <c r="X21" s="6"/>
       <c r="Y21" s="6"/>
       <c r="Z21" s="6"/>
-    </row>
-    <row r="22" spans="2:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA21" s="6"/>
+    </row>
+    <row r="22" spans="2:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="26" t="s">
         <v>69</v>
       </c>
@@ -2006,11 +2085,13 @@
       <c r="M22" s="22"/>
       <c r="N22" s="22"/>
       <c r="O22" s="22"/>
-      <c r="P22" s="16" t="s">
+      <c r="P22" s="22"/>
+      <c r="Q22" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="Q22" s="6"/>
-      <c r="R22" s="6"/>
+      <c r="R22" s="26" t="s">
+        <v>69</v>
+      </c>
       <c r="S22" s="6"/>
       <c r="T22" s="6"/>
       <c r="U22" s="6"/>
@@ -2019,8 +2100,9 @@
       <c r="X22" s="6"/>
       <c r="Y22" s="6"/>
       <c r="Z22" s="6"/>
-    </row>
-    <row r="23" spans="2:26" s="31" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA22" s="6"/>
+    </row>
+    <row r="23" spans="2:27" s="31" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="26" t="s">
         <v>94</v>
       </c>
@@ -2049,9 +2131,11 @@
       <c r="M23" s="22"/>
       <c r="N23" s="22"/>
       <c r="O23" s="22"/>
-      <c r="P23" s="16"/>
-      <c r="Q23" s="6"/>
-      <c r="R23" s="6"/>
+      <c r="P23" s="22"/>
+      <c r="Q23" s="16"/>
+      <c r="R23" s="26" t="s">
+        <v>94</v>
+      </c>
       <c r="S23" s="6"/>
       <c r="T23" s="6"/>
       <c r="U23" s="6"/>
@@ -2060,8 +2144,9 @@
       <c r="X23" s="6"/>
       <c r="Y23" s="6"/>
       <c r="Z23" s="6"/>
-    </row>
-    <row r="24" spans="2:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA23" s="6"/>
+    </row>
+    <row r="24" spans="2:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="26" t="s">
         <v>71</v>
       </c>
@@ -2090,11 +2175,13 @@
       <c r="M24" s="22"/>
       <c r="N24" s="22"/>
       <c r="O24" s="22"/>
-      <c r="P24" s="16" t="s">
+      <c r="P24" s="22"/>
+      <c r="Q24" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="Q24" s="6"/>
-      <c r="R24" s="6"/>
+      <c r="R24" s="26" t="s">
+        <v>71</v>
+      </c>
       <c r="S24" s="6"/>
       <c r="T24" s="6"/>
       <c r="U24" s="6"/>
@@ -2103,8 +2190,9 @@
       <c r="X24" s="6"/>
       <c r="Y24" s="6"/>
       <c r="Z24" s="6"/>
-    </row>
-    <row r="25" spans="2:26" s="31" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA24" s="6"/>
+    </row>
+    <row r="25" spans="2:27" s="31" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="26" t="s">
         <v>96</v>
       </c>
@@ -2133,11 +2221,13 @@
       <c r="M25" s="22"/>
       <c r="N25" s="22"/>
       <c r="O25" s="22"/>
-      <c r="P25" s="16" t="s">
+      <c r="P25" s="22"/>
+      <c r="Q25" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="Q25" s="6"/>
-      <c r="R25" s="6"/>
+      <c r="R25" s="26" t="s">
+        <v>96</v>
+      </c>
       <c r="S25" s="6"/>
       <c r="T25" s="6"/>
       <c r="U25" s="6"/>
@@ -2146,14 +2236,15 @@
       <c r="X25" s="6"/>
       <c r="Y25" s="6"/>
       <c r="Z25" s="6"/>
-    </row>
-    <row r="26" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="2:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="AA25" s="6"/>
+    </row>
+    <row r="26" spans="2:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="2:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="2:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="2:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="2:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="2:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="2:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3125,7 +3216,7 @@
     <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B2:P2"/>
+    <mergeCell ref="B2:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -7744,7 +7835,7 @@
     <row r="20" spans="1:16" s="41" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="40"/>
       <c r="B20" s="48" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C20" s="48"/>
       <c r="D20" s="48"/>
@@ -7764,7 +7855,7 @@
     <row r="21" spans="1:16" s="41" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="40"/>
       <c r="B21" s="42" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C21" s="42"/>
       <c r="D21" s="42"/>
@@ -7783,7 +7874,7 @@
     </row>
     <row r="22" spans="1:16" s="41" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="42" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C22" s="42"/>
       <c r="D22" s="42"/>

</xml_diff>

<commit_message>
Corrected diary tests and added new ones in
</commit_message>
<xml_diff>
--- a/Data/Test Suite Prerequisites.xlsx
+++ b/Data/Test Suite Prerequisites.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\development\feature\1.5.0\gpconnect-provider-testing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62B8C3E0-2BC6-41CC-8035-10B1E9B9B5DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D006B0FC-C44E-4A68-B3C3-82F73F24D5A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Patients" sheetId="1" r:id="rId1"/>
@@ -400,16 +400,6 @@
     <t>Diary</t>
   </si>
   <si>
-    <t>x
-With Problems Associated to the Patients Diary Entry</t>
-  </si>
-  <si>
-    <t>x
-With NO Problems Associated to the Patients Diary Entry
-&amp;
-Diary Occurrence should atleast 20 days prior to current date</t>
-  </si>
-  <si>
     <t xml:space="preserve">x
 </t>
   </si>
@@ -432,6 +422,17 @@
 - Consultation that is linked to a Topic or Heading  that is linked to all supported Clinical items 
 - Consultations linked to clincal Items ( Medication,  AllergyIntollerance, Immunization &amp;  Observation) 
 - No Problems associated with Patient/Consultations/Topics/Headings or Clinical Items </t>
+  </si>
+  <si>
+    <t xml:space="preserve">x
+With NO Problems Associated to the Patients Diary Entry
+</t>
+  </si>
+  <si>
+    <t>x
+With Problems Associated to the Patients Diary Entry
+&amp;
+Diary Occurrence should be somewhere up to 180 days in the future</t>
   </si>
 </sst>
 </file>
@@ -1080,7 +1081,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P7" sqref="P7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1233,7 +1236,7 @@
         <v>113</v>
       </c>
       <c r="Q4" s="16" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="R4" s="6"/>
       <c r="S4" s="6"/>
@@ -1319,10 +1322,10 @@
         <v>26</v>
       </c>
       <c r="K6" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="L6" s="22" t="s">
         <v>116</v>
-      </c>
-      <c r="L6" s="22" t="s">
-        <v>118</v>
       </c>
       <c r="M6" s="22" t="s">
         <v>107</v>
@@ -1334,7 +1337,7 @@
         <v>26</v>
       </c>
       <c r="P6" s="22" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="Q6" s="20"/>
       <c r="R6" s="18" t="s">
@@ -1382,7 +1385,7 @@
         <v>0</v>
       </c>
       <c r="L7" s="22" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="M7" s="22" t="s">
         <v>108</v>
@@ -1394,7 +1397,7 @@
         <v>0</v>
       </c>
       <c r="P7" s="22" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="Q7" s="20"/>
       <c r="R7" s="18" t="s">

</xml_diff>

<commit_message>
fixed meds and allergies warning tests and added one for referrals
</commit_message>
<xml_diff>
--- a/Data/Test Suite Prerequisites.xlsx
+++ b/Data/Test Suite Prerequisites.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\development\feature\1.5.0\gpconnect-provider-testing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D006B0FC-C44E-4A68-B3C3-82F73F24D5A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9DBD7A5-052A-4662-805C-DF4E3989C93C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,12 +19,22 @@
     <sheet name="Practitioner" sheetId="4" r:id="rId4"/>
     <sheet name="Slots" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="122">
   <si>
     <t>Required Organizations and Slots for testing</t>
   </si>
@@ -325,10 +335,6 @@
   </si>
   <si>
     <t>Uncategorised</t>
-  </si>
-  <si>
-    <t>Patient has an AllergyIntolerance with no allergy EndReason
-Patient Has Warning Codes :  Data in Transit &amp;  Confidential Items on  Allergies</t>
   </si>
   <si>
     <t>Problems</t>
@@ -433,6 +439,16 @@
 With Problems Associated to the Patients Diary Entry
 &amp;
 Diary Occurrence should be somewhere up to 180 days in the future</t>
+  </si>
+  <si>
+    <t>Patient has an AllergyIntolerance with no allergy EndReason
+Patient Has Warning Codes : Confidential Items on  Allergies</t>
+  </si>
+  <si>
+    <t>+ Ended Allergies</t>
+  </si>
+  <si>
+    <t>Patient has Ended Allergies</t>
   </si>
 </sst>
 </file>
@@ -615,7 +631,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -736,6 +752,9 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1081,8 +1100,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q21" sqref="Q21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1218,25 +1237,25 @@
         <v>98</v>
       </c>
       <c r="K4" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="L4" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="L4" s="22" t="s">
-        <v>101</v>
-      </c>
       <c r="M4" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="N4" s="22" t="s">
         <v>103</v>
       </c>
-      <c r="N4" s="22" t="s">
-        <v>104</v>
-      </c>
       <c r="O4" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="P4" s="22" t="s">
         <v>112</v>
       </c>
-      <c r="P4" s="22" t="s">
-        <v>113</v>
-      </c>
       <c r="Q4" s="16" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="R4" s="6"/>
       <c r="S4" s="6"/>
@@ -1313,7 +1332,7 @@
         <v>26</v>
       </c>
       <c r="H6" s="14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I6" s="14" t="s">
         <v>26</v>
@@ -1322,22 +1341,22 @@
         <v>26</v>
       </c>
       <c r="K6" s="14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="L6" s="22" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M6" s="22" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="N6" s="22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="O6" s="22" t="s">
         <v>26</v>
       </c>
       <c r="P6" s="22" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="Q6" s="20"/>
       <c r="R6" s="18" t="s">
@@ -1385,19 +1404,19 @@
         <v>0</v>
       </c>
       <c r="L7" s="22" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="M7" s="22" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="N7" s="22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="O7" s="22">
         <v>0</v>
       </c>
       <c r="P7" s="22" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="Q7" s="20"/>
       <c r="R7" s="18" t="s">
@@ -1976,11 +1995,11 @@
       <c r="C20" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D20" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="E20" s="29" t="s">
-        <v>22</v>
+      <c r="D20" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="E20" s="22" t="s">
+        <v>26</v>
       </c>
       <c r="F20" s="14" t="s">
         <v>22</v>
@@ -1996,11 +2015,13 @@
       <c r="K20" s="14"/>
       <c r="L20" s="22"/>
       <c r="M20" s="22"/>
-      <c r="N20" s="22"/>
+      <c r="N20" s="22" t="s">
+        <v>26</v>
+      </c>
       <c r="O20" s="22"/>
       <c r="P20" s="22"/>
       <c r="Q20" s="39" t="s">
-        <v>99</v>
+        <v>119</v>
       </c>
       <c r="R20" s="26" t="s">
         <v>64</v>
@@ -2022,8 +2043,8 @@
       <c r="C21" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="22" t="s">
-        <v>56</v>
+      <c r="D21" s="49" t="s">
+        <v>120</v>
       </c>
       <c r="E21" s="29" t="s">
         <v>22</v>
@@ -2045,7 +2066,9 @@
       <c r="N21" s="22"/>
       <c r="O21" s="22"/>
       <c r="P21" s="22"/>
-      <c r="Q21" s="20"/>
+      <c r="Q21" s="16" t="s">
+        <v>121</v>
+      </c>
       <c r="R21" s="26" t="s">
         <v>68</v>
       </c>
@@ -7838,7 +7861,7 @@
     <row r="20" spans="1:16" s="41" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="40"/>
       <c r="B20" s="48" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C20" s="48"/>
       <c r="D20" s="48"/>
@@ -7858,7 +7881,7 @@
     <row r="21" spans="1:16" s="41" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="40"/>
       <c r="B21" s="42" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C21" s="42"/>
       <c r="D21" s="42"/>
@@ -7877,7 +7900,7 @@
     </row>
     <row r="22" spans="1:16" s="41" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="42" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C22" s="42"/>
       <c r="D22" s="42"/>

</xml_diff>

<commit_message>
added problem related to another problem test
</commit_message>
<xml_diff>
--- a/Data/Test Suite Prerequisites.xlsx
+++ b/Data/Test Suite Prerequisites.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\development\feature\1.5.0\gpconnect-provider-testing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9DBD7A5-052A-4662-805C-DF4E3989C93C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2C27F2E-C942-4B5A-B6FA-B882069F7659}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="123">
   <si>
     <t>Required Organizations and Slots for testing</t>
   </si>
@@ -449,6 +449,10 @@
   </si>
   <si>
     <t>Patient has Ended Allergies</t>
+  </si>
+  <si>
+    <t>x
+Must have a Problem related to another Problem if Supported.</t>
   </si>
 </sst>
 </file>
@@ -739,6 +743,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -752,9 +759,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1100,8 +1104,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q21" sqref="Q21"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1153,24 +1157,24 @@
       <c r="AA1" s="2"/>
     </row>
     <row r="2" spans="1:27" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
-      <c r="K2" s="45"/>
-      <c r="L2" s="45"/>
-      <c r="M2" s="45"/>
-      <c r="N2" s="45"/>
-      <c r="O2" s="45"/>
-      <c r="P2" s="45"/>
-      <c r="Q2" s="44"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="46"/>
+      <c r="L2" s="46"/>
+      <c r="M2" s="46"/>
+      <c r="N2" s="46"/>
+      <c r="O2" s="46"/>
+      <c r="P2" s="46"/>
+      <c r="Q2" s="45"/>
       <c r="R2" s="6"/>
       <c r="S2" s="6"/>
       <c r="T2" s="6"/>
@@ -1338,7 +1342,7 @@
         <v>26</v>
       </c>
       <c r="J6" s="22" t="s">
-        <v>26</v>
+        <v>122</v>
       </c>
       <c r="K6" s="14" t="s">
         <v>113</v>
@@ -1412,8 +1416,8 @@
       <c r="N7" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="O7" s="22">
-        <v>0</v>
+      <c r="O7" s="22" t="s">
+        <v>22</v>
       </c>
       <c r="P7" s="22" t="s">
         <v>117</v>
@@ -2043,7 +2047,7 @@
       <c r="C21" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="49" t="s">
+      <c r="D21" s="43" t="s">
         <v>120</v>
       </c>
       <c r="E21" s="29" t="s">
@@ -4426,18 +4430,18 @@
     </row>
     <row r="2" spans="1:21" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44"/>
-      <c r="K2" s="44"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
+      <c r="K2" s="45"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
@@ -7478,11 +7482,11 @@
     </row>
     <row r="2" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11"/>
-      <c r="B2" s="47" t="s">
+      <c r="B2" s="48" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
       <c r="E2" s="34"/>
       <c r="F2" s="34"/>
       <c r="G2" s="11"/>
@@ -7860,13 +7864,13 @@
     </row>
     <row r="20" spans="1:16" s="41" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="40"/>
-      <c r="B20" s="48" t="s">
+      <c r="B20" s="49" t="s">
         <v>108</v>
       </c>
-      <c r="C20" s="48"/>
-      <c r="D20" s="48"/>
-      <c r="E20" s="48"/>
-      <c r="F20" s="48"/>
+      <c r="C20" s="49"/>
+      <c r="D20" s="49"/>
+      <c r="E20" s="49"/>
+      <c r="F20" s="49"/>
       <c r="G20" s="40"/>
       <c r="H20" s="40"/>
       <c r="I20" s="40"/>

</xml_diff>

<commit_message>
update to problem data requirements
</commit_message>
<xml_diff>
--- a/Data/Test Suite Prerequisites.xlsx
+++ b/Data/Test Suite Prerequisites.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\development\feature\1.5.0\gpconnect-provider-testing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2C27F2E-C942-4B5A-B6FA-B882069F7659}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3575D8D4-AD90-47BB-A91A-549D47408366}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -452,7 +452,7 @@
   </si>
   <si>
     <t>x
-Must have a Problem related to another Problem if Supported.</t>
+Must have a Problem related to another Problem(Parent-Child or Parent-Sibling) if Supported.</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
added in checks for no problems list and resources to all structured tests
</commit_message>
<xml_diff>
--- a/Data/Test Suite Prerequisites.xlsx
+++ b/Data/Test Suite Prerequisites.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\development\feature\1.5.0\gpconnect-provider-testing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3575D8D4-AD90-47BB-A91A-549D47408366}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6107B2A4-AABA-476C-97B0-AAF345C78E91}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="123">
   <si>
     <t>Required Organizations and Slots for testing</t>
   </si>
@@ -1104,8 +1104,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="G1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1518,7 +1519,9 @@
       </c>
       <c r="I9" s="14"/>
       <c r="J9" s="22"/>
-      <c r="K9" s="14"/>
+      <c r="K9" s="14">
+        <v>0</v>
+      </c>
       <c r="L9" s="22"/>
       <c r="M9" s="22"/>
       <c r="N9" s="22"/>
@@ -1562,7 +1565,9 @@
       </c>
       <c r="I10" s="14"/>
       <c r="J10" s="22"/>
-      <c r="K10" s="14"/>
+      <c r="K10" s="14">
+        <v>0</v>
+      </c>
       <c r="L10" s="22"/>
       <c r="M10" s="22"/>
       <c r="N10" s="22"/>
@@ -1606,7 +1611,9 @@
       </c>
       <c r="I11" s="14"/>
       <c r="J11" s="22"/>
-      <c r="K11" s="14"/>
+      <c r="K11" s="14">
+        <v>0</v>
+      </c>
       <c r="L11" s="22"/>
       <c r="M11" s="22"/>
       <c r="N11" s="22"/>
@@ -1650,7 +1657,9 @@
       </c>
       <c r="I12" s="14"/>
       <c r="J12" s="22"/>
-      <c r="K12" s="14"/>
+      <c r="K12" s="14">
+        <v>0</v>
+      </c>
       <c r="L12" s="22"/>
       <c r="M12" s="22"/>
       <c r="N12" s="22"/>
@@ -1694,7 +1703,9 @@
       </c>
       <c r="I13" s="14"/>
       <c r="J13" s="22"/>
-      <c r="K13" s="14"/>
+      <c r="K13" s="14" t="s">
+        <v>22</v>
+      </c>
       <c r="L13" s="22"/>
       <c r="M13" s="22"/>
       <c r="N13" s="22"/>
@@ -1740,7 +1751,9 @@
       </c>
       <c r="I14" s="14"/>
       <c r="J14" s="22"/>
-      <c r="K14" s="14"/>
+      <c r="K14" s="14" t="s">
+        <v>22</v>
+      </c>
       <c r="L14" s="22"/>
       <c r="M14" s="22"/>
       <c r="N14" s="22"/>
@@ -1786,7 +1799,9 @@
       </c>
       <c r="I15" s="14"/>
       <c r="J15" s="22"/>
-      <c r="K15" s="14"/>
+      <c r="K15" s="14" t="s">
+        <v>22</v>
+      </c>
       <c r="L15" s="22"/>
       <c r="M15" s="22"/>
       <c r="N15" s="22"/>
@@ -1832,7 +1847,9 @@
       </c>
       <c r="I16" s="14"/>
       <c r="J16" s="22"/>
-      <c r="K16" s="14"/>
+      <c r="K16" s="14">
+        <v>0</v>
+      </c>
       <c r="L16" s="22"/>
       <c r="M16" s="22"/>
       <c r="N16" s="22"/>
@@ -1878,7 +1895,9 @@
       </c>
       <c r="I17" s="14"/>
       <c r="J17" s="22"/>
-      <c r="K17" s="14"/>
+      <c r="K17" s="14">
+        <v>0</v>
+      </c>
       <c r="L17" s="22"/>
       <c r="M17" s="22"/>
       <c r="N17" s="22"/>
@@ -1924,7 +1943,9 @@
       </c>
       <c r="I18" s="14"/>
       <c r="J18" s="22"/>
-      <c r="K18" s="14"/>
+      <c r="K18" s="14" t="s">
+        <v>22</v>
+      </c>
       <c r="L18" s="22"/>
       <c r="M18" s="22"/>
       <c r="N18" s="22"/>
@@ -1970,7 +1991,9 @@
       </c>
       <c r="I19" s="14"/>
       <c r="J19" s="22"/>
-      <c r="K19" s="14"/>
+      <c r="K19" s="14" t="s">
+        <v>22</v>
+      </c>
       <c r="L19" s="22"/>
       <c r="M19" s="22"/>
       <c r="N19" s="22"/>
@@ -2016,7 +2039,9 @@
       </c>
       <c r="I20" s="14"/>
       <c r="J20" s="22"/>
-      <c r="K20" s="14"/>
+      <c r="K20" s="14">
+        <v>0</v>
+      </c>
       <c r="L20" s="22"/>
       <c r="M20" s="22"/>
       <c r="N20" s="22" t="s">
@@ -2064,7 +2089,9 @@
       </c>
       <c r="I21" s="14"/>
       <c r="J21" s="22"/>
-      <c r="K21" s="14"/>
+      <c r="K21" s="14" t="s">
+        <v>22</v>
+      </c>
       <c r="L21" s="22"/>
       <c r="M21" s="22"/>
       <c r="N21" s="22"/>
@@ -2110,7 +2137,9 @@
       </c>
       <c r="I22" s="14"/>
       <c r="J22" s="22"/>
-      <c r="K22" s="14"/>
+      <c r="K22" s="14" t="s">
+        <v>22</v>
+      </c>
       <c r="L22" s="22"/>
       <c r="M22" s="22"/>
       <c r="N22" s="22"/>
@@ -2156,7 +2185,9 @@
       </c>
       <c r="I23" s="14"/>
       <c r="J23" s="22"/>
-      <c r="K23" s="14"/>
+      <c r="K23" s="14" t="s">
+        <v>22</v>
+      </c>
       <c r="L23" s="22"/>
       <c r="M23" s="22"/>
       <c r="N23" s="22"/>
@@ -2200,7 +2231,9 @@
       </c>
       <c r="I24" s="14"/>
       <c r="J24" s="22"/>
-      <c r="K24" s="14"/>
+      <c r="K24" s="14" t="s">
+        <v>22</v>
+      </c>
       <c r="L24" s="22"/>
       <c r="M24" s="22"/>
       <c r="N24" s="22"/>
@@ -2246,7 +2279,9 @@
       </c>
       <c r="I25" s="14"/>
       <c r="J25" s="22"/>
-      <c r="K25" s="14"/>
+      <c r="K25" s="14" t="s">
+        <v>22</v>
+      </c>
       <c r="L25" s="22"/>
       <c r="M25" s="22"/>
       <c r="N25" s="22"/>

</xml_diff>

<commit_message>
updated data requirements sheet after some issues raised by emis
</commit_message>
<xml_diff>
--- a/Data/Test Suite Prerequisites.xlsx
+++ b/Data/Test Suite Prerequisites.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\development\feature\1.5.0\gpconnect-provider-testing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6107B2A4-AABA-476C-97B0-AAF345C78E91}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4998C70E-8037-4E63-8865-B686D39AC100}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1020" yWindow="465" windowWidth="28770" windowHeight="15570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Patients" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="123">
   <si>
     <t>Required Organizations and Slots for testing</t>
   </si>
@@ -120,9 +120,6 @@
     <t>x</t>
   </si>
   <si>
-    <t>4(Explicit "Confidential items" warning code)</t>
-  </si>
-  <si>
     <t>ManagingOrg</t>
   </si>
   <si>
@@ -205,9 +202,6 @@
   </si>
   <si>
     <t>Patient 14</t>
-  </si>
-  <si>
-    <t>1 (Explicit "Confidential items" warning code)</t>
   </si>
   <si>
     <t>Location 4</t>
@@ -445,14 +439,20 @@
 Patient Has Warning Codes : Confidential Items on  Allergies</t>
   </si>
   <si>
-    <t>+ Ended Allergies</t>
-  </si>
-  <si>
     <t>Patient has Ended Allergies</t>
   </si>
   <si>
     <t>x
 Must have a Problem related to another Problem(Parent-Child or Parent-Sibling) if Supported.</t>
+  </si>
+  <si>
+    <t>(Requires Allergies and atleast One Allergy that has Explicit "Confidential items" warning code)</t>
+  </si>
+  <si>
+    <t>(Requires Allergies with atleast one that is Ended)</t>
+  </si>
+  <si>
+    <t>(Requires Meds and one with Explicit "Confidential items" warning code)</t>
   </si>
 </sst>
 </file>
@@ -576,7 +576,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -631,11 +631,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -746,11 +783,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -759,6 +792,15 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1105,8 +1147,8 @@
   <dimension ref="A1:AA1001"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="G1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L9" sqref="L9"/>
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1128,7 +1170,7 @@
     <col min="19" max="27" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -1157,25 +1199,25 @@
       <c r="Z1" s="2"/>
       <c r="AA1" s="2"/>
     </row>
-    <row r="2" spans="1:27" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="44" t="s">
+    <row r="2" spans="1:27" ht="72.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
-      <c r="K2" s="46"/>
-      <c r="L2" s="46"/>
-      <c r="M2" s="46"/>
-      <c r="N2" s="46"/>
-      <c r="O2" s="46"/>
-      <c r="P2" s="46"/>
-      <c r="Q2" s="45"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="49"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="49"/>
+      <c r="O2" s="49"/>
+      <c r="P2" s="49"/>
+      <c r="Q2" s="50"/>
       <c r="R2" s="6"/>
       <c r="S2" s="6"/>
       <c r="T2" s="6"/>
@@ -1236,31 +1278,31 @@
         <v>15</v>
       </c>
       <c r="I4" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="J4" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="K4" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="J4" s="22" t="s">
+      <c r="L4" s="22" t="s">
         <v>98</v>
       </c>
-      <c r="K4" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="L4" s="22" t="s">
+      <c r="M4" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="M4" s="22" t="s">
-        <v>102</v>
-      </c>
       <c r="N4" s="22" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="O4" s="22" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="P4" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q4" s="16" t="s">
         <v>112</v>
-      </c>
-      <c r="Q4" s="16" t="s">
-        <v>114</v>
       </c>
       <c r="R4" s="6"/>
       <c r="S4" s="6"/>
@@ -1331,37 +1373,37 @@
         <v>26</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>27</v>
+        <v>122</v>
       </c>
       <c r="G6" s="14" t="s">
         <v>26</v>
       </c>
       <c r="H6" s="14" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="I6" s="14" t="s">
         <v>26</v>
       </c>
       <c r="J6" s="22" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="K6" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="L6" s="22" t="s">
         <v>113</v>
       </c>
-      <c r="L6" s="22" t="s">
-        <v>115</v>
-      </c>
       <c r="M6" s="22" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="N6" s="22" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="O6" s="22" t="s">
         <v>26</v>
       </c>
       <c r="P6" s="22" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="Q6" s="20"/>
       <c r="R6" s="18" t="s">
@@ -1379,7 +1421,7 @@
     </row>
     <row r="7" spans="1:27" ht="150" x14ac:dyDescent="0.25">
       <c r="B7" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C7" s="14" t="s">
         <v>22</v>
@@ -1409,23 +1451,23 @@
         <v>0</v>
       </c>
       <c r="L7" s="22" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="M7" s="22" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="N7" s="22" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="O7" s="22" t="s">
         <v>22</v>
       </c>
       <c r="P7" s="22" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="Q7" s="20"/>
       <c r="R7" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="S7" s="6"/>
       <c r="T7" s="6"/>
@@ -1439,7 +1481,7 @@
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B8" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C8" s="14" t="s">
         <v>22</v>
@@ -1477,13 +1519,15 @@
       <c r="N8" s="22">
         <v>0</v>
       </c>
-      <c r="O8" s="22"/>
+      <c r="O8" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="P8" s="22">
         <v>0</v>
       </c>
       <c r="Q8" s="20"/>
       <c r="R8" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="S8" s="6"/>
       <c r="T8" s="6"/>
@@ -1497,13 +1541,13 @@
     </row>
     <row r="9" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="15" t="s">
         <v>37</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>38</v>
       </c>
       <c r="E9" s="15">
         <v>0</v>
@@ -1517,19 +1561,33 @@
       <c r="H9" s="14">
         <v>0</v>
       </c>
-      <c r="I9" s="14"/>
-      <c r="J9" s="22"/>
+      <c r="I9" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J9" s="14" t="s">
+        <v>22</v>
+      </c>
       <c r="K9" s="14">
         <v>0</v>
       </c>
-      <c r="L9" s="22"/>
-      <c r="M9" s="22"/>
-      <c r="N9" s="22"/>
-      <c r="O9" s="22"/>
-      <c r="P9" s="22"/>
+      <c r="L9" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="M9" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="N9" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="O9" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="P9" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="Q9" s="20"/>
       <c r="R9" s="18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="S9" s="6"/>
       <c r="T9" s="6"/>
@@ -1543,7 +1601,7 @@
     </row>
     <row r="10" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C10" s="14" t="s">
         <v>22</v>
@@ -1563,19 +1621,33 @@
       <c r="H10" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="I10" s="14"/>
-      <c r="J10" s="22"/>
+      <c r="I10" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J10" s="14" t="s">
+        <v>22</v>
+      </c>
       <c r="K10" s="14">
         <v>0</v>
       </c>
-      <c r="L10" s="22"/>
-      <c r="M10" s="22"/>
-      <c r="N10" s="22"/>
-      <c r="O10" s="22"/>
-      <c r="P10" s="22"/>
+      <c r="L10" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="M10" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="N10" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="O10" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="P10" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="Q10" s="20"/>
       <c r="R10" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="S10" s="6"/>
       <c r="T10" s="6"/>
@@ -1589,7 +1661,7 @@
     </row>
     <row r="11" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C11" s="14" t="s">
         <v>22</v>
@@ -1609,19 +1681,33 @@
       <c r="H11" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="I11" s="14"/>
-      <c r="J11" s="22"/>
+      <c r="I11" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J11" s="14" t="s">
+        <v>22</v>
+      </c>
       <c r="K11" s="14">
         <v>0</v>
       </c>
-      <c r="L11" s="22"/>
-      <c r="M11" s="22"/>
-      <c r="N11" s="22"/>
-      <c r="O11" s="22"/>
-      <c r="P11" s="22"/>
+      <c r="L11" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="M11" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="N11" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="O11" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="P11" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="Q11" s="20"/>
       <c r="R11" s="18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="S11" s="6"/>
       <c r="T11" s="6"/>
@@ -1635,7 +1721,7 @@
     </row>
     <row r="12" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C12" s="14" t="s">
         <v>22</v>
@@ -1655,19 +1741,33 @@
       <c r="H12" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="I12" s="14"/>
-      <c r="J12" s="22"/>
+      <c r="I12" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J12" s="14" t="s">
+        <v>22</v>
+      </c>
       <c r="K12" s="14">
         <v>0</v>
       </c>
-      <c r="L12" s="22"/>
-      <c r="M12" s="22"/>
-      <c r="N12" s="22"/>
-      <c r="O12" s="22"/>
-      <c r="P12" s="22"/>
+      <c r="L12" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="M12" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="N12" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="O12" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="P12" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="Q12" s="20"/>
       <c r="R12" s="18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="S12" s="6"/>
       <c r="T12" s="6"/>
@@ -1681,7 +1781,7 @@
     </row>
     <row r="13" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C13" s="14" t="s">
         <v>22</v>
@@ -1701,21 +1801,35 @@
       <c r="H13" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="I13" s="14"/>
-      <c r="J13" s="22"/>
+      <c r="I13" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J13" s="14" t="s">
+        <v>22</v>
+      </c>
       <c r="K13" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="L13" s="22"/>
-      <c r="M13" s="22"/>
-      <c r="N13" s="22"/>
-      <c r="O13" s="22"/>
-      <c r="P13" s="22"/>
+      <c r="L13" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="M13" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="N13" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="O13" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="P13" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="Q13" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="R13" s="26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="S13" s="6"/>
       <c r="T13" s="6"/>
@@ -1729,7 +1843,7 @@
     </row>
     <row r="14" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="26" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C14" s="14" t="s">
         <v>22</v>
@@ -1749,21 +1863,35 @@
       <c r="H14" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="I14" s="14"/>
-      <c r="J14" s="22"/>
+      <c r="I14" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J14" s="14" t="s">
+        <v>22</v>
+      </c>
       <c r="K14" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="L14" s="22"/>
-      <c r="M14" s="22"/>
-      <c r="N14" s="22"/>
-      <c r="O14" s="22"/>
-      <c r="P14" s="22"/>
+      <c r="L14" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="M14" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="N14" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="O14" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="P14" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="Q14" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="R14" s="26" t="s">
         <v>44</v>
-      </c>
-      <c r="R14" s="26" t="s">
-        <v>45</v>
       </c>
       <c r="S14" s="6"/>
       <c r="T14" s="6"/>
@@ -1777,7 +1905,7 @@
     </row>
     <row r="15" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C15" s="14" t="s">
         <v>22</v>
@@ -1797,21 +1925,35 @@
       <c r="H15" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="I15" s="14"/>
-      <c r="J15" s="22"/>
+      <c r="I15" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J15" s="14" t="s">
+        <v>22</v>
+      </c>
       <c r="K15" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="L15" s="22"/>
-      <c r="M15" s="22"/>
-      <c r="N15" s="22"/>
-      <c r="O15" s="22"/>
-      <c r="P15" s="22"/>
+      <c r="L15" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="M15" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="N15" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="O15" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="P15" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="Q15" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="R15" s="26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="S15" s="6"/>
       <c r="T15" s="6"/>
@@ -1825,7 +1967,7 @@
     </row>
     <row r="16" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="26" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C16" s="14" t="s">
         <v>22</v>
@@ -1845,21 +1987,35 @@
       <c r="H16" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="I16" s="14"/>
-      <c r="J16" s="22"/>
+      <c r="I16" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J16" s="14" t="s">
+        <v>22</v>
+      </c>
       <c r="K16" s="14">
         <v>0</v>
       </c>
-      <c r="L16" s="22"/>
-      <c r="M16" s="22"/>
-      <c r="N16" s="22"/>
-      <c r="O16" s="22"/>
-      <c r="P16" s="22"/>
+      <c r="L16" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="M16" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="N16" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="O16" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="P16" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="Q16" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="R16" s="26" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="S16" s="6"/>
       <c r="T16" s="6"/>
@@ -1873,7 +2029,7 @@
     </row>
     <row r="17" spans="2:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="26" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C17" s="14" t="s">
         <v>22</v>
@@ -1893,21 +2049,35 @@
       <c r="H17" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="I17" s="14"/>
-      <c r="J17" s="22"/>
+      <c r="I17" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J17" s="14" t="s">
+        <v>22</v>
+      </c>
       <c r="K17" s="14">
         <v>0</v>
       </c>
-      <c r="L17" s="22"/>
-      <c r="M17" s="22"/>
-      <c r="N17" s="22"/>
-      <c r="O17" s="22"/>
-      <c r="P17" s="22"/>
+      <c r="L17" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="M17" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="N17" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="O17" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="P17" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="Q17" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="R17" s="26" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="S17" s="6"/>
       <c r="T17" s="6"/>
@@ -1921,7 +2091,7 @@
     </row>
     <row r="18" spans="2:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C18" s="14" t="s">
         <v>22</v>
@@ -1941,21 +2111,35 @@
       <c r="H18" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="I18" s="14"/>
-      <c r="J18" s="22"/>
+      <c r="I18" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J18" s="14" t="s">
+        <v>22</v>
+      </c>
       <c r="K18" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="L18" s="22"/>
-      <c r="M18" s="22"/>
-      <c r="N18" s="22"/>
-      <c r="O18" s="22"/>
-      <c r="P18" s="22"/>
+      <c r="L18" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="M18" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="N18" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="O18" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="P18" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="Q18" s="16" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="R18" s="26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="S18" s="6"/>
       <c r="T18" s="6"/>
@@ -1969,7 +2153,7 @@
     </row>
     <row r="19" spans="2:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="26" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C19" s="14" t="s">
         <v>22</v>
@@ -1989,21 +2173,35 @@
       <c r="H19" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="I19" s="14"/>
-      <c r="J19" s="22"/>
+      <c r="I19" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J19" s="14" t="s">
+        <v>22</v>
+      </c>
       <c r="K19" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="L19" s="22"/>
-      <c r="M19" s="22"/>
-      <c r="N19" s="22"/>
-      <c r="O19" s="22"/>
-      <c r="P19" s="22"/>
+      <c r="L19" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="M19" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="N19" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="O19" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="P19" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="Q19" s="16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="R19" s="26" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="S19" s="6"/>
       <c r="T19" s="6"/>
@@ -2017,13 +2215,13 @@
     </row>
     <row r="20" spans="2:27" ht="75" x14ac:dyDescent="0.25">
       <c r="B20" s="26" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C20" s="14" t="s">
         <v>22</v>
       </c>
       <c r="D20" s="22" t="s">
-        <v>56</v>
+        <v>120</v>
       </c>
       <c r="E20" s="22" t="s">
         <v>26</v>
@@ -2037,23 +2235,35 @@
       <c r="H20" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="I20" s="14"/>
-      <c r="J20" s="22"/>
+      <c r="I20" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J20" s="14" t="s">
+        <v>22</v>
+      </c>
       <c r="K20" s="14">
         <v>0</v>
       </c>
-      <c r="L20" s="22"/>
-      <c r="M20" s="22"/>
+      <c r="L20" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="M20" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="N20" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="O20" s="22"/>
-      <c r="P20" s="22"/>
+      <c r="O20" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="P20" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="Q20" s="39" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="R20" s="26" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="S20" s="6"/>
       <c r="T20" s="6"/>
@@ -2065,15 +2275,15 @@
       <c r="Z20" s="6"/>
       <c r="AA20" s="6"/>
     </row>
-    <row r="21" spans="2:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B21" s="26" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C21" s="14" t="s">
         <v>22</v>
       </c>
       <c r="D21" s="43" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E21" s="29" t="s">
         <v>22</v>
@@ -2087,21 +2297,35 @@
       <c r="H21" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="I21" s="14"/>
-      <c r="J21" s="22"/>
+      <c r="I21" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J21" s="14" t="s">
+        <v>22</v>
+      </c>
       <c r="K21" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="L21" s="22"/>
-      <c r="M21" s="22"/>
-      <c r="N21" s="22"/>
-      <c r="O21" s="22"/>
-      <c r="P21" s="22"/>
+      <c r="L21" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="M21" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="N21" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="O21" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="P21" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="Q21" s="16" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="R21" s="26" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="S21" s="6"/>
       <c r="T21" s="6"/>
@@ -2115,7 +2339,7 @@
     </row>
     <row r="22" spans="2:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="26" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C22" s="14" t="s">
         <v>22</v>
@@ -2135,21 +2359,35 @@
       <c r="H22" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="I22" s="14"/>
-      <c r="J22" s="22"/>
+      <c r="I22" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J22" s="14" t="s">
+        <v>22</v>
+      </c>
       <c r="K22" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="L22" s="22"/>
-      <c r="M22" s="22"/>
-      <c r="N22" s="22"/>
-      <c r="O22" s="22"/>
-      <c r="P22" s="22"/>
+      <c r="L22" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="M22" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="N22" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="O22" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="P22" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="Q22" s="16" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="R22" s="26" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="S22" s="6"/>
       <c r="T22" s="6"/>
@@ -2163,7 +2401,7 @@
     </row>
     <row r="23" spans="2:27" s="31" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="26" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C23" s="14" t="s">
         <v>22</v>
@@ -2183,19 +2421,33 @@
       <c r="H23" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="I23" s="14"/>
-      <c r="J23" s="22"/>
+      <c r="I23" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J23" s="14" t="s">
+        <v>22</v>
+      </c>
       <c r="K23" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="L23" s="22"/>
-      <c r="M23" s="22"/>
-      <c r="N23" s="22"/>
-      <c r="O23" s="22"/>
-      <c r="P23" s="22"/>
+      <c r="L23" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="M23" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="N23" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="O23" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="P23" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="Q23" s="16"/>
       <c r="R23" s="26" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="S23" s="6"/>
       <c r="T23" s="6"/>
@@ -2209,41 +2461,55 @@
     </row>
     <row r="24" spans="2:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="E24" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="F24" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G24" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="H24" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="I24" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J24" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="K24" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="L24" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="M24" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="N24" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="O24" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="P24" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q24" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="C24" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="D24" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="E24" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="F24" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="G24" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="H24" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="I24" s="14"/>
-      <c r="J24" s="22"/>
-      <c r="K24" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="L24" s="22"/>
-      <c r="M24" s="22"/>
-      <c r="N24" s="22"/>
-      <c r="O24" s="22"/>
-      <c r="P24" s="22"/>
-      <c r="Q24" s="16" t="s">
-        <v>73</v>
-      </c>
       <c r="R24" s="26" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="S24" s="6"/>
       <c r="T24" s="6"/>
@@ -2257,7 +2523,7 @@
     </row>
     <row r="25" spans="2:27" s="31" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="26" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C25" s="14" t="s">
         <v>22</v>
@@ -2277,21 +2543,35 @@
       <c r="H25" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="I25" s="14"/>
-      <c r="J25" s="22"/>
+      <c r="I25" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J25" s="14" t="s">
+        <v>22</v>
+      </c>
       <c r="K25" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="L25" s="22"/>
-      <c r="M25" s="22"/>
-      <c r="N25" s="22"/>
-      <c r="O25" s="22"/>
-      <c r="P25" s="22"/>
+      <c r="L25" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="M25" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="N25" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="O25" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="P25" s="22" t="s">
+        <v>22</v>
+      </c>
       <c r="Q25" s="16" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="R25" s="26" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="S25" s="6"/>
       <c r="T25" s="6"/>
@@ -4465,18 +4745,18 @@
     </row>
     <row r="2" spans="1:21" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="47" t="s">
+      <c r="B2" s="45" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
-      <c r="K2" s="45"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="44"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
@@ -4521,22 +4801,22 @@
         <v>24</v>
       </c>
       <c r="E4" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="21" t="s">
+      <c r="G4" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="G4" s="21" t="s">
+      <c r="H4" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="H4" s="19" t="s">
+      <c r="I4" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="I4" s="21" t="s">
+      <c r="J4" s="19" t="s">
         <v>32</v>
-      </c>
-      <c r="J4" s="19" t="s">
-        <v>33</v>
       </c>
       <c r="K4" s="23" t="s">
         <v>19</v>
@@ -4555,10 +4835,10 @@
     <row r="5" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="24" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D5" s="27" t="s">
         <v>22</v>
@@ -4596,10 +4876,10 @@
     <row r="6" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="25" t="s">
         <v>51</v>
-      </c>
-      <c r="C6" s="25" t="s">
-        <v>52</v>
       </c>
       <c r="D6" s="27" t="s">
         <v>22</v>
@@ -4637,10 +4917,10 @@
     <row r="7" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D7" s="27" t="s">
         <v>22</v>
@@ -4678,10 +4958,10 @@
     <row r="8" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="24" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D8" s="27" t="s">
         <v>22</v>
@@ -4719,10 +4999,10 @@
     <row r="9" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="24" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D9" s="27" t="s">
         <v>22</v>
@@ -4760,10 +5040,10 @@
     <row r="10" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="24" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D10" s="27" t="s">
         <v>22</v>
@@ -4801,10 +5081,10 @@
     <row r="11" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="24" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D11" s="27" t="s">
         <v>22</v>
@@ -4842,10 +5122,10 @@
     <row r="12" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="24" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D12" s="27" t="s">
         <v>22</v>
@@ -4883,10 +5163,10 @@
     <row r="13" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="30" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D13" s="27" t="s">
         <v>22</v>
@@ -4924,10 +5204,10 @@
     <row r="14" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="30" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D14" s="27" t="s">
         <v>22</v>
@@ -4965,10 +5245,10 @@
     <row r="15" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="30" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D15" s="27" t="s">
         <v>22</v>
@@ -6164,7 +6444,7 @@
     <row r="2" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="31"/>
       <c r="B2" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
@@ -6181,7 +6461,7 @@
     <row r="3" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="31"/>
       <c r="B3" s="33" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C3" s="33"/>
       <c r="D3" s="33"/>
@@ -6213,10 +6493,10 @@
     <row r="5" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="31"/>
       <c r="B5" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D5" s="31"/>
       <c r="E5" s="31"/>
@@ -6232,7 +6512,7 @@
     <row r="6" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="31"/>
       <c r="B6" s="7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C6" s="34">
         <v>0</v>
@@ -6251,7 +6531,7 @@
     <row r="7" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="31"/>
       <c r="B7" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C7" s="34">
         <v>1</v>
@@ -6270,7 +6550,7 @@
     <row r="8" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="31"/>
       <c r="B8" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C8" s="34">
         <v>2</v>
@@ -6289,7 +6569,7 @@
     <row r="9" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="31"/>
       <c r="B9" s="7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C9" s="34">
         <v>1</v>
@@ -6323,7 +6603,7 @@
     <row r="11" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="31"/>
       <c r="B11" s="9" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C11" s="33"/>
       <c r="D11" s="31"/>
@@ -6340,7 +6620,7 @@
     <row r="12" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="31"/>
       <c r="B12" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="31"/>
@@ -7517,11 +7797,11 @@
     </row>
     <row r="2" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11"/>
-      <c r="B2" s="48" t="s">
-        <v>76</v>
-      </c>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
+      <c r="B2" s="46" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
       <c r="E2" s="34"/>
       <c r="F2" s="34"/>
       <c r="G2" s="11"/>
@@ -7559,13 +7839,13 @@
         <v>4</v>
       </c>
       <c r="C4" s="35" t="s">
+        <v>84</v>
+      </c>
+      <c r="D4" s="35" t="s">
+        <v>85</v>
+      </c>
+      <c r="E4" s="35" t="s">
         <v>86</v>
-      </c>
-      <c r="D4" s="35" t="s">
-        <v>87</v>
-      </c>
-      <c r="E4" s="35" t="s">
-        <v>88</v>
       </c>
       <c r="F4" s="35" t="s">
         <v>19</v>
@@ -7593,7 +7873,7 @@
         <v>0.44097222222222199</v>
       </c>
       <c r="E5" s="37" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F5" s="37"/>
       <c r="G5" s="11"/>
@@ -7619,7 +7899,7 @@
         <v>0.52777777777777801</v>
       </c>
       <c r="E6" s="37" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F6" s="37"/>
       <c r="G6" s="11"/>
@@ -7645,10 +7925,10 @@
         <v>0.52777777777777801</v>
       </c>
       <c r="E7" s="37" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F7" s="37" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
@@ -7700,7 +7980,7 @@
     <row r="10" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11"/>
       <c r="B10" s="38" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C10" s="34"/>
       <c r="D10" s="34"/>
@@ -7738,7 +8018,7 @@
     <row r="12" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11"/>
       <c r="B12" s="34" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C12" s="34"/>
       <c r="D12" s="34"/>
@@ -7779,7 +8059,7 @@
         <v>4</v>
       </c>
       <c r="C14" s="35" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D14" s="34"/>
       <c r="E14" s="34"/>
@@ -7899,13 +8179,13 @@
     </row>
     <row r="20" spans="1:16" s="41" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="40"/>
-      <c r="B20" s="49" t="s">
-        <v>108</v>
-      </c>
-      <c r="C20" s="49"/>
-      <c r="D20" s="49"/>
-      <c r="E20" s="49"/>
-      <c r="F20" s="49"/>
+      <c r="B20" s="47" t="s">
+        <v>106</v>
+      </c>
+      <c r="C20" s="47"/>
+      <c r="D20" s="47"/>
+      <c r="E20" s="47"/>
+      <c r="F20" s="47"/>
       <c r="G20" s="40"/>
       <c r="H20" s="40"/>
       <c r="I20" s="40"/>
@@ -7920,7 +8200,7 @@
     <row r="21" spans="1:16" s="41" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="40"/>
       <c r="B21" s="42" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C21" s="42"/>
       <c r="D21" s="42"/>
@@ -7939,7 +8219,7 @@
     </row>
     <row r="22" spans="1:16" s="41" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="42" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C22" s="42"/>
       <c r="D22" s="42"/>

</xml_diff>

<commit_message>
Updated consultations to remove test with  no problems
</commit_message>
<xml_diff>
--- a/Data/Test Suite Prerequisites.xlsx
+++ b/Data/Test Suite Prerequisites.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\development\feature\1.5.0\gpconnect-provider-testing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4998C70E-8037-4E63-8865-B686D39AC100}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4973EFC-D5F2-4090-839D-F6CFA4B89F27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="465" windowWidth="28770" windowHeight="15570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30" yWindow="390" windowWidth="28770" windowHeight="15570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Patients" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="122">
   <si>
     <t>Required Organizations and Slots for testing</t>
   </si>
@@ -407,52 +407,45 @@
     <t>Other Requirements / Comments</t>
   </si>
   <si>
+    <t xml:space="preserve">x
+With NO Problems Associated to the Patients Diary Entry
+</t>
+  </si>
+  <si>
     <t>x
+With Problems Associated to the Patients Diary Entry
+&amp;
+Diary Occurrence should be somewhere up to 180 days in the future</t>
+  </si>
+  <si>
+    <t>Patient has an AllergyIntolerance with no allergy EndReason
+Patient Has Warning Codes : Confidential Items on  Allergies</t>
+  </si>
+  <si>
+    <t>Patient has Ended Allergies</t>
+  </si>
+  <si>
+    <t>x
+Must have a Problem related to another Problem(Parent-Child or Parent-Sibling) if Supported.</t>
+  </si>
+  <si>
+    <t>(Requires Allergies and atleast One Allergy that has Explicit "Confidential items" warning code)</t>
+  </si>
+  <si>
+    <t>(Requires Allergies with atleast one that is Ended)</t>
+  </si>
+  <si>
+    <t>(Requires Meds and one with Explicit "Confidential items" warning code)</t>
+  </si>
+  <si>
+    <t>x
+-- UNDER REVIEW --
 - Consultation that is linked to only clinical items
 - Consultation That is only Linked to A topic that is only linked to clinical items (no heading)
 - Consultation that is linked to a Topic or Heading  that is linked to all supported Clinical items 
 - Consultation that is linked to a topic that is linked to a problem
 - Consultation linked to a problem but not linked to a topic or heading
 -  A Consultation linked to a problem linked and to a Medication,  AllergyIntollerance, Immunization &amp;  Observation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">x
-- Consultation that is linked to only clinical items 
- - Consultation That is only Linked to A topic that is only linked to clinical items (no heading)
-- Consultation that is linked to a Topic or Heading  that is linked to all supported Clinical items 
-- Consultations linked to clincal Items ( Medication,  AllergyIntollerance, Immunization &amp;  Observation) 
-- No Problems associated with Patient/Consultations/Topics/Headings or Clinical Items </t>
-  </si>
-  <si>
-    <t xml:space="preserve">x
-With NO Problems Associated to the Patients Diary Entry
-</t>
-  </si>
-  <si>
-    <t>x
-With Problems Associated to the Patients Diary Entry
-&amp;
-Diary Occurrence should be somewhere up to 180 days in the future</t>
-  </si>
-  <si>
-    <t>Patient has an AllergyIntolerance with no allergy EndReason
-Patient Has Warning Codes : Confidential Items on  Allergies</t>
-  </si>
-  <si>
-    <t>Patient has Ended Allergies</t>
-  </si>
-  <si>
-    <t>x
-Must have a Problem related to another Problem(Parent-Child or Parent-Sibling) if Supported.</t>
-  </si>
-  <si>
-    <t>(Requires Allergies and atleast One Allergy that has Explicit "Confidential items" warning code)</t>
-  </si>
-  <si>
-    <t>(Requires Allergies with atleast one that is Ended)</t>
-  </si>
-  <si>
-    <t>(Requires Meds and one with Explicit "Confidential items" warning code)</t>
   </si>
 </sst>
 </file>
@@ -783,16 +776,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -801,6 +784,16 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1147,8 +1140,8 @@
   <dimension ref="A1:AA1001"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight"/>
+      <pane xSplit="2" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1200,24 +1193,24 @@
       <c r="AA1" s="2"/>
     </row>
     <row r="2" spans="1:27" ht="72.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="48" t="s">
+      <c r="B2" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="49"/>
-      <c r="L2" s="49"/>
-      <c r="M2" s="49"/>
-      <c r="N2" s="49"/>
-      <c r="O2" s="49"/>
-      <c r="P2" s="49"/>
-      <c r="Q2" s="50"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
+      <c r="K2" s="45"/>
+      <c r="L2" s="45"/>
+      <c r="M2" s="45"/>
+      <c r="N2" s="45"/>
+      <c r="O2" s="45"/>
+      <c r="P2" s="45"/>
+      <c r="Q2" s="46"/>
       <c r="R2" s="6"/>
       <c r="S2" s="6"/>
       <c r="T2" s="6"/>
@@ -1359,7 +1352,7 @@
       <c r="Z5" s="6"/>
       <c r="AA5" s="6"/>
     </row>
-    <row r="6" spans="1:27" ht="195" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" ht="210" x14ac:dyDescent="0.25">
       <c r="B6" s="18" t="s">
         <v>25</v>
       </c>
@@ -1373,7 +1366,7 @@
         <v>26</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G6" s="14" t="s">
         <v>26</v>
@@ -1385,13 +1378,13 @@
         <v>26</v>
       </c>
       <c r="J6" s="22" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="K6" s="14" t="s">
         <v>111</v>
       </c>
       <c r="L6" s="22" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="M6" s="22" t="s">
         <v>104</v>
@@ -1403,7 +1396,7 @@
         <v>26</v>
       </c>
       <c r="P6" s="22" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="Q6" s="20"/>
       <c r="R6" s="18" t="s">
@@ -1419,7 +1412,7 @@
       <c r="Z6" s="6"/>
       <c r="AA6" s="6"/>
     </row>
-    <row r="7" spans="1:27" ht="150" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" ht="105" x14ac:dyDescent="0.25">
       <c r="B7" s="18" t="s">
         <v>33</v>
       </c>
@@ -1450,8 +1443,8 @@
       <c r="K7" s="14">
         <v>0</v>
       </c>
-      <c r="L7" s="22" t="s">
-        <v>114</v>
+      <c r="L7" s="22">
+        <v>0</v>
       </c>
       <c r="M7" s="22" t="s">
         <v>105</v>
@@ -1463,7 +1456,7 @@
         <v>22</v>
       </c>
       <c r="P7" s="22" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="Q7" s="20"/>
       <c r="R7" s="18" t="s">
@@ -2221,7 +2214,7 @@
         <v>22</v>
       </c>
       <c r="D20" s="22" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E20" s="22" t="s">
         <v>26</v>
@@ -2260,7 +2253,7 @@
         <v>22</v>
       </c>
       <c r="Q20" s="39" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="R20" s="26" t="s">
         <v>62</v>
@@ -2283,7 +2276,7 @@
         <v>22</v>
       </c>
       <c r="D21" s="43" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E21" s="29" t="s">
         <v>22</v>
@@ -2322,7 +2315,7 @@
         <v>22</v>
       </c>
       <c r="Q21" s="16" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="R21" s="26" t="s">
         <v>66</v>
@@ -4745,18 +4738,18 @@
     </row>
     <row r="2" spans="1:21" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="45" t="s">
+      <c r="B2" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44"/>
-      <c r="K2" s="44"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="48"/>
+      <c r="J2" s="48"/>
+      <c r="K2" s="48"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
@@ -7797,11 +7790,11 @@
     </row>
     <row r="2" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11"/>
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="49" t="s">
         <v>74</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
       <c r="E2" s="34"/>
       <c r="F2" s="34"/>
       <c r="G2" s="11"/>
@@ -8179,13 +8172,13 @@
     </row>
     <row r="20" spans="1:16" s="41" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="40"/>
-      <c r="B20" s="47" t="s">
+      <c r="B20" s="50" t="s">
         <v>106</v>
       </c>
-      <c r="C20" s="47"/>
-      <c r="D20" s="47"/>
-      <c r="E20" s="47"/>
-      <c r="F20" s="47"/>
+      <c r="C20" s="50"/>
+      <c r="D20" s="50"/>
+      <c r="E20" s="50"/>
+      <c r="F20" s="50"/>
       <c r="G20" s="40"/>
       <c r="H20" s="40"/>
       <c r="I20" s="40"/>

</xml_diff>

<commit_message>
updated diary data requirements and general update to make clearer
</commit_message>
<xml_diff>
--- a/Data/Test Suite Prerequisites.xlsx
+++ b/Data/Test Suite Prerequisites.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\development\feature\1.5.0\gpconnect-provider-testing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4973EFC-D5F2-4090-839D-F6CFA4B89F27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EB37C8C-7830-4D79-9EBE-947D2C3D1668}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30" yWindow="390" windowWidth="28770" windowHeight="15570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -108,9 +108,6 @@
     <t>?</t>
   </si>
   <si>
-    <t>0 (Without 'No Known Allergies' coding)</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
@@ -148,9 +145,6 @@
   </si>
   <si>
     <t>Patient 5</t>
-  </si>
-  <si>
-    <t>0 (Explicit 'No Known Allergies' coding)</t>
   </si>
   <si>
     <t>Patient 6</t>
@@ -412,12 +406,6 @@
 </t>
   </si>
   <si>
-    <t>x
-With Problems Associated to the Patients Diary Entry
-&amp;
-Diary Occurrence should be somewhere up to 180 days in the future</t>
-  </si>
-  <si>
     <t>Patient has an AllergyIntolerance with no allergy EndReason
 Patient Has Warning Codes : Confidential Items on  Allergies</t>
   </si>
@@ -446,6 +434,21 @@
 - Consultation that is linked to a topic that is linked to a problem
 - Consultation linked to a problem but not linked to a topic or heading
 -  A Consultation linked to a problem linked and to a Medication,  AllergyIntollerance, Immunization &amp;  Observation</t>
+  </si>
+  <si>
+    <t>x
+With Problems Associated to the Patients Diary Entry
+&amp;
+Diary Occurrence should be somewhere up to 10 Years in the future</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+0
+(Without 'No Known Allergies' coding)</t>
+  </si>
+  <si>
+    <t>0 
+(Explicit 'No Known Allergies' coding)</t>
   </si>
 </sst>
 </file>
@@ -569,7 +572,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -628,28 +631,6 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -665,7 +646,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -776,15 +757,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -794,6 +766,12 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1140,16 +1118,16 @@
   <dimension ref="A1:AA1001"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L7" sqref="L7"/>
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.7109375" customWidth="1"/>
-    <col min="2" max="2" width="22.5703125" customWidth="1"/>
+    <col min="2" max="2" width="53" customWidth="1"/>
     <col min="3" max="3" width="19.85546875" customWidth="1"/>
-    <col min="4" max="4" width="54" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" style="49" customWidth="1"/>
     <col min="5" max="8" width="19.85546875" customWidth="1"/>
     <col min="9" max="10" width="19.85546875" style="31" customWidth="1"/>
     <col min="11" max="11" width="25" style="31" customWidth="1"/>
@@ -1192,25 +1170,25 @@
       <c r="Z1" s="2"/>
       <c r="AA1" s="2"/>
     </row>
-    <row r="2" spans="1:27" ht="72.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="44" t="s">
+    <row r="2" spans="1:27" ht="122.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
-      <c r="K2" s="45"/>
-      <c r="L2" s="45"/>
-      <c r="M2" s="45"/>
-      <c r="N2" s="45"/>
-      <c r="O2" s="45"/>
-      <c r="P2" s="45"/>
-      <c r="Q2" s="46"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="6"/>
       <c r="R2" s="6"/>
       <c r="S2" s="6"/>
       <c r="T2" s="6"/>
@@ -1271,31 +1249,31 @@
         <v>15</v>
       </c>
       <c r="I4" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="J4" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="K4" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="J4" s="22" t="s">
+      <c r="L4" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="K4" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="L4" s="22" t="s">
+      <c r="M4" s="22" t="s">
         <v>98</v>
       </c>
-      <c r="M4" s="22" t="s">
-        <v>100</v>
-      </c>
       <c r="N4" s="22" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="O4" s="22" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="P4" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q4" s="16" t="s">
         <v>110</v>
-      </c>
-      <c r="Q4" s="16" t="s">
-        <v>112</v>
       </c>
       <c r="R4" s="6"/>
       <c r="S4" s="6"/>
@@ -1308,15 +1286,15 @@
       <c r="Z4" s="6"/>
       <c r="AA4" s="6"/>
     </row>
-    <row r="5" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" ht="60" x14ac:dyDescent="0.25">
       <c r="B5" s="18" t="s">
         <v>20</v>
       </c>
       <c r="C5" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="15" t="s">
-        <v>23</v>
+      <c r="D5" s="22" t="s">
+        <v>120</v>
       </c>
       <c r="E5" s="15">
         <v>0</v>
@@ -1354,53 +1332,53 @@
     </row>
     <row r="6" spans="1:27" ht="210" x14ac:dyDescent="0.25">
       <c r="B6" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>26</v>
-      </c>
       <c r="E6" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H6" s="14" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J6" s="22" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="K6" s="14" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="L6" s="22" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="M6" s="22" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="N6" s="22" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="O6" s="22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P6" s="22" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="Q6" s="20"/>
       <c r="R6" s="18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="S6" s="6"/>
       <c r="T6" s="6"/>
@@ -1414,16 +1392,16 @@
     </row>
     <row r="7" spans="1:27" ht="105" x14ac:dyDescent="0.25">
       <c r="B7" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C7" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="15" t="s">
-        <v>26</v>
+      <c r="D7" s="22" t="s">
+        <v>25</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F7" s="14">
         <v>0</v>
@@ -1432,13 +1410,13 @@
         <v>0</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I7" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J7" s="22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K7" s="14">
         <v>0</v>
@@ -1447,20 +1425,20 @@
         <v>0</v>
       </c>
       <c r="M7" s="22" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="N7" s="22" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="O7" s="22" t="s">
         <v>22</v>
       </c>
       <c r="P7" s="22" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="Q7" s="20"/>
       <c r="R7" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="S7" s="6"/>
       <c r="T7" s="6"/>
@@ -1474,16 +1452,16 @@
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B8" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C8" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="15" t="s">
-        <v>26</v>
+      <c r="D8" s="22" t="s">
+        <v>25</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F8" s="14">
         <v>0</v>
@@ -1520,7 +1498,7 @@
       </c>
       <c r="Q8" s="20"/>
       <c r="R8" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="S8" s="6"/>
       <c r="T8" s="6"/>
@@ -1532,24 +1510,24 @@
       <c r="Z8" s="6"/>
       <c r="AA8" s="6"/>
     </row>
-    <row r="9" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" ht="45" x14ac:dyDescent="0.25">
       <c r="B9" s="18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C9" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="15" t="s">
-        <v>37</v>
+      <c r="D9" s="22" t="s">
+        <v>121</v>
       </c>
       <c r="E9" s="15">
         <v>0</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H9" s="14">
         <v>0</v>
@@ -1580,7 +1558,7 @@
       </c>
       <c r="Q9" s="20"/>
       <c r="R9" s="18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="S9" s="6"/>
       <c r="T9" s="6"/>
@@ -1594,16 +1572,16 @@
     </row>
     <row r="10" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="18" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C10" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="15" t="s">
-        <v>26</v>
+      <c r="D10" s="22" t="s">
+        <v>25</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F10" s="14" t="s">
         <v>22</v>
@@ -1640,7 +1618,7 @@
       </c>
       <c r="Q10" s="20"/>
       <c r="R10" s="18" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="S10" s="6"/>
       <c r="T10" s="6"/>
@@ -1654,16 +1632,16 @@
     </row>
     <row r="11" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="18" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C11" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="15" t="s">
-        <v>26</v>
+      <c r="D11" s="22" t="s">
+        <v>25</v>
       </c>
       <c r="E11" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F11" s="14" t="s">
         <v>22</v>
@@ -1700,7 +1678,7 @@
       </c>
       <c r="Q11" s="20"/>
       <c r="R11" s="18" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="S11" s="6"/>
       <c r="T11" s="6"/>
@@ -1714,16 +1692,16 @@
     </row>
     <row r="12" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="18" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C12" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="15" t="s">
-        <v>26</v>
+      <c r="D12" s="22" t="s">
+        <v>25</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F12" s="14" t="s">
         <v>22</v>
@@ -1760,7 +1738,7 @@
       </c>
       <c r="Q12" s="20"/>
       <c r="R12" s="18" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="S12" s="6"/>
       <c r="T12" s="6"/>
@@ -1774,16 +1752,16 @@
     </row>
     <row r="13" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="26" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C13" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="15" t="s">
-        <v>26</v>
+      <c r="D13" s="22" t="s">
+        <v>25</v>
       </c>
       <c r="E13" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F13" s="14" t="s">
         <v>22</v>
@@ -1819,10 +1797,10 @@
         <v>22</v>
       </c>
       <c r="Q13" s="16" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="R13" s="26" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="S13" s="6"/>
       <c r="T13" s="6"/>
@@ -1836,16 +1814,16 @@
     </row>
     <row r="14" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="26" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C14" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="15" t="s">
-        <v>26</v>
+      <c r="D14" s="22" t="s">
+        <v>25</v>
       </c>
       <c r="E14" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F14" s="14" t="s">
         <v>22</v>
@@ -1881,10 +1859,10 @@
         <v>22</v>
       </c>
       <c r="Q14" s="16" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="R14" s="26" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="S14" s="6"/>
       <c r="T14" s="6"/>
@@ -1898,16 +1876,16 @@
     </row>
     <row r="15" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="26" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C15" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="15" t="s">
-        <v>26</v>
+      <c r="D15" s="22" t="s">
+        <v>25</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F15" s="14" t="s">
         <v>22</v>
@@ -1943,10 +1921,10 @@
         <v>22</v>
       </c>
       <c r="Q15" s="16" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="R15" s="26" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="S15" s="6"/>
       <c r="T15" s="6"/>
@@ -1960,16 +1938,16 @@
     </row>
     <row r="16" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="26" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C16" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="15" t="s">
-        <v>26</v>
+      <c r="D16" s="22" t="s">
+        <v>25</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F16" s="14">
         <v>0</v>
@@ -1978,7 +1956,7 @@
         <v>0</v>
       </c>
       <c r="H16" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I16" s="14" t="s">
         <v>22</v>
@@ -2005,10 +1983,10 @@
         <v>22</v>
       </c>
       <c r="Q16" s="16" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="R16" s="26" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="S16" s="6"/>
       <c r="T16" s="6"/>
@@ -2022,16 +2000,16 @@
     </row>
     <row r="17" spans="2:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="26" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C17" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="15" t="s">
-        <v>26</v>
+      <c r="D17" s="22" t="s">
+        <v>25</v>
       </c>
       <c r="E17" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F17" s="14" t="s">
         <v>22</v>
@@ -2067,10 +2045,10 @@
         <v>22</v>
       </c>
       <c r="Q17" s="16" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="R17" s="26" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="S17" s="6"/>
       <c r="T17" s="6"/>
@@ -2084,13 +2062,13 @@
     </row>
     <row r="18" spans="2:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="26" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C18" s="14" t="s">
         <v>22</v>
       </c>
       <c r="D18" s="22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E18" s="15" t="s">
         <v>22</v>
@@ -2129,10 +2107,10 @@
         <v>22</v>
       </c>
       <c r="Q18" s="16" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="R18" s="26" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="S18" s="6"/>
       <c r="T18" s="6"/>
@@ -2146,55 +2124,55 @@
     </row>
     <row r="19" spans="2:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="F19" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G19" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="H19" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="I19" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J19" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="K19" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="L19" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="M19" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="N19" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="O19" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="P19" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q19" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="C19" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="D19" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="E19" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="F19" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="G19" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="H19" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="I19" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="J19" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="K19" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="L19" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="M19" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="N19" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="O19" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="P19" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q19" s="16" t="s">
-        <v>60</v>
-      </c>
       <c r="R19" s="26" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="S19" s="6"/>
       <c r="T19" s="6"/>
@@ -2208,16 +2186,16 @@
     </row>
     <row r="20" spans="2:27" ht="75" x14ac:dyDescent="0.25">
       <c r="B20" s="26" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C20" s="14" t="s">
         <v>22</v>
       </c>
       <c r="D20" s="22" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E20" s="22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F20" s="14" t="s">
         <v>22</v>
@@ -2244,7 +2222,7 @@
         <v>22</v>
       </c>
       <c r="N20" s="22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="O20" s="22" t="s">
         <v>22</v>
@@ -2253,10 +2231,10 @@
         <v>22</v>
       </c>
       <c r="Q20" s="39" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="R20" s="26" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="S20" s="6"/>
       <c r="T20" s="6"/>
@@ -2268,15 +2246,15 @@
       <c r="Z20" s="6"/>
       <c r="AA20" s="6"/>
     </row>
-    <row r="21" spans="2:27" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:27" ht="30" x14ac:dyDescent="0.25">
       <c r="B21" s="26" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C21" s="14" t="s">
         <v>22</v>
       </c>
       <c r="D21" s="43" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E21" s="29" t="s">
         <v>22</v>
@@ -2315,10 +2293,10 @@
         <v>22</v>
       </c>
       <c r="Q21" s="16" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="R21" s="26" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="S21" s="6"/>
       <c r="T21" s="6"/>
@@ -2332,7 +2310,7 @@
     </row>
     <row r="22" spans="2:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="26" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C22" s="14" t="s">
         <v>22</v>
@@ -2377,10 +2355,10 @@
         <v>22</v>
       </c>
       <c r="Q22" s="16" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="R22" s="26" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="S22" s="6"/>
       <c r="T22" s="6"/>
@@ -2394,7 +2372,7 @@
     </row>
     <row r="23" spans="2:27" s="31" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="26" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C23" s="14" t="s">
         <v>22</v>
@@ -2440,7 +2418,7 @@
       </c>
       <c r="Q23" s="16"/>
       <c r="R23" s="26" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="S23" s="6"/>
       <c r="T23" s="6"/>
@@ -2454,55 +2432,55 @@
     </row>
     <row r="24" spans="2:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="E24" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="F24" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G24" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="H24" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="I24" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J24" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="K24" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="L24" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="M24" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="N24" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="O24" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="P24" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q24" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="C24" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="D24" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="E24" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="F24" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="G24" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="H24" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="I24" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="J24" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="K24" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="L24" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="M24" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="N24" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="O24" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="P24" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q24" s="16" t="s">
-        <v>71</v>
-      </c>
       <c r="R24" s="26" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="S24" s="6"/>
       <c r="T24" s="6"/>
@@ -2516,7 +2494,7 @@
     </row>
     <row r="25" spans="2:27" s="31" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="26" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C25" s="14" t="s">
         <v>22</v>
@@ -2561,10 +2539,10 @@
         <v>22</v>
       </c>
       <c r="Q25" s="16" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="R25" s="26" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="S25" s="6"/>
       <c r="T25" s="6"/>
@@ -3553,9 +3531,6 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B2:Q2"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -4738,18 +4713,18 @@
     </row>
     <row r="2" spans="1:21" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="47" t="s">
+      <c r="B2" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
-      <c r="J2" s="48"/>
-      <c r="K2" s="48"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
+      <c r="K2" s="45"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
@@ -4791,25 +4766,25 @@
         <v>21</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E4" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="21" t="s">
+      <c r="G4" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="G4" s="21" t="s">
+      <c r="H4" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="H4" s="19" t="s">
+      <c r="I4" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="I4" s="21" t="s">
+      <c r="J4" s="19" t="s">
         <v>31</v>
-      </c>
-      <c r="J4" s="19" t="s">
-        <v>32</v>
       </c>
       <c r="K4" s="23" t="s">
         <v>19</v>
@@ -4828,10 +4803,10 @@
     <row r="5" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C5" s="25" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D5" s="27" t="s">
         <v>22</v>
@@ -4869,10 +4844,10 @@
     <row r="6" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="24" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D6" s="27" t="s">
         <v>22</v>
@@ -4910,10 +4885,10 @@
     <row r="7" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="24" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D7" s="27" t="s">
         <v>22</v>
@@ -4951,10 +4926,10 @@
     <row r="8" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="24" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D8" s="27" t="s">
         <v>22</v>
@@ -4992,10 +4967,10 @@
     <row r="9" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="24" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C9" s="25" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D9" s="27" t="s">
         <v>22</v>
@@ -5033,10 +5008,10 @@
     <row r="10" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="24" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C10" s="25" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D10" s="27" t="s">
         <v>22</v>
@@ -5074,10 +5049,10 @@
     <row r="11" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="24" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C11" s="25" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D11" s="27" t="s">
         <v>22</v>
@@ -5115,10 +5090,10 @@
     <row r="12" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="24" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D12" s="27" t="s">
         <v>22</v>
@@ -5156,10 +5131,10 @@
     <row r="13" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="30" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C13" s="25" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D13" s="27" t="s">
         <v>22</v>
@@ -5197,10 +5172,10 @@
     <row r="14" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="30" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C14" s="25" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D14" s="27" t="s">
         <v>22</v>
@@ -5238,10 +5213,10 @@
     <row r="15" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="30" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D15" s="27" t="s">
         <v>22</v>
@@ -6437,7 +6412,7 @@
     <row r="2" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="31"/>
       <c r="B2" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
@@ -6454,7 +6429,7 @@
     <row r="3" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="31"/>
       <c r="B3" s="33" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C3" s="33"/>
       <c r="D3" s="33"/>
@@ -6486,10 +6461,10 @@
     <row r="5" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="31"/>
       <c r="B5" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D5" s="31"/>
       <c r="E5" s="31"/>
@@ -6505,7 +6480,7 @@
     <row r="6" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="31"/>
       <c r="B6" s="7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C6" s="34">
         <v>0</v>
@@ -6524,7 +6499,7 @@
     <row r="7" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="31"/>
       <c r="B7" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C7" s="34">
         <v>1</v>
@@ -6543,7 +6518,7 @@
     <row r="8" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="31"/>
       <c r="B8" s="7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C8" s="34">
         <v>2</v>
@@ -6562,7 +6537,7 @@
     <row r="9" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="31"/>
       <c r="B9" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C9" s="34">
         <v>1</v>
@@ -6596,7 +6571,7 @@
     <row r="11" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="31"/>
       <c r="B11" s="9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C11" s="33"/>
       <c r="D11" s="31"/>
@@ -6613,7 +6588,7 @@
     <row r="12" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="31"/>
       <c r="B12" s="7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="31"/>
@@ -7790,11 +7765,11 @@
     </row>
     <row r="2" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11"/>
-      <c r="B2" s="49" t="s">
-        <v>74</v>
-      </c>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
+      <c r="B2" s="46" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
       <c r="E2" s="34"/>
       <c r="F2" s="34"/>
       <c r="G2" s="11"/>
@@ -7832,13 +7807,13 @@
         <v>4</v>
       </c>
       <c r="C4" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="D4" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="E4" s="35" t="s">
         <v>84</v>
-      </c>
-      <c r="D4" s="35" t="s">
-        <v>85</v>
-      </c>
-      <c r="E4" s="35" t="s">
-        <v>86</v>
       </c>
       <c r="F4" s="35" t="s">
         <v>19</v>
@@ -7866,7 +7841,7 @@
         <v>0.44097222222222199</v>
       </c>
       <c r="E5" s="37" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F5" s="37"/>
       <c r="G5" s="11"/>
@@ -7892,7 +7867,7 @@
         <v>0.52777777777777801</v>
       </c>
       <c r="E6" s="37" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F6" s="37"/>
       <c r="G6" s="11"/>
@@ -7918,10 +7893,10 @@
         <v>0.52777777777777801</v>
       </c>
       <c r="E7" s="37" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F7" s="37" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G7" s="11"/>
       <c r="H7" s="11"/>
@@ -7973,7 +7948,7 @@
     <row r="10" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11"/>
       <c r="B10" s="38" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C10" s="34"/>
       <c r="D10" s="34"/>
@@ -8011,7 +7986,7 @@
     <row r="12" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11"/>
       <c r="B12" s="34" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C12" s="34"/>
       <c r="D12" s="34"/>
@@ -8052,7 +8027,7 @@
         <v>4</v>
       </c>
       <c r="C14" s="35" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D14" s="34"/>
       <c r="E14" s="34"/>
@@ -8172,13 +8147,13 @@
     </row>
     <row r="20" spans="1:16" s="41" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="40"/>
-      <c r="B20" s="50" t="s">
-        <v>106</v>
-      </c>
-      <c r="C20" s="50"/>
-      <c r="D20" s="50"/>
-      <c r="E20" s="50"/>
-      <c r="F20" s="50"/>
+      <c r="B20" s="47" t="s">
+        <v>104</v>
+      </c>
+      <c r="C20" s="47"/>
+      <c r="D20" s="47"/>
+      <c r="E20" s="47"/>
+      <c r="F20" s="47"/>
       <c r="G20" s="40"/>
       <c r="H20" s="40"/>
       <c r="I20" s="40"/>
@@ -8193,7 +8168,7 @@
     <row r="21" spans="1:16" s="41" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="40"/>
       <c r="B21" s="42" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C21" s="42"/>
       <c r="D21" s="42"/>
@@ -8212,7 +8187,7 @@
     </row>
     <row r="22" spans="1:16" s="41" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="42" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C22" s="42"/>
       <c r="D22" s="42"/>

</xml_diff>

<commit_message>
updated consultations data rqmts and fixed issues raised by emis
</commit_message>
<xml_diff>
--- a/Data/Test Suite Prerequisites.xlsx
+++ b/Data/Test Suite Prerequisites.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\development\feature\1.5.0\gpconnect-provider-testing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EB37C8C-7830-4D79-9EBE-947D2C3D1668}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9339DEBB-9E82-47C9-8528-DAEB3D0951F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="390" windowWidth="28770" windowHeight="15570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Patients" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="122">
   <si>
     <t>Required Organizations and Slots for testing</t>
   </si>
@@ -347,14 +347,6 @@
   <si>
     <t>x
 Patient Linked to ReferralRequests and  NOT linked to a problem</t>
-  </si>
-  <si>
-    <t>x
-Patient Linked to DiagnosticReport linked to a  ProcedureRequest,  specimen, test group, test report filing and also a problem linked to a diagnostic report</t>
-  </si>
-  <si>
-    <t>x
-Patient Linked to DiagnosticReport linked to a  ProcedureRequest,  specimen, test group, test report filing BUT NOT linked to any problems</t>
   </si>
   <si>
     <t>Requirements for Schedule and Slots for Tests relating to serviceCategory and serviceType</t>
@@ -427,16 +419,6 @@
   </si>
   <si>
     <t>x
--- UNDER REVIEW --
-- Consultation that is linked to only clinical items
-- Consultation That is only Linked to A topic that is only linked to clinical items (no heading)
-- Consultation that is linked to a Topic or Heading  that is linked to all supported Clinical items 
-- Consultation that is linked to a topic that is linked to a problem
-- Consultation linked to a problem but not linked to a topic or heading
--  A Consultation linked to a problem linked and to a Medication,  AllergyIntollerance, Immunization &amp;  Observation</t>
-  </si>
-  <si>
-    <t>x
 With Problems Associated to the Patients Diary Entry
 &amp;
 Diary Occurrence should be somewhere up to 10 Years in the future</t>
@@ -449,6 +431,20 @@
   <si>
     <t>0 
 (Explicit 'No Known Allergies' coding)</t>
+  </si>
+  <si>
+    <t>x
+Patient Linked to a DiagnosticReport linked to a  ProcedureRequest,  specimen, test group, test report filing and also a problem linked to a diagnostic report</t>
+  </si>
+  <si>
+    <t>x
+Patient Linked to a DiagnosticReport linked to a  ProcedureRequest,  specimen, test group, test report filing BUT NOT linked to any problems</t>
+  </si>
+  <si>
+    <t>x
+- Consultation that is linked to a Topic or Heading that is linked to a MedicationRequest, AllergyIntollerance, Immunization &amp;  Observation
+- Consultation that is linked to a topic that is linked to a problem
+- A Consultation linked to a problem that is linked to a Medication,  AllergyIntollerance, Immunization &amp;  Observation</t>
   </si>
 </sst>
 </file>
@@ -757,6 +753,12 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -766,12 +768,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1118,8 +1114,8 @@
   <dimension ref="A1:AA1001"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B2" sqref="B2"/>
+      <pane xSplit="2" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1127,7 +1123,7 @@
     <col min="1" max="1" width="2.7109375" customWidth="1"/>
     <col min="2" max="2" width="53" customWidth="1"/>
     <col min="3" max="3" width="19.85546875" customWidth="1"/>
-    <col min="4" max="4" width="24.7109375" style="49" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" style="45" customWidth="1"/>
     <col min="5" max="8" width="19.85546875" customWidth="1"/>
     <col min="9" max="10" width="19.85546875" style="31" customWidth="1"/>
     <col min="11" max="11" width="25" style="31" customWidth="1"/>
@@ -1171,7 +1167,7 @@
       <c r="AA1" s="2"/>
     </row>
     <row r="2" spans="1:27" ht="122.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="48" t="s">
+      <c r="B2" s="44" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="6"/>
@@ -1267,13 +1263,13 @@
         <v>99</v>
       </c>
       <c r="O4" s="22" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="P4" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q4" s="16" t="s">
         <v>108</v>
-      </c>
-      <c r="Q4" s="16" t="s">
-        <v>110</v>
       </c>
       <c r="R4" s="6"/>
       <c r="S4" s="6"/>
@@ -1294,7 +1290,7 @@
         <v>22</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E5" s="15">
         <v>0</v>
@@ -1330,7 +1326,7 @@
       <c r="Z5" s="6"/>
       <c r="AA5" s="6"/>
     </row>
-    <row r="6" spans="1:27" ht="210" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" ht="135" x14ac:dyDescent="0.25">
       <c r="B6" s="18" t="s">
         <v>24</v>
       </c>
@@ -1344,7 +1340,7 @@
         <v>25</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G6" s="14" t="s">
         <v>25</v>
@@ -1356,16 +1352,16 @@
         <v>25</v>
       </c>
       <c r="J6" s="22" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K6" s="14" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="L6" s="22" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="M6" s="22" t="s">
-        <v>102</v>
+        <v>119</v>
       </c>
       <c r="N6" s="22" t="s">
         <v>100</v>
@@ -1374,7 +1370,7 @@
         <v>25</v>
       </c>
       <c r="P6" s="22" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="Q6" s="20"/>
       <c r="R6" s="18" t="s">
@@ -1421,11 +1417,11 @@
       <c r="K7" s="14">
         <v>0</v>
       </c>
-      <c r="L7" s="22">
-        <v>0</v>
+      <c r="L7" s="22" t="s">
+        <v>22</v>
       </c>
       <c r="M7" s="22" t="s">
-        <v>103</v>
+        <v>120</v>
       </c>
       <c r="N7" s="22" t="s">
         <v>101</v>
@@ -1434,7 +1430,7 @@
         <v>22</v>
       </c>
       <c r="P7" s="22" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="Q7" s="20"/>
       <c r="R7" s="18" t="s">
@@ -1518,7 +1514,7 @@
         <v>22</v>
       </c>
       <c r="D9" s="22" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E9" s="15">
         <v>0</v>
@@ -2192,7 +2188,7 @@
         <v>22</v>
       </c>
       <c r="D20" s="22" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E20" s="22" t="s">
         <v>25</v>
@@ -2231,7 +2227,7 @@
         <v>22</v>
       </c>
       <c r="Q20" s="39" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="R20" s="26" t="s">
         <v>60</v>
@@ -2254,7 +2250,7 @@
         <v>22</v>
       </c>
       <c r="D21" s="43" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E21" s="29" t="s">
         <v>22</v>
@@ -2293,7 +2289,7 @@
         <v>22</v>
       </c>
       <c r="Q21" s="16" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="R21" s="26" t="s">
         <v>64</v>
@@ -4713,18 +4709,18 @@
     </row>
     <row r="2" spans="1:21" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
-      <c r="K2" s="45"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47"/>
+      <c r="J2" s="47"/>
+      <c r="K2" s="47"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
@@ -7765,11 +7761,11 @@
     </row>
     <row r="2" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11"/>
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="48" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="47"/>
       <c r="E2" s="34"/>
       <c r="F2" s="34"/>
       <c r="G2" s="11"/>
@@ -8147,13 +8143,13 @@
     </row>
     <row r="20" spans="1:16" s="41" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="40"/>
-      <c r="B20" s="47" t="s">
-        <v>104</v>
-      </c>
-      <c r="C20" s="47"/>
-      <c r="D20" s="47"/>
-      <c r="E20" s="47"/>
-      <c r="F20" s="47"/>
+      <c r="B20" s="49" t="s">
+        <v>102</v>
+      </c>
+      <c r="C20" s="49"/>
+      <c r="D20" s="49"/>
+      <c r="E20" s="49"/>
+      <c r="F20" s="49"/>
       <c r="G20" s="40"/>
       <c r="H20" s="40"/>
       <c r="I20" s="40"/>
@@ -8168,7 +8164,7 @@
     <row r="21" spans="1:16" s="41" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="40"/>
       <c r="B21" s="42" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C21" s="42"/>
       <c r="D21" s="42"/>
@@ -8187,7 +8183,7 @@
     </row>
     <row r="22" spans="1:16" s="41" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="42" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C22" s="42"/>
       <c r="D22" s="42"/>

</xml_diff>

<commit_message>
updated data requirements for investigations
</commit_message>
<xml_diff>
--- a/Data/Test Suite Prerequisites.xlsx
+++ b/Data/Test Suite Prerequisites.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\development\feature\1.5.0\gpconnect-provider-testing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9339DEBB-9E82-47C9-8528-DAEB3D0951F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5A9DF26-DC2D-4450-9CB5-95EF37524A01}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Patients" sheetId="1" r:id="rId1"/>
@@ -434,17 +434,19 @@
   </si>
   <si>
     <t>x
-Patient Linked to a DiagnosticReport linked to a  ProcedureRequest,  specimen, test group, test report filing and also a problem linked to a diagnostic report</t>
-  </si>
-  <si>
-    <t>x
-Patient Linked to a DiagnosticReport linked to a  ProcedureRequest,  specimen, test group, test report filing BUT NOT linked to any problems</t>
-  </si>
-  <si>
-    <t>x
 - Consultation that is linked to a Topic or Heading that is linked to a MedicationRequest, AllergyIntollerance, Immunization &amp;  Observation
 - Consultation that is linked to a topic that is linked to a problem
 - A Consultation linked to a problem that is linked to a Medication,  AllergyIntollerance, Immunization &amp;  Observation</t>
+  </si>
+  <si>
+    <t>x
+Patient Linked to a DiagnosticReport linked to a  ProcedureRequest,  specimen, test group, test report filing and also a problem linked to a diagnostic report
+- Use Supplied EDIFACT Message and Link Diagnostic Report to a Problem</t>
+  </si>
+  <si>
+    <t>x
+Patient Linked to a DiagnosticReport linked to a  ProcedureRequest,  specimen, test group, test report filing BUT NOT linked to any problems
+- Use Supplied EDIFACT Message</t>
   </si>
 </sst>
 </file>
@@ -1115,7 +1117,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L7" sqref="L7"/>
+      <selection pane="topRight" activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1326,7 +1328,7 @@
       <c r="Z5" s="6"/>
       <c r="AA5" s="6"/>
     </row>
-    <row r="6" spans="1:27" ht="135" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" ht="180" x14ac:dyDescent="0.25">
       <c r="B6" s="18" t="s">
         <v>24</v>
       </c>
@@ -1358,10 +1360,10 @@
         <v>107</v>
       </c>
       <c r="L6" s="22" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="M6" s="22" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="N6" s="22" t="s">
         <v>100</v>
@@ -1386,7 +1388,7 @@
       <c r="Z6" s="6"/>
       <c r="AA6" s="6"/>
     </row>
-    <row r="7" spans="1:27" ht="105" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" ht="135" x14ac:dyDescent="0.25">
       <c r="B7" s="18" t="s">
         <v>32</v>
       </c>
@@ -1421,7 +1423,7 @@
         <v>22</v>
       </c>
       <c r="M7" s="22" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="N7" s="22" t="s">
         <v>101</v>

</xml_diff>

<commit_message>
Split ProcedureRequest checks into separate Tests
</commit_message>
<xml_diff>
--- a/Data/Test Suite Prerequisites.xlsx
+++ b/Data/Test Suite Prerequisites.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\development\feature\1.5.0\gpconnect-provider-testing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5A9DF26-DC2D-4450-9CB5-95EF37524A01}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A01CA17-69D8-40CB-84F5-BFA6F1B70618}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -441,11 +441,13 @@
   <si>
     <t>x
 Patient Linked to a DiagnosticReport linked to a  ProcedureRequest,  specimen, test group, test report filing and also a problem linked to a diagnostic report
+Note : ProcedureRequest is Optional and Tested Separately - Test can be ignored if not supported
 - Use Supplied EDIFACT Message and Link Diagnostic Report to a Problem</t>
   </si>
   <si>
     <t>x
 Patient Linked to a DiagnosticReport linked to a  ProcedureRequest,  specimen, test group, test report filing BUT NOT linked to any problems
+Note : ProcedureRequest is Optional and Tested Separately - Test can be ignored if not supported
 - Use Supplied EDIFACT Message</t>
   </si>
 </sst>
@@ -1113,14 +1115,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AA1001"/>
+  <dimension ref="A1:AA25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M8" sqref="M8"/>
+      <pane xSplit="2" topLeftCell="K1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.7109375" customWidth="1"/>
     <col min="2" max="2" width="53" customWidth="1"/>
@@ -1130,7 +1132,7 @@
     <col min="9" max="10" width="19.85546875" style="31" customWidth="1"/>
     <col min="11" max="11" width="25" style="31" customWidth="1"/>
     <col min="12" max="12" width="54.140625" style="31" customWidth="1"/>
-    <col min="13" max="13" width="24.7109375" style="31" customWidth="1"/>
+    <col min="13" max="13" width="55.85546875" style="31" customWidth="1"/>
     <col min="14" max="14" width="19.85546875" style="31" customWidth="1"/>
     <col min="15" max="15" width="13.7109375" style="31" customWidth="1"/>
     <col min="16" max="16" width="19.42578125" style="31" customWidth="1"/>
@@ -1139,7 +1141,7 @@
     <col min="19" max="27" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -1168,7 +1170,7 @@
       <c r="Z1" s="2"/>
       <c r="AA1" s="2"/>
     </row>
-    <row r="2" spans="1:27" ht="122.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:27" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="44" t="s">
         <v>2</v>
       </c>
@@ -1198,7 +1200,7 @@
       <c r="Z2" s="6"/>
       <c r="AA2" s="6"/>
     </row>
-    <row r="3" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B3" s="6"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -1328,7 +1330,7 @@
       <c r="Z5" s="6"/>
       <c r="AA5" s="6"/>
     </row>
-    <row r="6" spans="1:27" ht="180" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" ht="150" x14ac:dyDescent="0.25">
       <c r="B6" s="18" t="s">
         <v>24</v>
       </c>
@@ -1568,7 +1570,7 @@
       <c r="Z9" s="6"/>
       <c r="AA9" s="6"/>
     </row>
-    <row r="10" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B10" s="18" t="s">
         <v>36</v>
       </c>
@@ -1628,7 +1630,7 @@
       <c r="Z10" s="6"/>
       <c r="AA10" s="6"/>
     </row>
-    <row r="11" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B11" s="18" t="s">
         <v>37</v>
       </c>
@@ -1688,7 +1690,7 @@
       <c r="Z11" s="6"/>
       <c r="AA11" s="6"/>
     </row>
-    <row r="12" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B12" s="18" t="s">
         <v>38</v>
       </c>
@@ -1748,7 +1750,7 @@
       <c r="Z12" s="6"/>
       <c r="AA12" s="6"/>
     </row>
-    <row r="13" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B13" s="26" t="s">
         <v>40</v>
       </c>
@@ -1810,7 +1812,7 @@
       <c r="Z13" s="6"/>
       <c r="AA13" s="6"/>
     </row>
-    <row r="14" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B14" s="26" t="s">
         <v>42</v>
       </c>
@@ -1872,7 +1874,7 @@
       <c r="Z14" s="6"/>
       <c r="AA14" s="6"/>
     </row>
-    <row r="15" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B15" s="26" t="s">
         <v>43</v>
       </c>
@@ -1934,7 +1936,7 @@
       <c r="Z15" s="6"/>
       <c r="AA15" s="6"/>
     </row>
-    <row r="16" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B16" s="26" t="s">
         <v>45</v>
       </c>
@@ -1996,7 +1998,7 @@
       <c r="Z16" s="6"/>
       <c r="AA16" s="6"/>
     </row>
-    <row r="17" spans="2:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B17" s="26" t="s">
         <v>47</v>
       </c>
@@ -2058,7 +2060,7 @@
       <c r="Z17" s="6"/>
       <c r="AA17" s="6"/>
     </row>
-    <row r="18" spans="2:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:27" ht="30" x14ac:dyDescent="0.25">
       <c r="B18" s="26" t="s">
         <v>52</v>
       </c>
@@ -2120,7 +2122,7 @@
       <c r="Z18" s="6"/>
       <c r="AA18" s="6"/>
     </row>
-    <row r="19" spans="2:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:27" ht="30" x14ac:dyDescent="0.25">
       <c r="B19" s="26" t="s">
         <v>56</v>
       </c>
@@ -2306,7 +2308,7 @@
       <c r="Z21" s="6"/>
       <c r="AA21" s="6"/>
     </row>
-    <row r="22" spans="2:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:27" ht="30" x14ac:dyDescent="0.25">
       <c r="B22" s="26" t="s">
         <v>65</v>
       </c>
@@ -2368,7 +2370,7 @@
       <c r="Z22" s="6"/>
       <c r="AA22" s="6"/>
     </row>
-    <row r="23" spans="2:27" s="31" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:27" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="26" t="s">
         <v>90</v>
       </c>
@@ -2428,7 +2430,7 @@
       <c r="Z23" s="6"/>
       <c r="AA23" s="6"/>
     </row>
-    <row r="24" spans="2:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:27" ht="30" x14ac:dyDescent="0.25">
       <c r="B24" s="26" t="s">
         <v>67</v>
       </c>
@@ -2490,7 +2492,7 @@
       <c r="Z24" s="6"/>
       <c r="AA24" s="6"/>
     </row>
-    <row r="25" spans="2:27" s="31" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:27" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="26" t="s">
         <v>92</v>
       </c>
@@ -2552,982 +2554,6 @@
       <c r="Z25" s="6"/>
       <c r="AA25" s="6"/>
     </row>
-    <row r="26" spans="2:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="2:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="2:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="2:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="2:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="2:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="53" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="55" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="56" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="57" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="58" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="59" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="60" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="61" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="62" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="63" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="64" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="65" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="66" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="67" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="68" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="69" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="70" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="71" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="72" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="73" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="74" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="76" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="77" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="79" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="80" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="81" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="82" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="83" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="84" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="85" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="86" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="87" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="88" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="89" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="90" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="91" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="92" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="93" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="94" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="95" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="96" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="97" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="98" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="99" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="100" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="101" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="102" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="103" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="104" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="105" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="106" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="107" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="108" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="109" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="110" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="111" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="112" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="113" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="114" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="115" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="116" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="117" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="118" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="119" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="120" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="121" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="122" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="123" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="124" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="125" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="126" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="127" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="128" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="129" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="130" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="131" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="132" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="133" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="134" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="135" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="136" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="137" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="138" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="139" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="140" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="141" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="142" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="143" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="144" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="145" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="146" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="147" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="148" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="149" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="150" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="151" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="152" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="153" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="154" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="155" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="156" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="157" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="158" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="159" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="160" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="161" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="162" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="163" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="164" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="165" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="166" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="167" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="168" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="169" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="170" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="171" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="172" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="173" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="174" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="175" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="176" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="177" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="178" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="179" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="180" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="181" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="182" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="183" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="184" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="185" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="186" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="187" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="188" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="189" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="190" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="192" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="193" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="194" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="195" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="196" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="197" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="198" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="199" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="200" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="201" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="202" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="203" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="204" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="205" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="206" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="207" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="208" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="209" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="210" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="211" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="212" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="213" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="214" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="215" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="216" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="217" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="218" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="219" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="220" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="221" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="222" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="223" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="224" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="225" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="226" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="227" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="228" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="229" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="230" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="231" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="232" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="233" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="234" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="235" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="236" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="237" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="238" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="239" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="240" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="241" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="242" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="243" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="244" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="245" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="246" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="247" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="248" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="249" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="250" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="251" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="252" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="253" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="254" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="255" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="256" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="257" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="258" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="259" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="260" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="261" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="262" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="263" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="264" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="265" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="266" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="267" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="268" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="269" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="270" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="271" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="272" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="273" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="274" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="275" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="276" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="277" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="278" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="279" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="280" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="281" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="282" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="283" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="284" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="285" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="286" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="287" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="288" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="289" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="290" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="291" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="292" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="293" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="294" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="295" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="296" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="297" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="298" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="299" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="300" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="301" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="302" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="303" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="304" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="305" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="306" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="307" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="308" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="309" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="310" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="311" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="312" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="313" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="314" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="315" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="316" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="317" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="318" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="319" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="320" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="322" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="323" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="324" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="325" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="326" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="327" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="328" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="329" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="330" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="331" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="332" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="333" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="334" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="335" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="336" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="337" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="338" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="339" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="340" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="341" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="342" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="343" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="344" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="345" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="346" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="347" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="348" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="349" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="350" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="351" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="352" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="353" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="354" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="355" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="356" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="357" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="358" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="359" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="360" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="361" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="362" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="363" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="364" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="365" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="366" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="367" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="368" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="369" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="370" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="371" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="372" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="373" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="374" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="375" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="376" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="377" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="378" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="379" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="380" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="381" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="382" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="383" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="384" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="385" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="386" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="387" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="388" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="389" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="390" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="391" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="392" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="393" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="394" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="395" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="396" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="397" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="398" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="399" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="400" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="401" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="402" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="403" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="404" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="405" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="406" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="407" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="408" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="409" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="410" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="411" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="412" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="413" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="414" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="415" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="416" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="417" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="418" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="419" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="420" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="421" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="422" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="423" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="424" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="425" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="426" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="427" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="428" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="429" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="430" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="431" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="432" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="433" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="434" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="435" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="436" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="437" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="438" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="439" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="440" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="441" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="442" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="443" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="444" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="445" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="446" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="447" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="448" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="449" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="450" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="451" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="452" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="453" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="454" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="455" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="456" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="457" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="458" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="459" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="460" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="461" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="462" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="463" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="464" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="465" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="466" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="467" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="468" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="469" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="470" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="471" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="472" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="473" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="474" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="475" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="476" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="477" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="478" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="479" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="480" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="481" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="482" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="483" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="484" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="485" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="486" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="487" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="488" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="489" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="490" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="491" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="492" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="493" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="494" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="495" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="496" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="497" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="498" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="499" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="500" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="501" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="502" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="503" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="504" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="505" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="506" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="507" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="508" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="509" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="510" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="511" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="512" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="513" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="514" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="515" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="516" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="517" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="518" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="519" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="520" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="521" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="522" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="523" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="524" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="525" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="526" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="527" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="528" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="529" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="530" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="531" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="532" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="533" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="534" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="535" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="536" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="537" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="538" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="539" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="540" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="541" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="542" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="543" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="544" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="545" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="546" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="547" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="548" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="549" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="550" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="551" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="552" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="553" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="554" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="555" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="556" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="557" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="558" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="559" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="560" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="561" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="562" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="563" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="564" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="565" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="566" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="567" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="568" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="569" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="570" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="571" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="572" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="573" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="574" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="575" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="576" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="577" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="578" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="579" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="580" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="581" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="582" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="583" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="584" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="585" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="586" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="587" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="588" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="589" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="590" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="591" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="592" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="593" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="594" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="595" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="596" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="597" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="598" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="599" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="600" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="601" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="602" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="603" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="604" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="605" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="606" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="607" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="608" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="609" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="610" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="611" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="612" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="613" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="614" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="615" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="616" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="617" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="618" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="619" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="620" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="621" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="622" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="623" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="624" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="625" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="626" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="627" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="628" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="629" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="630" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="631" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="632" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="633" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="634" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="635" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="636" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="637" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="638" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="639" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="640" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="641" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="642" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="643" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="644" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="645" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="646" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="647" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="648" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="649" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="650" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="651" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="652" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="653" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="654" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="655" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="656" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="657" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="658" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="659" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="660" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="661" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="662" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="663" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="664" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="665" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="666" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="667" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="668" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="669" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="670" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="671" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="672" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="673" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="674" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="675" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="676" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="677" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="678" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="679" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="680" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="681" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="682" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="683" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="684" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="685" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="686" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="687" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="688" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="689" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="690" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="691" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="692" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="693" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="694" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="695" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="696" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="697" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="698" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="699" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="700" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="701" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="702" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="703" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="704" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="705" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="706" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="707" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="708" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="709" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="710" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="711" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="712" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="713" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="714" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="715" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="716" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="717" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="718" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="719" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="720" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="721" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="722" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="723" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="724" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="725" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="726" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="727" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="728" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="729" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="730" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="731" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="732" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="733" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="734" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="735" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="736" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="737" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="738" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="739" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="740" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="741" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="742" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="743" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="744" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="745" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="746" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="747" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="748" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="749" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="750" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="751" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="752" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="753" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="754" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="755" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="756" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="757" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="758" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="759" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="760" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="761" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="762" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="763" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="764" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="765" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="766" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="767" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="768" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="769" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="770" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="771" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="772" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="773" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="774" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="775" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="776" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="777" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="778" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="779" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="780" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="781" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="782" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="783" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="784" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="785" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="786" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="787" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="788" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="789" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="790" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="791" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="792" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="793" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="794" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="795" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="796" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="797" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="798" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="799" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="800" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="801" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="802" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="803" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="804" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="805" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="806" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="807" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="808" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="809" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="810" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="811" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="812" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="813" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="814" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="815" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="816" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="817" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="818" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="819" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="820" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="821" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="822" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="823" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="824" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="825" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="826" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="827" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="828" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="829" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="830" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="831" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="832" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="833" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="834" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="835" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="836" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="837" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="838" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="839" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="840" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="841" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="842" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="843" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="844" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="845" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="846" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="847" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="848" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="849" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="850" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="851" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="852" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="853" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="854" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="855" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="856" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="857" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="858" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="859" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="860" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="861" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="862" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="863" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="864" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="865" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="866" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="867" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="868" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="869" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="870" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="871" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="872" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="873" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="874" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="875" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="876" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="877" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="878" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="879" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="880" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="881" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="882" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="883" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="884" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="885" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="886" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="887" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="888" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="889" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="890" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="891" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="892" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="893" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="894" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="895" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="896" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="897" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="898" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="899" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="900" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="901" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="902" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="903" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="904" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="905" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="906" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="907" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="908" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="909" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="910" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="911" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="912" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="913" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="914" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="915" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="916" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="917" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="918" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="919" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="920" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="921" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="922" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="923" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="924" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="925" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="926" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="927" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="928" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="929" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="930" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="931" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="932" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="933" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="934" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="935" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="936" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="937" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="938" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="939" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="940" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="941" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="942" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="943" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="944" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="945" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="946" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="947" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="948" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="949" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="950" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="951" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="952" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="953" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="954" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="955" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="956" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="957" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="958" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="959" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="960" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="961" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="962" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="963" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="964" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="965" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="966" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="967" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="968" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="969" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="970" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="971" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="972" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="973" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="974" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="975" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="976" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="977" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="978" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="979" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="980" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="981" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="982" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="983" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="984" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="985" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="986" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="987" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="988" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="990" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Further updates to 1.5.0 for latest changes
</commit_message>
<xml_diff>
--- a/Data/Test Suite Prerequisites.xlsx
+++ b/Data/Test Suite Prerequisites.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\development\feature\1.5.0\gpconnect-provider-testing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A01CA17-69D8-40CB-84F5-BFA6F1B70618}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{929D1B64-2A60-435A-BC95-5CBC67857DC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -386,10 +386,6 @@
     <t>Diary</t>
   </si>
   <si>
-    <t xml:space="preserve">x
-</t>
-  </si>
-  <si>
     <t>Other Requirements / Comments</t>
   </si>
   <si>
@@ -449,6 +445,11 @@
 Patient Linked to a DiagnosticReport linked to a  ProcedureRequest,  specimen, test group, test report filing BUT NOT linked to any problems
 Note : ProcedureRequest is Optional and Tested Separately - Test can be ignored if not supported
 - Use Supplied EDIFACT Message</t>
+  </si>
+  <si>
+    <t>x
+Problem(s) - Linked to Medication Request, Consultation and Uncategorised Data.
+If Supported Also have a  problem linked to another problem</t>
   </si>
 </sst>
 </file>
@@ -1118,8 +1119,8 @@
   <dimension ref="A1:AA25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="K1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="R6" sqref="R6"/>
+      <pane xSplit="2" topLeftCell="G1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1273,7 +1274,7 @@
         <v>106</v>
       </c>
       <c r="Q4" s="16" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="R4" s="6"/>
       <c r="S4" s="6"/>
@@ -1294,7 +1295,7 @@
         <v>22</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E5" s="15">
         <v>0</v>
@@ -1344,7 +1345,7 @@
         <v>25</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G6" s="14" t="s">
         <v>25</v>
@@ -1356,16 +1357,16 @@
         <v>25</v>
       </c>
       <c r="J6" s="22" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K6" s="14" t="s">
-        <v>107</v>
+        <v>121</v>
       </c>
       <c r="L6" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="M6" s="22" t="s">
         <v>119</v>
-      </c>
-      <c r="M6" s="22" t="s">
-        <v>120</v>
       </c>
       <c r="N6" s="22" t="s">
         <v>100</v>
@@ -1374,7 +1375,7 @@
         <v>25</v>
       </c>
       <c r="P6" s="22" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="Q6" s="20"/>
       <c r="R6" s="18" t="s">
@@ -1425,7 +1426,7 @@
         <v>22</v>
       </c>
       <c r="M7" s="22" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="N7" s="22" t="s">
         <v>101</v>
@@ -1434,7 +1435,7 @@
         <v>22</v>
       </c>
       <c r="P7" s="22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="Q7" s="20"/>
       <c r="R7" s="18" t="s">
@@ -1518,7 +1519,7 @@
         <v>22</v>
       </c>
       <c r="D9" s="22" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E9" s="15">
         <v>0</v>
@@ -2192,7 +2193,7 @@
         <v>22</v>
       </c>
       <c r="D20" s="22" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E20" s="22" t="s">
         <v>25</v>
@@ -2231,7 +2232,7 @@
         <v>22</v>
       </c>
       <c r="Q20" s="39" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="R20" s="26" t="s">
         <v>60</v>
@@ -2254,7 +2255,7 @@
         <v>22</v>
       </c>
       <c r="D21" s="43" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E21" s="29" t="s">
         <v>22</v>
@@ -2293,7 +2294,7 @@
         <v>22</v>
       </c>
       <c r="Q21" s="16" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="R21" s="26" t="s">
         <v>64</v>

</xml_diff>

<commit_message>
updated test prereqisities sheet
</commit_message>
<xml_diff>
--- a/Data/Test Suite Prerequisites.xlsx
+++ b/Data/Test Suite Prerequisites.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\development\feature\1.5.0\gpconnect-provider-testing\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\development\Merge\1.5.0-oct-update-wip\gpconnect-provider-testing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{929D1B64-2A60-435A-BC95-5CBC67857DC5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{713E78B0-99D6-43AE-9391-AE3FA7239E77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -430,12 +430,6 @@
   </si>
   <si>
     <t>x
-- Consultation that is linked to a Topic or Heading that is linked to a MedicationRequest, AllergyIntollerance, Immunization &amp;  Observation
-- Consultation that is linked to a topic that is linked to a problem
-- A Consultation linked to a problem that is linked to a Medication,  AllergyIntollerance, Immunization &amp;  Observation</t>
-  </si>
-  <si>
-    <t>x
 Patient Linked to a DiagnosticReport linked to a  ProcedureRequest,  specimen, test group, test report filing and also a problem linked to a diagnostic report
 Note : ProcedureRequest is Optional and Tested Separately - Test can be ignored if not supported
 - Use Supplied EDIFACT Message and Link Diagnostic Report to a Problem</t>
@@ -450,6 +444,12 @@
     <t>x
 Problem(s) - Linked to Medication Request, Consultation and Uncategorised Data.
 If Supported Also have a  problem linked to another problem</t>
+  </si>
+  <si>
+    <t>x
+- Consultation that is linked to a Topic or Heading that is linked to a MedicationRequest,  Uncategorised 
+- Consultation that is linked to a topic that is linked to a problem
+- A Consultation linked to a problem that is linked to a Medication and Uncategorised Data</t>
   </si>
 </sst>
 </file>
@@ -1119,8 +1119,8 @@
   <dimension ref="A1:AA25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="G1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K6" sqref="K6"/>
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1360,13 +1360,13 @@
         <v>111</v>
       </c>
       <c r="K6" s="14" t="s">
+        <v>120</v>
+      </c>
+      <c r="L6" s="22" t="s">
         <v>121</v>
       </c>
-      <c r="L6" s="22" t="s">
+      <c r="M6" s="22" t="s">
         <v>118</v>
-      </c>
-      <c r="M6" s="22" t="s">
-        <v>119</v>
       </c>
       <c r="N6" s="22" t="s">
         <v>100</v>
@@ -1426,7 +1426,7 @@
         <v>22</v>
       </c>
       <c r="M7" s="22" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="N7" s="22" t="s">
         <v>101</v>

</xml_diff>

<commit_message>
updated data requirement to remove need for test report filing to be linked to DR
</commit_message>
<xml_diff>
--- a/Data/Test Suite Prerequisites.xlsx
+++ b/Data/Test Suite Prerequisites.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\development\Merge\1.5.0-oct-update-wip\gpconnect-provider-testing\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\development\feature\1.5.0\gpconnect-provider-testing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{713E78B0-99D6-43AE-9391-AE3FA7239E77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F0BFF86-ECB2-41C0-996D-EDBD2601467A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -430,18 +430,6 @@
   </si>
   <si>
     <t>x
-Patient Linked to a DiagnosticReport linked to a  ProcedureRequest,  specimen, test group, test report filing and also a problem linked to a diagnostic report
-Note : ProcedureRequest is Optional and Tested Separately - Test can be ignored if not supported
-- Use Supplied EDIFACT Message and Link Diagnostic Report to a Problem</t>
-  </si>
-  <si>
-    <t>x
-Patient Linked to a DiagnosticReport linked to a  ProcedureRequest,  specimen, test group, test report filing BUT NOT linked to any problems
-Note : ProcedureRequest is Optional and Tested Separately - Test can be ignored if not supported
-- Use Supplied EDIFACT Message</t>
-  </si>
-  <si>
-    <t>x
 Problem(s) - Linked to Medication Request, Consultation and Uncategorised Data.
 If Supported Also have a  problem linked to another problem</t>
   </si>
@@ -450,6 +438,18 @@
 - Consultation that is linked to a Topic or Heading that is linked to a MedicationRequest,  Uncategorised 
 - Consultation that is linked to a topic that is linked to a problem
 - A Consultation linked to a problem that is linked to a Medication and Uncategorised Data</t>
+  </si>
+  <si>
+    <t>x
+Patient Linked to a DiagnosticReport linked to a  ProcedureRequest,  specimen, test group and also a problem linked to a diagnostic report
+Note : ProcedureRequest is Optional and Tested Separately - Test can be ignored if not supported
+- Use Supplied EDIFACT Message and Link Diagnostic Report to a Problem</t>
+  </si>
+  <si>
+    <t>x
+Patient Linked to a DiagnosticReport linked to a  ProcedureRequest,  specimen, test group BUT NOT linked to any problems
+Note : ProcedureRequest is Optional and Tested Separately - Test can be ignored if not supported
+- Use Supplied EDIFACT Message</t>
   </si>
 </sst>
 </file>
@@ -1118,9 +1118,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="H1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1360,13 +1360,13 @@
         <v>111</v>
       </c>
       <c r="K6" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="L6" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="M6" s="22" t="s">
         <v>120</v>
-      </c>
-      <c r="L6" s="22" t="s">
-        <v>121</v>
-      </c>
-      <c r="M6" s="22" t="s">
-        <v>118</v>
       </c>
       <c r="N6" s="22" t="s">
         <v>100</v>
@@ -1426,7 +1426,7 @@
         <v>22</v>
       </c>
       <c r="M7" s="22" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="N7" s="22" t="s">
         <v>101</v>

</xml_diff>

<commit_message>
Bunlde.id update and various updates for 1.5.0 latest changes
</commit_message>
<xml_diff>
--- a/Data/Test Suite Prerequisites.xlsx
+++ b/Data/Test Suite Prerequisites.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\development\feature\1.5.0\gpconnect-provider-testing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F0BFF86-ECB2-41C0-996D-EDBD2601467A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3133472F-6941-466A-9D18-883F557EF245}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-240" yWindow="0" windowWidth="29040" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Patients" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="123">
   <si>
     <t>Required Organizations and Slots for testing</t>
   </si>
@@ -450,6 +450,10 @@
 Patient Linked to a DiagnosticReport linked to a  ProcedureRequest,  specimen, test group BUT NOT linked to any problems
 Note : ProcedureRequest is Optional and Tested Separately - Test can be ignored if not supported
 - Use Supplied EDIFACT Message</t>
+  </si>
+  <si>
+    <t>x
+One Document over 5mb in size</t>
   </si>
 </sst>
 </file>
@@ -1120,7 +1124,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N7" sqref="N7"/>
+      <selection pane="topRight" activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1451,7 +1455,7 @@
       <c r="Z7" s="6"/>
       <c r="AA7" s="6"/>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" ht="75" x14ac:dyDescent="0.25">
       <c r="B8" s="18" t="s">
         <v>33</v>
       </c>
@@ -1492,7 +1496,7 @@
         <v>0</v>
       </c>
       <c r="O8" s="22" t="s">
-        <v>22</v>
+        <v>122</v>
       </c>
       <c r="P8" s="22">
         <v>0</v>

</xml_diff>

<commit_message>
Updated Test Requirements Spreadsheet with a clarification
</commit_message>
<xml_diff>
--- a/Data/Test Suite Prerequisites.xlsx
+++ b/Data/Test Suite Prerequisites.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\development\feature\1.2.8\gpconnect-provider-testing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06A66B45-326F-4092-B455-15E7C84D6680}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CCF80CB-074A-4D0F-9366-6BA002B7A943}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6735" yWindow="2190" windowWidth="21600" windowHeight="11385" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Patients" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="116">
   <si>
     <t>Required Organizations and Slots for testing</t>
   </si>
@@ -397,6 +397,9 @@
   </si>
   <si>
     <t>These healthcare services need to be assigned a valid DOS id for the tests around Healthcare Services and also need one of them associated with a schedule with free slots</t>
+  </si>
+  <si>
+    <t>NOTE : Service Filtering is expected to be switch ON for both supplier and organisation for the automation tests</t>
   </si>
 </sst>
 </file>
@@ -579,7 +582,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -696,6 +699,7 @@
     <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4492,7 +4496,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:U1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -9007,10 +9013,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26844639-70FA-4321-B11C-81EB4222BE38}">
-  <dimension ref="B2:S11"/>
+  <dimension ref="B2:S12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9048,47 +9054,64 @@
       <c r="R3" s="7"/>
       <c r="S3" s="7"/>
     </row>
-    <row r="4" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
+    <row r="4" spans="2:19" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="46" t="s">
+        <v>115</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="7"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="7"/>
+      <c r="S4" s="7"/>
     </row>
     <row r="5" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="31"/>
+      <c r="C5" s="31"/>
+    </row>
+    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B6" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C6" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D6" s="9" t="s">
         <v>113</v>
-      </c>
-    </row>
-    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B6" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="C6" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="D6" s="7" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C7" s="7" t="b">
         <v>1</v>
       </c>
       <c r="D7" s="7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B8" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="C8" s="7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
+      <c r="D8" s="7" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B9" s="7"/>
@@ -9096,12 +9119,17 @@
       <c r="D9" s="7"/>
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B10" s="31"/>
-      <c r="C10" s="31"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B11" s="31"/>
       <c r="C11" s="31"/>
+    </row>
+    <row r="12" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B12" s="31"/>
+      <c r="C12" s="31"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added extra checks for confidential note on lists and cleaned up migrate feature also updated data rqmts
</commit_message>
<xml_diff>
--- a/Data/Test Suite Prerequisites.xlsx
+++ b/Data/Test Suite Prerequisites.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\development\feature\1.6.0\gpconnect-provider-testing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E42825EB-8CF3-4AD4-B84A-581B3DD74827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC8B01BA-ACBB-4022-98A3-48B4EF40C631}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-135" yWindow="-135" windowWidth="29070" windowHeight="15870" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Patients" sheetId="1" r:id="rId1"/>
@@ -464,9 +464,10 @@
 and Have No Documents</t>
   </si>
   <si>
-    <t>x
-Patient should have data for all structured areas
-and Have atleast One document inked to the patient (100 mb or less)</t>
+    <t xml:space="preserve">x
+Patient should have data for all structured areas that also includes Senstive Medication and  Uncategorised data associated to Patient and also a  Sensitive Medication associated to a problem for the patient
+and Have atleast One document inked to the patient (100 mb or less)
+</t>
   </si>
 </sst>
 </file>
@@ -1135,9 +1136,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="H1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="R5" sqref="R5"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1153,7 +1154,8 @@
     <col min="13" max="13" width="55.85546875" style="31" customWidth="1"/>
     <col min="14" max="14" width="19.85546875" style="31" customWidth="1"/>
     <col min="15" max="15" width="13.7109375" style="31" customWidth="1"/>
-    <col min="16" max="17" width="19.42578125" style="31" customWidth="1"/>
+    <col min="16" max="16" width="19.42578125" style="31" customWidth="1"/>
+    <col min="17" max="17" width="29.5703125" style="31" customWidth="1"/>
     <col min="18" max="18" width="36.28515625" customWidth="1"/>
     <col min="19" max="19" width="24.5703125" customWidth="1"/>
     <col min="20" max="28" width="11.5703125" customWidth="1"/>
@@ -1373,7 +1375,7 @@
       <c r="AA5" s="6"/>
       <c r="AB5" s="6"/>
     </row>
-    <row r="6" spans="1:28" ht="150" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" ht="163.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="18" t="s">
         <v>24</v>
       </c>

</xml_diff>

<commit_message>
Removed test "Structured Migrate request for Patient3 excluding Sensitive Data expect No Docs and success" due to inconsistent with TestSuitePrerequisites spreadsheet and  "Structured Migrate request for Patient2 Excluding Sensitive Data expect success" test does the same checks.
</commit_message>
<xml_diff>
--- a/Data/Test Suite Prerequisites.xlsx
+++ b/Data/Test Suite Prerequisites.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GPConnect\Provider\1.6.0\gpconnect-provider-testing\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GPConnect\Provider\1.6\gpconnect-provider-testing\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FB28762-CA4E-4447-8750-AFF7FBD11B1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9266B7B-DA86-4BCD-8ADD-8DDEFECB494F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1136,9 +1136,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P12" sqref="P12"/>
+      <selection pane="bottomLeft" activeCell="S12" sqref="S12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
@@ -1781,8 +1781,8 @@
       <c r="J12" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="K12" s="14" t="s">
-        <v>22</v>
+      <c r="K12" s="14">
+        <v>0</v>
       </c>
       <c r="L12" s="22" t="s">
         <v>22</v>
@@ -1793,8 +1793,8 @@
       <c r="N12" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="O12" s="22">
-        <v>0</v>
+      <c r="O12" s="22" t="s">
+        <v>22</v>
       </c>
       <c r="P12" s="22" t="s">
         <v>22</v>

</xml_diff>